<commit_message>
HoaNT2 : update code qsi014
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者住所変更届.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者住所変更届.xlsx
@@ -4197,15 +4197,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>61</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4220,7 +4220,73 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7562850" y="1514475"/>
+          <a:off x="7572375" y="1485900"/>
+          <a:ext cx="409575" cy="114300"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="A1_52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7581900" y="1628775"/>
           <a:ext cx="409575" cy="114300"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4264,80 +4330,14 @@
     <xdr:from>
       <xdr:col>61</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="A1_52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7572375" y="1657350"/>
-          <a:ext cx="409575" cy="114300"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>64</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:rowOff>219075</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4352,7 +4352,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7562850" y="1800225"/>
+          <a:off x="7572375" y="1771650"/>
           <a:ext cx="409575" cy="114300"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4945,7 +4945,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
+        <a:ln w="6350" cmpd="sng">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -5333,7 +5333,7 @@
   <dimension ref="A1:CE76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4:AH4"/>
+      <selection activeCell="AU31" sqref="AU31:BN31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="17.25" customHeight="1"/>

</xml_diff>

<commit_message>
HoaNT2 : commit code
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者住所変更届.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者住所変更届.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5265"/>
   </bookViews>
   <sheets>
     <sheet name="被保険者住所変更届（一枚目）" sheetId="6" r:id="rId1"/>
@@ -2840,8 +2840,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3269796" y="2630575"/>
-          <a:ext cx="206829" cy="375557"/>
+          <a:off x="3305175" y="2947621"/>
+          <a:ext cx="209550" cy="371475"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2910,7 +2910,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9553575" y="847725"/>
+          <a:off x="9582150" y="1238250"/>
           <a:ext cx="209550" cy="628650"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -3055,8 +3055,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="9525"/>
-          <a:ext cx="2133600" cy="504825"/>
+          <a:off x="0" y="342900"/>
+          <a:ext cx="2133600" cy="499855"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3116,8 +3116,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1266825" cy="695325"/>
+          <a:off x="0" y="333375"/>
+          <a:ext cx="1266825" cy="687456"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3872,68 +3872,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>72</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>77</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="A2_19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8905875" y="5762625"/>
-          <a:ext cx="609600" cy="161925"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>28</xdr:col>
@@ -4980,15 +4918,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>73</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>80</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>209549</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5003,7 +4941,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9039225" y="5743574"/>
+          <a:off x="9010650" y="5772149"/>
           <a:ext cx="800100" cy="142875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5332,8 +5270,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:CE76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AU31" sqref="AU31:BN31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12:CB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="17.25" customHeight="1"/>

</xml_diff>

<commit_message>
HoaNT2: familyid not set data
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者住所変更届.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者住所変更届.xlsx
@@ -676,8 +676,8 @@
     <t>◎記入方法は裏面に書いてありますからよく読んでください。</t>
   </si>
   <si>
-    <t xml:space="preserve">   短期在留　  住民票住所以外の居所注１　
-   海外居住   その他（　　　　　　　　　）  </t>
+    <t xml:space="preserve">      短期在留　   住民票住所以外の居所注１　
+      海外居住       その他（　　　　　　　　）  </t>
   </si>
 </sst>
 </file>
@@ -792,18 +792,17 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="8.5"/>
-      <color theme="1"/>
-      <name val="MS Gothic"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="ＭＳ Ｐ明朝"/>
     </font>
     <font>
       <sz val="11"/>
+      <name val="ＭＳ Ｐ明朝"/>
+    </font>
+    <font>
+      <sz val="8.5"/>
+      <color theme="1"/>
       <name val="ＭＳ Ｐ明朝"/>
     </font>
   </fonts>
@@ -1829,7 +1828,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="306">
+  <cellXfs count="308">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2176,6 +2175,15 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2635,6 +2643,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2707,43 +2730,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3540,274 +3545,6 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>61</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>64</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1033" name="221" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1033"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>61</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>64</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>228600</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1034" name="223" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1034"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>67</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>70</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1035" name="222" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1035"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>67</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>70</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>228600</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1036" name="224" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1036"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
           <xdr:col>10</xdr:col>
           <xdr:colOff>66675</xdr:colOff>
           <xdr:row>17</xdr:row>
@@ -4071,16 +3808,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>48</xdr:col>
+      <xdr:col>50</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>58</xdr:col>
+      <xdr:col>60</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4095,7 +3832,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5981700" y="3152775"/>
+          <a:off x="6229350" y="3133725"/>
           <a:ext cx="1247775" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4591,266 +4328,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>62</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>63</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>31146</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="A4_221">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7705725" y="5581650"/>
-          <a:ext cx="152400" cy="154971"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>✔</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>68</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>69</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>50196</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="A4_222">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8334375" y="5600700"/>
-          <a:ext cx="152400" cy="154971"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>✔</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>62</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>63</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>183546</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="A4_223">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7705725" y="5734050"/>
-          <a:ext cx="152400" cy="154971"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>✔</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>68</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>69</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>202596</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="A4_224">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8343900" y="5753100"/>
-          <a:ext cx="152400" cy="154971"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>✔</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -5094,6 +4571,658 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>61</xdr:col>
+          <xdr:colOff>95250</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>64</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="221" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1039"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>61</xdr:col>
+          <xdr:colOff>95250</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>64</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>228600</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1040" name="223" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1040"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>67</xdr:col>
+          <xdr:colOff>114300</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>47625</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>70</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>57150</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1041" name="222" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1041"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>67</xdr:col>
+          <xdr:colOff>114300</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>70</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>219075</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1042" name="224" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1042"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="A2_19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9001124" y="5753100"/>
+          <a:ext cx="866775" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>21621</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="A4_221">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8220075" y="5553075"/>
+          <a:ext cx="152400" cy="154971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>✔</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12096</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="A4_222">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8362950" y="5562600"/>
+          <a:ext cx="152400" cy="154971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>✔</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>193071</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="A4_223">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8229600" y="5724525"/>
+          <a:ext cx="152400" cy="154971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>✔</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>183546</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="A4_224">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9010650" y="5715000"/>
+          <a:ext cx="152400" cy="154971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>✔</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>238126</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="A2_19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9686925" y="5724525"/>
+          <a:ext cx="809626" cy="200026"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5390,7 +5519,7 @@
   <dimension ref="A1:CE76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AF25" sqref="AF25:BM26"/>
+      <selection activeCell="N12" sqref="N12:CB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="17.25" customHeight="1"/>
@@ -5406,87 +5535,87 @@
   <sheetData>
     <row r="1" spans="1:81" ht="26.25" customHeight="1"/>
     <row r="2" spans="1:81" ht="20.25" customHeight="1">
-      <c r="A2" s="150"/>
-      <c r="B2" s="150"/>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="157"/>
-      <c r="H2" s="157"/>
-      <c r="BI2" s="184" t="s">
+      <c r="A2" s="153"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="BI2" s="187" t="s">
         <v>55</v>
       </c>
-      <c r="BJ2" s="180"/>
-      <c r="BK2" s="180"/>
-      <c r="BL2" s="180"/>
-      <c r="BM2" s="180"/>
-      <c r="BN2" s="181" t="s">
+      <c r="BJ2" s="183"/>
+      <c r="BK2" s="183"/>
+      <c r="BL2" s="183"/>
+      <c r="BM2" s="183"/>
+      <c r="BN2" s="184" t="s">
         <v>21</v>
       </c>
-      <c r="BO2" s="182"/>
-      <c r="BP2" s="182"/>
-      <c r="BQ2" s="182"/>
-      <c r="BR2" s="182"/>
-      <c r="BS2" s="183"/>
-      <c r="BT2" s="180" t="s">
+      <c r="BO2" s="185"/>
+      <c r="BP2" s="185"/>
+      <c r="BQ2" s="185"/>
+      <c r="BR2" s="185"/>
+      <c r="BS2" s="186"/>
+      <c r="BT2" s="183" t="s">
         <v>22</v>
       </c>
-      <c r="BU2" s="180"/>
-      <c r="BV2" s="180"/>
-      <c r="BW2" s="180"/>
-      <c r="BX2" s="180"/>
-      <c r="BY2" s="177" t="s">
+      <c r="BU2" s="183"/>
+      <c r="BV2" s="183"/>
+      <c r="BW2" s="183"/>
+      <c r="BX2" s="183"/>
+      <c r="BY2" s="180" t="s">
         <v>23</v>
       </c>
-      <c r="BZ2" s="178"/>
-      <c r="CA2" s="178"/>
-      <c r="CB2" s="178"/>
-      <c r="CC2" s="179"/>
+      <c r="BZ2" s="181"/>
+      <c r="CA2" s="181"/>
+      <c r="CB2" s="181"/>
+      <c r="CC2" s="182"/>
     </row>
     <row r="3" spans="1:81" ht="18" customHeight="1">
-      <c r="A3" s="150"/>
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="W3" s="191"/>
-      <c r="X3" s="191"/>
-      <c r="Y3" s="191"/>
-      <c r="Z3" s="191"/>
-      <c r="AA3" s="191"/>
-      <c r="AB3" s="191"/>
-      <c r="AC3" s="191"/>
-      <c r="AD3" s="191"/>
-      <c r="AE3" s="191"/>
-      <c r="AF3" s="191"/>
-      <c r="AG3" s="191"/>
-      <c r="AH3" s="191"/>
+      <c r="A3" s="153"/>
+      <c r="B3" s="153"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="W3" s="194"/>
+      <c r="X3" s="194"/>
+      <c r="Y3" s="194"/>
+      <c r="Z3" s="194"/>
+      <c r="AA3" s="194"/>
+      <c r="AB3" s="194"/>
+      <c r="AC3" s="194"/>
+      <c r="AD3" s="194"/>
+      <c r="AE3" s="194"/>
+      <c r="AF3" s="194"/>
+      <c r="AG3" s="194"/>
+      <c r="AH3" s="194"/>
       <c r="AI3" s="6"/>
       <c r="AJ3" s="6"/>
-      <c r="AK3" s="190" t="s">
+      <c r="AK3" s="193" t="s">
         <v>24</v>
       </c>
-      <c r="AL3" s="190"/>
-      <c r="AM3" s="190"/>
-      <c r="AN3" s="190"/>
-      <c r="AO3" s="190"/>
-      <c r="AP3" s="190"/>
-      <c r="AQ3" s="190"/>
-      <c r="AR3" s="190"/>
-      <c r="AS3" s="190"/>
-      <c r="AT3" s="190"/>
-      <c r="AU3" s="190"/>
-      <c r="AV3" s="190"/>
-      <c r="AW3" s="190"/>
-      <c r="AX3" s="190"/>
-      <c r="AY3" s="190"/>
-      <c r="AZ3" s="190"/>
-      <c r="BA3" s="190"/>
-      <c r="BB3" s="190"/>
+      <c r="AL3" s="193"/>
+      <c r="AM3" s="193"/>
+      <c r="AN3" s="193"/>
+      <c r="AO3" s="193"/>
+      <c r="AP3" s="193"/>
+      <c r="AQ3" s="193"/>
+      <c r="AR3" s="193"/>
+      <c r="AS3" s="193"/>
+      <c r="AT3" s="193"/>
+      <c r="AU3" s="193"/>
+      <c r="AV3" s="193"/>
+      <c r="AW3" s="193"/>
+      <c r="AX3" s="193"/>
+      <c r="AY3" s="193"/>
+      <c r="AZ3" s="193"/>
+      <c r="BA3" s="193"/>
+      <c r="BB3" s="193"/>
       <c r="BC3" s="6"/>
       <c r="BD3" s="6"/>
       <c r="BE3" s="6"/>
@@ -5516,90 +5645,90 @@
       <c r="CC3" s="50"/>
     </row>
     <row r="4" spans="1:81" ht="18" customHeight="1">
-      <c r="W4" s="190"/>
-      <c r="X4" s="190"/>
-      <c r="Y4" s="190"/>
-      <c r="Z4" s="190"/>
-      <c r="AA4" s="190"/>
-      <c r="AB4" s="190"/>
-      <c r="AC4" s="190"/>
-      <c r="AD4" s="190"/>
-      <c r="AE4" s="190"/>
-      <c r="AF4" s="190"/>
-      <c r="AG4" s="190"/>
-      <c r="AH4" s="190"/>
+      <c r="W4" s="193"/>
+      <c r="X4" s="193"/>
+      <c r="Y4" s="193"/>
+      <c r="Z4" s="193"/>
+      <c r="AA4" s="193"/>
+      <c r="AB4" s="193"/>
+      <c r="AC4" s="193"/>
+      <c r="AD4" s="193"/>
+      <c r="AE4" s="193"/>
+      <c r="AF4" s="193"/>
+      <c r="AG4" s="193"/>
+      <c r="AH4" s="193"/>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6"/>
-      <c r="AK4" s="190"/>
-      <c r="AL4" s="190"/>
-      <c r="AM4" s="190"/>
-      <c r="AN4" s="190"/>
-      <c r="AO4" s="190"/>
-      <c r="AP4" s="190"/>
-      <c r="AQ4" s="190"/>
-      <c r="AR4" s="190"/>
-      <c r="AS4" s="190"/>
-      <c r="AT4" s="190"/>
-      <c r="AU4" s="190"/>
-      <c r="AV4" s="190"/>
-      <c r="AW4" s="190"/>
-      <c r="AX4" s="190"/>
-      <c r="AY4" s="190"/>
-      <c r="AZ4" s="190"/>
-      <c r="BA4" s="190"/>
-      <c r="BB4" s="190"/>
+      <c r="AK4" s="193"/>
+      <c r="AL4" s="193"/>
+      <c r="AM4" s="193"/>
+      <c r="AN4" s="193"/>
+      <c r="AO4" s="193"/>
+      <c r="AP4" s="193"/>
+      <c r="AQ4" s="193"/>
+      <c r="AR4" s="193"/>
+      <c r="AS4" s="193"/>
+      <c r="AT4" s="193"/>
+      <c r="AU4" s="193"/>
+      <c r="AV4" s="193"/>
+      <c r="AW4" s="193"/>
+      <c r="AX4" s="193"/>
+      <c r="AY4" s="193"/>
+      <c r="AZ4" s="193"/>
+      <c r="BA4" s="193"/>
+      <c r="BB4" s="193"/>
       <c r="BC4" s="6"/>
       <c r="BD4" s="6"/>
       <c r="BE4" s="6"/>
       <c r="BF4" s="6"/>
       <c r="BG4" s="6"/>
       <c r="BH4" s="7"/>
-      <c r="BI4" s="185"/>
-      <c r="BJ4" s="186"/>
-      <c r="BK4" s="186"/>
-      <c r="BL4" s="186"/>
-      <c r="BM4" s="187"/>
-      <c r="BN4" s="185"/>
-      <c r="BO4" s="186"/>
-      <c r="BP4" s="186"/>
-      <c r="BQ4" s="186"/>
-      <c r="BR4" s="186"/>
-      <c r="BS4" s="187"/>
-      <c r="BT4" s="185"/>
-      <c r="BU4" s="186"/>
-      <c r="BV4" s="186"/>
-      <c r="BW4" s="186"/>
-      <c r="BX4" s="187"/>
-      <c r="BY4" s="185"/>
-      <c r="BZ4" s="186"/>
-      <c r="CA4" s="186"/>
-      <c r="CB4" s="186"/>
-      <c r="CC4" s="187"/>
+      <c r="BI4" s="188"/>
+      <c r="BJ4" s="189"/>
+      <c r="BK4" s="189"/>
+      <c r="BL4" s="189"/>
+      <c r="BM4" s="190"/>
+      <c r="BN4" s="188"/>
+      <c r="BO4" s="189"/>
+      <c r="BP4" s="189"/>
+      <c r="BQ4" s="189"/>
+      <c r="BR4" s="189"/>
+      <c r="BS4" s="190"/>
+      <c r="BT4" s="188"/>
+      <c r="BU4" s="189"/>
+      <c r="BV4" s="189"/>
+      <c r="BW4" s="189"/>
+      <c r="BX4" s="190"/>
+      <c r="BY4" s="188"/>
+      <c r="BZ4" s="189"/>
+      <c r="CA4" s="189"/>
+      <c r="CB4" s="189"/>
+      <c r="CC4" s="190"/>
     </row>
     <row r="5" spans="1:81" ht="9" customHeight="1"/>
     <row r="6" spans="1:81" ht="24" customHeight="1">
-      <c r="A6" s="292" t="s">
+      <c r="A6" s="300" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="292"/>
-      <c r="C6" s="165" t="s">
+      <c r="B6" s="300"/>
+      <c r="C6" s="168" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="165"/>
-      <c r="E6" s="160" t="s">
+      <c r="D6" s="168"/>
+      <c r="E6" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="160"/>
-      <c r="G6" s="160"/>
-      <c r="H6" s="160"/>
-      <c r="I6" s="160"/>
-      <c r="J6" s="160"/>
-      <c r="K6" s="160"/>
-      <c r="L6" s="160"/>
-      <c r="M6" s="160"/>
-      <c r="N6" s="160"/>
-      <c r="O6" s="160"/>
-      <c r="P6" s="160"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="163"/>
+      <c r="K6" s="163"/>
+      <c r="L6" s="163"/>
+      <c r="M6" s="163"/>
+      <c r="N6" s="163"/>
+      <c r="O6" s="163"/>
+      <c r="P6" s="163"/>
       <c r="Q6" s="95" t="s">
         <v>53</v>
       </c>
@@ -5670,28 +5799,28 @@
       <c r="BX6" s="49"/>
       <c r="BY6" s="49"/>
       <c r="BZ6" s="50"/>
-      <c r="CA6" s="195"/>
-      <c r="CB6" s="196"/>
+      <c r="CA6" s="198"/>
+      <c r="CB6" s="199"/>
       <c r="CC6" s="10"/>
     </row>
     <row r="7" spans="1:81" ht="15.75" customHeight="1">
-      <c r="A7" s="292"/>
-      <c r="B7" s="292"/>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="159"/>
-      <c r="I7" s="162"/>
-      <c r="J7" s="147"/>
-      <c r="K7" s="147"/>
-      <c r="L7" s="147"/>
-      <c r="M7" s="147"/>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="161"/>
-      <c r="Q7" s="176"/>
+      <c r="A7" s="300"/>
+      <c r="B7" s="300"/>
+      <c r="C7" s="168"/>
+      <c r="D7" s="168"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="161"/>
+      <c r="H7" s="162"/>
+      <c r="I7" s="165"/>
+      <c r="J7" s="150"/>
+      <c r="K7" s="150"/>
+      <c r="L7" s="150"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="150"/>
+      <c r="O7" s="150"/>
+      <c r="P7" s="164"/>
+      <c r="Q7" s="179"/>
       <c r="R7" s="60"/>
       <c r="S7" s="60"/>
       <c r="T7" s="60"/>
@@ -5704,9 +5833,9 @@
       <c r="AA7" s="54"/>
       <c r="AB7" s="54"/>
       <c r="AC7" s="73"/>
-      <c r="AD7" s="188"/>
+      <c r="AD7" s="191"/>
       <c r="AE7" s="111"/>
-      <c r="AF7" s="197"/>
+      <c r="AF7" s="200"/>
       <c r="AG7" s="111"/>
       <c r="AH7" s="54"/>
       <c r="AI7" s="54"/>
@@ -5718,66 +5847,66 @@
       <c r="AO7" s="54"/>
       <c r="AP7" s="54"/>
       <c r="AQ7" s="54"/>
-      <c r="AR7" s="142"/>
-      <c r="AS7" s="143"/>
-      <c r="AT7" s="145" t="s">
+      <c r="AR7" s="145"/>
+      <c r="AS7" s="146"/>
+      <c r="AT7" s="148" t="s">
         <v>37</v>
       </c>
-      <c r="AU7" s="146"/>
-      <c r="AV7" s="228"/>
-      <c r="AW7" s="228"/>
-      <c r="AX7" s="228"/>
-      <c r="AY7" s="228"/>
-      <c r="AZ7" s="228"/>
-      <c r="BA7" s="229"/>
-      <c r="BB7" s="192"/>
-      <c r="BC7" s="193"/>
-      <c r="BD7" s="193"/>
-      <c r="BE7" s="193"/>
-      <c r="BF7" s="193"/>
-      <c r="BG7" s="193"/>
-      <c r="BH7" s="193"/>
-      <c r="BI7" s="194"/>
-      <c r="BJ7" s="126" t="s">
+      <c r="AU7" s="149"/>
+      <c r="AV7" s="231"/>
+      <c r="AW7" s="231"/>
+      <c r="AX7" s="231"/>
+      <c r="AY7" s="231"/>
+      <c r="AZ7" s="231"/>
+      <c r="BA7" s="232"/>
+      <c r="BB7" s="195"/>
+      <c r="BC7" s="196"/>
+      <c r="BD7" s="196"/>
+      <c r="BE7" s="196"/>
+      <c r="BF7" s="196"/>
+      <c r="BG7" s="196"/>
+      <c r="BH7" s="196"/>
+      <c r="BI7" s="197"/>
+      <c r="BJ7" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="BK7" s="127"/>
-      <c r="BL7" s="127"/>
-      <c r="BM7" s="128"/>
+      <c r="BK7" s="130"/>
+      <c r="BL7" s="130"/>
+      <c r="BM7" s="131"/>
       <c r="BN7" s="109"/>
       <c r="BO7" s="56"/>
-      <c r="BP7" s="155"/>
-      <c r="BQ7" s="151"/>
-      <c r="BR7" s="152"/>
+      <c r="BP7" s="158"/>
+      <c r="BQ7" s="154"/>
+      <c r="BR7" s="155"/>
       <c r="BS7" s="56"/>
-      <c r="BT7" s="155"/>
-      <c r="BU7" s="155"/>
+      <c r="BT7" s="158"/>
+      <c r="BU7" s="158"/>
       <c r="BV7" s="112"/>
       <c r="BW7" s="56"/>
-      <c r="BX7" s="155"/>
-      <c r="BY7" s="155"/>
-      <c r="BZ7" s="156"/>
-      <c r="CA7" s="195"/>
-      <c r="CB7" s="196"/>
+      <c r="BX7" s="158"/>
+      <c r="BY7" s="158"/>
+      <c r="BZ7" s="159"/>
+      <c r="CA7" s="198"/>
+      <c r="CB7" s="199"/>
       <c r="CC7" s="10"/>
     </row>
     <row r="8" spans="1:81" ht="21.75" customHeight="1">
-      <c r="A8" s="292"/>
-      <c r="B8" s="292"/>
-      <c r="C8" s="165"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="167"/>
-      <c r="H8" s="168"/>
-      <c r="I8" s="162"/>
-      <c r="J8" s="147"/>
-      <c r="K8" s="147"/>
-      <c r="L8" s="147"/>
-      <c r="M8" s="147"/>
-      <c r="N8" s="147"/>
-      <c r="O8" s="147"/>
-      <c r="P8" s="161"/>
+      <c r="A8" s="300"/>
+      <c r="B8" s="300"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="167"/>
+      <c r="G8" s="170"/>
+      <c r="H8" s="171"/>
+      <c r="I8" s="165"/>
+      <c r="J8" s="150"/>
+      <c r="K8" s="150"/>
+      <c r="L8" s="150"/>
+      <c r="M8" s="150"/>
+      <c r="N8" s="150"/>
+      <c r="O8" s="150"/>
+      <c r="P8" s="164"/>
       <c r="Q8" s="63"/>
       <c r="R8" s="64"/>
       <c r="S8" s="64"/>
@@ -5785,57 +5914,57 @@
       <c r="U8" s="64"/>
       <c r="V8" s="63"/>
       <c r="W8" s="98"/>
-      <c r="X8" s="169"/>
+      <c r="X8" s="172"/>
       <c r="Y8" s="74"/>
       <c r="Z8" s="74"/>
       <c r="AA8" s="74"/>
       <c r="AB8" s="74"/>
       <c r="AC8" s="75"/>
-      <c r="AD8" s="189"/>
+      <c r="AD8" s="192"/>
       <c r="AE8" s="72"/>
-      <c r="AF8" s="198"/>
+      <c r="AF8" s="201"/>
       <c r="AG8" s="72"/>
       <c r="AH8" s="74"/>
       <c r="AI8" s="74"/>
       <c r="AJ8" s="74"/>
       <c r="AK8" s="75"/>
-      <c r="AL8" s="169"/>
+      <c r="AL8" s="172"/>
       <c r="AM8" s="74"/>
       <c r="AN8" s="74"/>
       <c r="AO8" s="74"/>
       <c r="AP8" s="74"/>
       <c r="AQ8" s="74"/>
-      <c r="AR8" s="144"/>
+      <c r="AR8" s="147"/>
       <c r="AS8" s="115"/>
-      <c r="AT8" s="136" t="s">
+      <c r="AT8" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="AU8" s="137"/>
-      <c r="AV8" s="230"/>
-      <c r="AW8" s="230"/>
-      <c r="AX8" s="230"/>
-      <c r="AY8" s="230"/>
-      <c r="AZ8" s="230"/>
-      <c r="BA8" s="231"/>
-      <c r="BB8" s="232" t="s">
+      <c r="AU8" s="140"/>
+      <c r="AV8" s="233"/>
+      <c r="AW8" s="233"/>
+      <c r="AX8" s="233"/>
+      <c r="AY8" s="233"/>
+      <c r="AZ8" s="233"/>
+      <c r="BA8" s="234"/>
+      <c r="BB8" s="235" t="s">
         <v>20</v>
       </c>
-      <c r="BC8" s="233"/>
-      <c r="BD8" s="138"/>
-      <c r="BE8" s="138"/>
-      <c r="BF8" s="138"/>
-      <c r="BG8" s="138"/>
-      <c r="BH8" s="138"/>
-      <c r="BI8" s="139"/>
-      <c r="BJ8" s="129"/>
-      <c r="BK8" s="130"/>
-      <c r="BL8" s="130"/>
-      <c r="BM8" s="131"/>
+      <c r="BC8" s="236"/>
+      <c r="BD8" s="141"/>
+      <c r="BE8" s="141"/>
+      <c r="BF8" s="141"/>
+      <c r="BG8" s="141"/>
+      <c r="BH8" s="141"/>
+      <c r="BI8" s="142"/>
+      <c r="BJ8" s="132"/>
+      <c r="BK8" s="133"/>
+      <c r="BL8" s="133"/>
+      <c r="BM8" s="134"/>
       <c r="BN8" s="111"/>
       <c r="BO8" s="53"/>
       <c r="BP8" s="54"/>
-      <c r="BQ8" s="153"/>
-      <c r="BR8" s="154"/>
+      <c r="BQ8" s="156"/>
+      <c r="BR8" s="157"/>
       <c r="BS8" s="53"/>
       <c r="BT8" s="54"/>
       <c r="BU8" s="54"/>
@@ -5844,24 +5973,24 @@
       <c r="BX8" s="54"/>
       <c r="BY8" s="54"/>
       <c r="BZ8" s="73"/>
-      <c r="CA8" s="195"/>
-      <c r="CB8" s="196"/>
+      <c r="CA8" s="198"/>
+      <c r="CB8" s="199"/>
       <c r="CC8" s="10"/>
     </row>
     <row r="9" spans="1:81" ht="15.75" customHeight="1">
-      <c r="A9" s="292"/>
-      <c r="B9" s="292"/>
-      <c r="C9" s="165"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="199" t="s">
+      <c r="A9" s="300"/>
+      <c r="B9" s="300"/>
+      <c r="C9" s="168"/>
+      <c r="D9" s="168"/>
+      <c r="E9" s="202" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="200"/>
-      <c r="G9" s="201"/>
-      <c r="H9" s="148" t="s">
+      <c r="F9" s="203"/>
+      <c r="G9" s="204"/>
+      <c r="H9" s="151" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="149"/>
+      <c r="I9" s="152"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
@@ -5885,75 +6014,75 @@
       </c>
       <c r="AC9" s="66"/>
       <c r="AD9" s="67"/>
-      <c r="AE9" s="140" t="s">
+      <c r="AE9" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="AF9" s="141"/>
-      <c r="AG9" s="141"/>
-      <c r="AH9" s="141"/>
-      <c r="AI9" s="132"/>
-      <c r="AJ9" s="132"/>
-      <c r="AK9" s="132"/>
-      <c r="AL9" s="132"/>
-      <c r="AM9" s="132"/>
-      <c r="AN9" s="132"/>
-      <c r="AO9" s="132"/>
-      <c r="AP9" s="132"/>
-      <c r="AQ9" s="132"/>
-      <c r="AR9" s="132"/>
-      <c r="AS9" s="132"/>
-      <c r="AT9" s="132"/>
-      <c r="AU9" s="132"/>
-      <c r="AV9" s="132"/>
-      <c r="AW9" s="132"/>
-      <c r="AX9" s="132"/>
-      <c r="AY9" s="132"/>
-      <c r="AZ9" s="132"/>
-      <c r="BA9" s="132"/>
-      <c r="BB9" s="132"/>
-      <c r="BC9" s="132"/>
-      <c r="BD9" s="132"/>
-      <c r="BE9" s="132"/>
-      <c r="BF9" s="132"/>
-      <c r="BG9" s="132"/>
-      <c r="BH9" s="132"/>
-      <c r="BI9" s="132"/>
-      <c r="BJ9" s="132"/>
-      <c r="BK9" s="132"/>
-      <c r="BL9" s="132"/>
-      <c r="BM9" s="132"/>
-      <c r="BN9" s="132"/>
-      <c r="BO9" s="132"/>
-      <c r="BP9" s="132"/>
-      <c r="BQ9" s="132"/>
-      <c r="BR9" s="132"/>
-      <c r="BS9" s="132"/>
-      <c r="BT9" s="132"/>
-      <c r="BU9" s="132"/>
-      <c r="BV9" s="132"/>
-      <c r="BW9" s="132"/>
-      <c r="BX9" s="132"/>
-      <c r="BY9" s="132"/>
-      <c r="BZ9" s="132"/>
-      <c r="CA9" s="132"/>
-      <c r="CB9" s="133"/>
+      <c r="AF9" s="144"/>
+      <c r="AG9" s="144"/>
+      <c r="AH9" s="144"/>
+      <c r="AI9" s="135"/>
+      <c r="AJ9" s="135"/>
+      <c r="AK9" s="135"/>
+      <c r="AL9" s="135"/>
+      <c r="AM9" s="135"/>
+      <c r="AN9" s="135"/>
+      <c r="AO9" s="135"/>
+      <c r="AP9" s="135"/>
+      <c r="AQ9" s="135"/>
+      <c r="AR9" s="135"/>
+      <c r="AS9" s="135"/>
+      <c r="AT9" s="135"/>
+      <c r="AU9" s="135"/>
+      <c r="AV9" s="135"/>
+      <c r="AW9" s="135"/>
+      <c r="AX9" s="135"/>
+      <c r="AY9" s="135"/>
+      <c r="AZ9" s="135"/>
+      <c r="BA9" s="135"/>
+      <c r="BB9" s="135"/>
+      <c r="BC9" s="135"/>
+      <c r="BD9" s="135"/>
+      <c r="BE9" s="135"/>
+      <c r="BF9" s="135"/>
+      <c r="BG9" s="135"/>
+      <c r="BH9" s="135"/>
+      <c r="BI9" s="135"/>
+      <c r="BJ9" s="135"/>
+      <c r="BK9" s="135"/>
+      <c r="BL9" s="135"/>
+      <c r="BM9" s="135"/>
+      <c r="BN9" s="135"/>
+      <c r="BO9" s="135"/>
+      <c r="BP9" s="135"/>
+      <c r="BQ9" s="135"/>
+      <c r="BR9" s="135"/>
+      <c r="BS9" s="135"/>
+      <c r="BT9" s="135"/>
+      <c r="BU9" s="135"/>
+      <c r="BV9" s="135"/>
+      <c r="BW9" s="135"/>
+      <c r="BX9" s="135"/>
+      <c r="BY9" s="135"/>
+      <c r="BZ9" s="135"/>
+      <c r="CA9" s="135"/>
+      <c r="CB9" s="136"/>
     </row>
     <row r="10" spans="1:81" ht="15.75" customHeight="1">
-      <c r="A10" s="292"/>
-      <c r="B10" s="292"/>
-      <c r="C10" s="165"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="202"/>
-      <c r="F10" s="203"/>
-      <c r="G10" s="204"/>
-      <c r="H10" s="218" t="s">
+      <c r="A10" s="300"/>
+      <c r="B10" s="300"/>
+      <c r="C10" s="168"/>
+      <c r="D10" s="168"/>
+      <c r="E10" s="205"/>
+      <c r="F10" s="206"/>
+      <c r="G10" s="207"/>
+      <c r="H10" s="221" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="219"/>
-      <c r="J10" s="219"/>
-      <c r="K10" s="219"/>
-      <c r="L10" s="219"/>
-      <c r="M10" s="219"/>
+      <c r="I10" s="222"/>
+      <c r="J10" s="222"/>
+      <c r="K10" s="222"/>
+      <c r="L10" s="222"/>
+      <c r="M10" s="222"/>
       <c r="N10" s="72"/>
       <c r="O10" s="74"/>
       <c r="P10" s="74"/>
@@ -5971,71 +6100,71 @@
       <c r="AB10" s="65"/>
       <c r="AC10" s="66"/>
       <c r="AD10" s="67"/>
-      <c r="AE10" s="208"/>
-      <c r="AF10" s="209"/>
-      <c r="AG10" s="209"/>
-      <c r="AH10" s="209"/>
-      <c r="AI10" s="209"/>
-      <c r="AJ10" s="209"/>
-      <c r="AK10" s="209"/>
-      <c r="AL10" s="209"/>
-      <c r="AM10" s="209"/>
-      <c r="AN10" s="209"/>
-      <c r="AO10" s="209"/>
-      <c r="AP10" s="209"/>
-      <c r="AQ10" s="209"/>
-      <c r="AR10" s="209"/>
-      <c r="AS10" s="209"/>
-      <c r="AT10" s="209"/>
-      <c r="AU10" s="209"/>
-      <c r="AV10" s="209"/>
-      <c r="AW10" s="209"/>
-      <c r="AX10" s="209"/>
-      <c r="AY10" s="209"/>
-      <c r="AZ10" s="209"/>
-      <c r="BA10" s="209"/>
-      <c r="BB10" s="209"/>
-      <c r="BC10" s="209"/>
-      <c r="BD10" s="209"/>
-      <c r="BE10" s="209"/>
-      <c r="BF10" s="209"/>
-      <c r="BG10" s="209"/>
-      <c r="BH10" s="209"/>
-      <c r="BI10" s="209"/>
-      <c r="BJ10" s="209"/>
-      <c r="BK10" s="209"/>
-      <c r="BL10" s="209"/>
-      <c r="BM10" s="209"/>
-      <c r="BN10" s="209"/>
-      <c r="BO10" s="209"/>
-      <c r="BP10" s="209"/>
-      <c r="BQ10" s="209"/>
-      <c r="BR10" s="209"/>
-      <c r="BS10" s="209"/>
-      <c r="BT10" s="209"/>
-      <c r="BU10" s="209"/>
-      <c r="BV10" s="209"/>
-      <c r="BW10" s="209"/>
-      <c r="BX10" s="209"/>
-      <c r="BY10" s="209"/>
-      <c r="BZ10" s="209"/>
-      <c r="CA10" s="209"/>
-      <c r="CB10" s="210"/>
+      <c r="AE10" s="211"/>
+      <c r="AF10" s="212"/>
+      <c r="AG10" s="212"/>
+      <c r="AH10" s="212"/>
+      <c r="AI10" s="212"/>
+      <c r="AJ10" s="212"/>
+      <c r="AK10" s="212"/>
+      <c r="AL10" s="212"/>
+      <c r="AM10" s="212"/>
+      <c r="AN10" s="212"/>
+      <c r="AO10" s="212"/>
+      <c r="AP10" s="212"/>
+      <c r="AQ10" s="212"/>
+      <c r="AR10" s="212"/>
+      <c r="AS10" s="212"/>
+      <c r="AT10" s="212"/>
+      <c r="AU10" s="212"/>
+      <c r="AV10" s="212"/>
+      <c r="AW10" s="212"/>
+      <c r="AX10" s="212"/>
+      <c r="AY10" s="212"/>
+      <c r="AZ10" s="212"/>
+      <c r="BA10" s="212"/>
+      <c r="BB10" s="212"/>
+      <c r="BC10" s="212"/>
+      <c r="BD10" s="212"/>
+      <c r="BE10" s="212"/>
+      <c r="BF10" s="212"/>
+      <c r="BG10" s="212"/>
+      <c r="BH10" s="212"/>
+      <c r="BI10" s="212"/>
+      <c r="BJ10" s="212"/>
+      <c r="BK10" s="212"/>
+      <c r="BL10" s="212"/>
+      <c r="BM10" s="212"/>
+      <c r="BN10" s="212"/>
+      <c r="BO10" s="212"/>
+      <c r="BP10" s="212"/>
+      <c r="BQ10" s="212"/>
+      <c r="BR10" s="212"/>
+      <c r="BS10" s="212"/>
+      <c r="BT10" s="212"/>
+      <c r="BU10" s="212"/>
+      <c r="BV10" s="212"/>
+      <c r="BW10" s="212"/>
+      <c r="BX10" s="212"/>
+      <c r="BY10" s="212"/>
+      <c r="BZ10" s="212"/>
+      <c r="CA10" s="212"/>
+      <c r="CB10" s="213"/>
     </row>
     <row r="11" spans="1:81" ht="15.75" customHeight="1">
-      <c r="A11" s="292"/>
-      <c r="B11" s="292"/>
-      <c r="C11" s="165"/>
-      <c r="D11" s="165"/>
-      <c r="E11" s="205"/>
-      <c r="F11" s="206"/>
-      <c r="G11" s="207"/>
-      <c r="H11" s="220"/>
-      <c r="I11" s="221"/>
-      <c r="J11" s="221"/>
-      <c r="K11" s="221"/>
-      <c r="L11" s="221"/>
-      <c r="M11" s="221"/>
+      <c r="A11" s="300"/>
+      <c r="B11" s="300"/>
+      <c r="C11" s="168"/>
+      <c r="D11" s="168"/>
+      <c r="E11" s="208"/>
+      <c r="F11" s="209"/>
+      <c r="G11" s="210"/>
+      <c r="H11" s="223"/>
+      <c r="I11" s="224"/>
+      <c r="J11" s="224"/>
+      <c r="K11" s="224"/>
+      <c r="L11" s="224"/>
+      <c r="M11" s="224"/>
       <c r="N11" s="72"/>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
@@ -6053,232 +6182,232 @@
       <c r="AB11" s="68"/>
       <c r="AC11" s="69"/>
       <c r="AD11" s="70"/>
-      <c r="AE11" s="211"/>
-      <c r="AF11" s="212"/>
-      <c r="AG11" s="212"/>
-      <c r="AH11" s="212"/>
-      <c r="AI11" s="212"/>
-      <c r="AJ11" s="212"/>
-      <c r="AK11" s="212"/>
-      <c r="AL11" s="212"/>
-      <c r="AM11" s="212"/>
-      <c r="AN11" s="212"/>
-      <c r="AO11" s="212"/>
-      <c r="AP11" s="212"/>
-      <c r="AQ11" s="212"/>
-      <c r="AR11" s="212"/>
-      <c r="AS11" s="212"/>
-      <c r="AT11" s="212"/>
-      <c r="AU11" s="212"/>
-      <c r="AV11" s="212"/>
-      <c r="AW11" s="212"/>
-      <c r="AX11" s="212"/>
-      <c r="AY11" s="212"/>
-      <c r="AZ11" s="212"/>
-      <c r="BA11" s="212"/>
-      <c r="BB11" s="212"/>
-      <c r="BC11" s="212"/>
-      <c r="BD11" s="212"/>
-      <c r="BE11" s="212"/>
-      <c r="BF11" s="212"/>
-      <c r="BG11" s="212"/>
-      <c r="BH11" s="212"/>
-      <c r="BI11" s="212"/>
-      <c r="BJ11" s="212"/>
-      <c r="BK11" s="212"/>
-      <c r="BL11" s="212"/>
-      <c r="BM11" s="212"/>
-      <c r="BN11" s="212"/>
-      <c r="BO11" s="212"/>
-      <c r="BP11" s="212"/>
-      <c r="BQ11" s="212"/>
-      <c r="BR11" s="212"/>
-      <c r="BS11" s="212"/>
-      <c r="BT11" s="212"/>
-      <c r="BU11" s="212"/>
-      <c r="BV11" s="212"/>
-      <c r="BW11" s="212"/>
-      <c r="BX11" s="212"/>
-      <c r="BY11" s="212"/>
-      <c r="BZ11" s="212"/>
-      <c r="CA11" s="212"/>
-      <c r="CB11" s="213"/>
+      <c r="AE11" s="214"/>
+      <c r="AF11" s="215"/>
+      <c r="AG11" s="215"/>
+      <c r="AH11" s="215"/>
+      <c r="AI11" s="215"/>
+      <c r="AJ11" s="215"/>
+      <c r="AK11" s="215"/>
+      <c r="AL11" s="215"/>
+      <c r="AM11" s="215"/>
+      <c r="AN11" s="215"/>
+      <c r="AO11" s="215"/>
+      <c r="AP11" s="215"/>
+      <c r="AQ11" s="215"/>
+      <c r="AR11" s="215"/>
+      <c r="AS11" s="215"/>
+      <c r="AT11" s="215"/>
+      <c r="AU11" s="215"/>
+      <c r="AV11" s="215"/>
+      <c r="AW11" s="215"/>
+      <c r="AX11" s="215"/>
+      <c r="AY11" s="215"/>
+      <c r="AZ11" s="215"/>
+      <c r="BA11" s="215"/>
+      <c r="BB11" s="215"/>
+      <c r="BC11" s="215"/>
+      <c r="BD11" s="215"/>
+      <c r="BE11" s="215"/>
+      <c r="BF11" s="215"/>
+      <c r="BG11" s="215"/>
+      <c r="BH11" s="215"/>
+      <c r="BI11" s="215"/>
+      <c r="BJ11" s="215"/>
+      <c r="BK11" s="215"/>
+      <c r="BL11" s="215"/>
+      <c r="BM11" s="215"/>
+      <c r="BN11" s="215"/>
+      <c r="BO11" s="215"/>
+      <c r="BP11" s="215"/>
+      <c r="BQ11" s="215"/>
+      <c r="BR11" s="215"/>
+      <c r="BS11" s="215"/>
+      <c r="BT11" s="215"/>
+      <c r="BU11" s="215"/>
+      <c r="BV11" s="215"/>
+      <c r="BW11" s="215"/>
+      <c r="BX11" s="215"/>
+      <c r="BY11" s="215"/>
+      <c r="BZ11" s="215"/>
+      <c r="CA11" s="215"/>
+      <c r="CB11" s="216"/>
     </row>
     <row r="12" spans="1:81" ht="15.75" customHeight="1">
-      <c r="A12" s="292"/>
-      <c r="B12" s="292"/>
-      <c r="C12" s="165"/>
-      <c r="D12" s="165"/>
+      <c r="A12" s="300"/>
+      <c r="B12" s="300"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="168"/>
       <c r="E12" s="89" t="s">
         <v>3</v>
       </c>
       <c r="F12" s="90"/>
       <c r="G12" s="91"/>
-      <c r="H12" s="247" t="s">
+      <c r="H12" s="250" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="248"/>
-      <c r="J12" s="222" t="s">
+      <c r="I12" s="251"/>
+      <c r="J12" s="225" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="222"/>
-      <c r="L12" s="222"/>
-      <c r="M12" s="223"/>
-      <c r="N12" s="214"/>
-      <c r="O12" s="215"/>
-      <c r="P12" s="215"/>
-      <c r="Q12" s="215"/>
-      <c r="R12" s="215"/>
-      <c r="S12" s="215"/>
-      <c r="T12" s="215"/>
-      <c r="U12" s="215"/>
-      <c r="V12" s="215"/>
-      <c r="W12" s="215"/>
-      <c r="X12" s="215"/>
-      <c r="Y12" s="215"/>
-      <c r="Z12" s="215"/>
-      <c r="AA12" s="215"/>
-      <c r="AB12" s="215"/>
-      <c r="AC12" s="215"/>
-      <c r="AD12" s="215"/>
-      <c r="AE12" s="215"/>
-      <c r="AF12" s="215"/>
-      <c r="AG12" s="215"/>
-      <c r="AH12" s="215"/>
-      <c r="AI12" s="215"/>
-      <c r="AJ12" s="215"/>
-      <c r="AK12" s="215"/>
-      <c r="AL12" s="215"/>
-      <c r="AM12" s="215"/>
-      <c r="AN12" s="215"/>
-      <c r="AO12" s="215"/>
-      <c r="AP12" s="215"/>
-      <c r="AQ12" s="215"/>
-      <c r="AR12" s="215"/>
-      <c r="AS12" s="215"/>
-      <c r="AT12" s="215"/>
-      <c r="AU12" s="215"/>
-      <c r="AV12" s="215"/>
-      <c r="AW12" s="215"/>
-      <c r="AX12" s="215"/>
-      <c r="AY12" s="215"/>
-      <c r="AZ12" s="215"/>
-      <c r="BA12" s="215"/>
-      <c r="BB12" s="215"/>
-      <c r="BC12" s="215"/>
-      <c r="BD12" s="215"/>
-      <c r="BE12" s="215"/>
-      <c r="BF12" s="215"/>
-      <c r="BG12" s="215"/>
-      <c r="BH12" s="215"/>
-      <c r="BI12" s="215"/>
-      <c r="BJ12" s="215"/>
-      <c r="BK12" s="215"/>
-      <c r="BL12" s="215"/>
-      <c r="BM12" s="215"/>
-      <c r="BN12" s="215"/>
-      <c r="BO12" s="215"/>
-      <c r="BP12" s="215"/>
-      <c r="BQ12" s="215"/>
-      <c r="BR12" s="215"/>
-      <c r="BS12" s="215"/>
-      <c r="BT12" s="215"/>
-      <c r="BU12" s="215"/>
-      <c r="BV12" s="215"/>
-      <c r="BW12" s="215"/>
-      <c r="BX12" s="215"/>
-      <c r="BY12" s="215"/>
-      <c r="BZ12" s="215"/>
-      <c r="CA12" s="215"/>
-      <c r="CB12" s="216"/>
+      <c r="K12" s="225"/>
+      <c r="L12" s="225"/>
+      <c r="M12" s="226"/>
+      <c r="N12" s="217"/>
+      <c r="O12" s="218"/>
+      <c r="P12" s="218"/>
+      <c r="Q12" s="218"/>
+      <c r="R12" s="218"/>
+      <c r="S12" s="218"/>
+      <c r="T12" s="218"/>
+      <c r="U12" s="218"/>
+      <c r="V12" s="218"/>
+      <c r="W12" s="218"/>
+      <c r="X12" s="218"/>
+      <c r="Y12" s="218"/>
+      <c r="Z12" s="218"/>
+      <c r="AA12" s="218"/>
+      <c r="AB12" s="218"/>
+      <c r="AC12" s="218"/>
+      <c r="AD12" s="218"/>
+      <c r="AE12" s="218"/>
+      <c r="AF12" s="218"/>
+      <c r="AG12" s="218"/>
+      <c r="AH12" s="218"/>
+      <c r="AI12" s="218"/>
+      <c r="AJ12" s="218"/>
+      <c r="AK12" s="218"/>
+      <c r="AL12" s="218"/>
+      <c r="AM12" s="218"/>
+      <c r="AN12" s="218"/>
+      <c r="AO12" s="218"/>
+      <c r="AP12" s="218"/>
+      <c r="AQ12" s="218"/>
+      <c r="AR12" s="218"/>
+      <c r="AS12" s="218"/>
+      <c r="AT12" s="218"/>
+      <c r="AU12" s="218"/>
+      <c r="AV12" s="218"/>
+      <c r="AW12" s="218"/>
+      <c r="AX12" s="218"/>
+      <c r="AY12" s="218"/>
+      <c r="AZ12" s="218"/>
+      <c r="BA12" s="218"/>
+      <c r="BB12" s="218"/>
+      <c r="BC12" s="218"/>
+      <c r="BD12" s="218"/>
+      <c r="BE12" s="218"/>
+      <c r="BF12" s="218"/>
+      <c r="BG12" s="218"/>
+      <c r="BH12" s="218"/>
+      <c r="BI12" s="218"/>
+      <c r="BJ12" s="218"/>
+      <c r="BK12" s="218"/>
+      <c r="BL12" s="218"/>
+      <c r="BM12" s="218"/>
+      <c r="BN12" s="218"/>
+      <c r="BO12" s="218"/>
+      <c r="BP12" s="218"/>
+      <c r="BQ12" s="218"/>
+      <c r="BR12" s="218"/>
+      <c r="BS12" s="218"/>
+      <c r="BT12" s="218"/>
+      <c r="BU12" s="218"/>
+      <c r="BV12" s="218"/>
+      <c r="BW12" s="218"/>
+      <c r="BX12" s="218"/>
+      <c r="BY12" s="218"/>
+      <c r="BZ12" s="218"/>
+      <c r="CA12" s="218"/>
+      <c r="CB12" s="219"/>
     </row>
     <row r="13" spans="1:81" ht="15.75" customHeight="1">
-      <c r="A13" s="292"/>
-      <c r="B13" s="292"/>
-      <c r="C13" s="165"/>
-      <c r="D13" s="165"/>
+      <c r="A13" s="300"/>
+      <c r="B13" s="300"/>
+      <c r="C13" s="168"/>
+      <c r="D13" s="168"/>
       <c r="E13" s="92"/>
       <c r="F13" s="93"/>
       <c r="G13" s="94"/>
       <c r="H13" s="15"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="221"/>
-      <c r="K13" s="221"/>
-      <c r="L13" s="221"/>
-      <c r="M13" s="224"/>
-      <c r="N13" s="211"/>
-      <c r="O13" s="212"/>
-      <c r="P13" s="212"/>
-      <c r="Q13" s="212"/>
-      <c r="R13" s="212"/>
-      <c r="S13" s="212"/>
-      <c r="T13" s="212"/>
-      <c r="U13" s="212"/>
-      <c r="V13" s="212"/>
-      <c r="W13" s="212"/>
-      <c r="X13" s="212"/>
-      <c r="Y13" s="212"/>
-      <c r="Z13" s="212"/>
-      <c r="AA13" s="212"/>
-      <c r="AB13" s="212"/>
-      <c r="AC13" s="212"/>
-      <c r="AD13" s="212"/>
-      <c r="AE13" s="212"/>
-      <c r="AF13" s="212"/>
-      <c r="AG13" s="212"/>
-      <c r="AH13" s="212"/>
-      <c r="AI13" s="212"/>
-      <c r="AJ13" s="212"/>
-      <c r="AK13" s="212"/>
-      <c r="AL13" s="212"/>
-      <c r="AM13" s="212"/>
-      <c r="AN13" s="212"/>
-      <c r="AO13" s="212"/>
-      <c r="AP13" s="212"/>
-      <c r="AQ13" s="212"/>
-      <c r="AR13" s="212"/>
-      <c r="AS13" s="212"/>
-      <c r="AT13" s="212"/>
-      <c r="AU13" s="212"/>
-      <c r="AV13" s="212"/>
-      <c r="AW13" s="212"/>
-      <c r="AX13" s="212"/>
-      <c r="AY13" s="212"/>
-      <c r="AZ13" s="212"/>
-      <c r="BA13" s="212"/>
-      <c r="BB13" s="212"/>
-      <c r="BC13" s="212"/>
-      <c r="BD13" s="212"/>
-      <c r="BE13" s="212"/>
-      <c r="BF13" s="212"/>
-      <c r="BG13" s="212"/>
-      <c r="BH13" s="212"/>
-      <c r="BI13" s="212"/>
-      <c r="BJ13" s="212"/>
-      <c r="BK13" s="212"/>
-      <c r="BL13" s="212"/>
-      <c r="BM13" s="212"/>
-      <c r="BN13" s="212"/>
-      <c r="BO13" s="212"/>
-      <c r="BP13" s="212"/>
-      <c r="BQ13" s="212"/>
-      <c r="BR13" s="212"/>
-      <c r="BS13" s="212"/>
-      <c r="BT13" s="212"/>
-      <c r="BU13" s="212"/>
-      <c r="BV13" s="212"/>
-      <c r="BW13" s="212"/>
-      <c r="BX13" s="212"/>
-      <c r="BY13" s="212"/>
-      <c r="BZ13" s="212"/>
-      <c r="CA13" s="212"/>
-      <c r="CB13" s="213"/>
+      <c r="J13" s="224"/>
+      <c r="K13" s="224"/>
+      <c r="L13" s="224"/>
+      <c r="M13" s="227"/>
+      <c r="N13" s="214"/>
+      <c r="O13" s="215"/>
+      <c r="P13" s="215"/>
+      <c r="Q13" s="215"/>
+      <c r="R13" s="215"/>
+      <c r="S13" s="215"/>
+      <c r="T13" s="215"/>
+      <c r="U13" s="215"/>
+      <c r="V13" s="215"/>
+      <c r="W13" s="215"/>
+      <c r="X13" s="215"/>
+      <c r="Y13" s="215"/>
+      <c r="Z13" s="215"/>
+      <c r="AA13" s="215"/>
+      <c r="AB13" s="215"/>
+      <c r="AC13" s="215"/>
+      <c r="AD13" s="215"/>
+      <c r="AE13" s="215"/>
+      <c r="AF13" s="215"/>
+      <c r="AG13" s="215"/>
+      <c r="AH13" s="215"/>
+      <c r="AI13" s="215"/>
+      <c r="AJ13" s="215"/>
+      <c r="AK13" s="215"/>
+      <c r="AL13" s="215"/>
+      <c r="AM13" s="215"/>
+      <c r="AN13" s="215"/>
+      <c r="AO13" s="215"/>
+      <c r="AP13" s="215"/>
+      <c r="AQ13" s="215"/>
+      <c r="AR13" s="215"/>
+      <c r="AS13" s="215"/>
+      <c r="AT13" s="215"/>
+      <c r="AU13" s="215"/>
+      <c r="AV13" s="215"/>
+      <c r="AW13" s="215"/>
+      <c r="AX13" s="215"/>
+      <c r="AY13" s="215"/>
+      <c r="AZ13" s="215"/>
+      <c r="BA13" s="215"/>
+      <c r="BB13" s="215"/>
+      <c r="BC13" s="215"/>
+      <c r="BD13" s="215"/>
+      <c r="BE13" s="215"/>
+      <c r="BF13" s="215"/>
+      <c r="BG13" s="215"/>
+      <c r="BH13" s="215"/>
+      <c r="BI13" s="215"/>
+      <c r="BJ13" s="215"/>
+      <c r="BK13" s="215"/>
+      <c r="BL13" s="215"/>
+      <c r="BM13" s="215"/>
+      <c r="BN13" s="215"/>
+      <c r="BO13" s="215"/>
+      <c r="BP13" s="215"/>
+      <c r="BQ13" s="215"/>
+      <c r="BR13" s="215"/>
+      <c r="BS13" s="215"/>
+      <c r="BT13" s="215"/>
+      <c r="BU13" s="215"/>
+      <c r="BV13" s="215"/>
+      <c r="BW13" s="215"/>
+      <c r="BX13" s="215"/>
+      <c r="BY13" s="215"/>
+      <c r="BZ13" s="215"/>
+      <c r="CA13" s="215"/>
+      <c r="CB13" s="216"/>
     </row>
     <row r="14" spans="1:81" ht="15.75" customHeight="1">
-      <c r="A14" s="292"/>
-      <c r="B14" s="292"/>
-      <c r="C14" s="165"/>
-      <c r="D14" s="165"/>
+      <c r="A14" s="300"/>
+      <c r="B14" s="300"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="168"/>
       <c r="E14" s="85" t="s">
         <v>5</v>
       </c>
@@ -6287,14 +6416,14 @@
       <c r="H14" s="85"/>
       <c r="I14" s="85"/>
       <c r="J14" s="86"/>
-      <c r="K14" s="225" t="s">
+      <c r="K14" s="228" t="s">
         <v>49</v>
       </c>
-      <c r="L14" s="226"/>
-      <c r="M14" s="226"/>
-      <c r="N14" s="227"/>
+      <c r="L14" s="229"/>
+      <c r="M14" s="229"/>
+      <c r="N14" s="230"/>
       <c r="O14" s="56"/>
-      <c r="P14" s="155"/>
+      <c r="P14" s="158"/>
       <c r="Q14" s="112"/>
       <c r="R14" s="108"/>
       <c r="S14" s="108"/>
@@ -6303,51 +6432,51 @@
       <c r="V14" s="108"/>
       <c r="W14" s="108"/>
       <c r="X14" s="109"/>
-      <c r="Y14" s="155"/>
-      <c r="Z14" s="156"/>
-      <c r="AA14" s="119"/>
-      <c r="AB14" s="120"/>
-      <c r="AC14" s="121"/>
+      <c r="Y14" s="158"/>
+      <c r="Z14" s="159"/>
+      <c r="AA14" s="122"/>
+      <c r="AB14" s="123"/>
+      <c r="AC14" s="124"/>
       <c r="AD14" s="76" t="s">
         <v>14</v>
       </c>
       <c r="AE14" s="77"/>
       <c r="AF14" s="77"/>
       <c r="AG14" s="77"/>
-      <c r="AH14" s="303" t="s">
+      <c r="AH14" s="116" t="s">
         <v>57</v>
       </c>
-      <c r="AI14" s="304"/>
-      <c r="AJ14" s="304"/>
-      <c r="AK14" s="304"/>
-      <c r="AL14" s="304"/>
-      <c r="AM14" s="304"/>
-      <c r="AN14" s="304"/>
-      <c r="AO14" s="304"/>
-      <c r="AP14" s="304"/>
-      <c r="AQ14" s="304"/>
-      <c r="AR14" s="304"/>
-      <c r="AS14" s="304"/>
-      <c r="AT14" s="304"/>
-      <c r="AU14" s="304"/>
-      <c r="AV14" s="304"/>
-      <c r="AW14" s="304"/>
-      <c r="AX14" s="304"/>
-      <c r="AY14" s="304"/>
-      <c r="AZ14" s="304"/>
-      <c r="BA14" s="304"/>
-      <c r="BB14" s="304"/>
-      <c r="BC14" s="304"/>
-      <c r="BD14" s="304"/>
-      <c r="BE14" s="304"/>
-      <c r="BF14" s="304"/>
-      <c r="BG14" s="304"/>
-      <c r="BH14" s="304"/>
-      <c r="BI14" s="304"/>
-      <c r="BJ14" s="304"/>
-      <c r="BK14" s="304"/>
-      <c r="BL14" s="304"/>
-      <c r="BM14" s="305"/>
+      <c r="AI14" s="117"/>
+      <c r="AJ14" s="117"/>
+      <c r="AK14" s="117"/>
+      <c r="AL14" s="117"/>
+      <c r="AM14" s="117"/>
+      <c r="AN14" s="117"/>
+      <c r="AO14" s="117"/>
+      <c r="AP14" s="117"/>
+      <c r="AQ14" s="117"/>
+      <c r="AR14" s="117"/>
+      <c r="AS14" s="117"/>
+      <c r="AT14" s="117"/>
+      <c r="AU14" s="117"/>
+      <c r="AV14" s="117"/>
+      <c r="AW14" s="117"/>
+      <c r="AX14" s="117"/>
+      <c r="AY14" s="117"/>
+      <c r="AZ14" s="117"/>
+      <c r="BA14" s="117"/>
+      <c r="BB14" s="117"/>
+      <c r="BC14" s="117"/>
+      <c r="BD14" s="117"/>
+      <c r="BE14" s="117"/>
+      <c r="BF14" s="117"/>
+      <c r="BG14" s="117"/>
+      <c r="BH14" s="117"/>
+      <c r="BI14" s="117"/>
+      <c r="BJ14" s="117"/>
+      <c r="BK14" s="117"/>
+      <c r="BL14" s="117"/>
+      <c r="BM14" s="118"/>
       <c r="BN14" s="33"/>
       <c r="BO14" s="33"/>
       <c r="BP14" s="33"/>
@@ -6365,20 +6494,20 @@
       <c r="CB14" s="33"/>
     </row>
     <row r="15" spans="1:81" ht="15.75" customHeight="1">
-      <c r="A15" s="292"/>
-      <c r="B15" s="292"/>
-      <c r="C15" s="165"/>
-      <c r="D15" s="165"/>
+      <c r="A15" s="300"/>
+      <c r="B15" s="300"/>
+      <c r="C15" s="168"/>
+      <c r="D15" s="168"/>
       <c r="E15" s="85"/>
       <c r="F15" s="85"/>
       <c r="G15" s="85"/>
       <c r="H15" s="85"/>
       <c r="I15" s="85"/>
       <c r="J15" s="86"/>
-      <c r="K15" s="225"/>
-      <c r="L15" s="226"/>
-      <c r="M15" s="226"/>
-      <c r="N15" s="227"/>
+      <c r="K15" s="228"/>
+      <c r="L15" s="229"/>
+      <c r="M15" s="229"/>
+      <c r="N15" s="230"/>
       <c r="O15" s="53"/>
       <c r="P15" s="54"/>
       <c r="Q15" s="107"/>
@@ -6391,45 +6520,45 @@
       <c r="X15" s="111"/>
       <c r="Y15" s="54"/>
       <c r="Z15" s="73"/>
-      <c r="AA15" s="122"/>
-      <c r="AB15" s="123"/>
-      <c r="AC15" s="124"/>
+      <c r="AA15" s="125"/>
+      <c r="AB15" s="126"/>
+      <c r="AC15" s="127"/>
       <c r="AD15" s="78"/>
       <c r="AE15" s="79"/>
       <c r="AF15" s="79"/>
       <c r="AG15" s="79"/>
-      <c r="AH15" s="116"/>
-      <c r="AI15" s="117"/>
-      <c r="AJ15" s="117"/>
-      <c r="AK15" s="117"/>
-      <c r="AL15" s="117"/>
-      <c r="AM15" s="117"/>
-      <c r="AN15" s="117"/>
-      <c r="AO15" s="117"/>
-      <c r="AP15" s="117"/>
-      <c r="AQ15" s="117"/>
-      <c r="AR15" s="117"/>
-      <c r="AS15" s="117"/>
-      <c r="AT15" s="117"/>
-      <c r="AU15" s="117"/>
-      <c r="AV15" s="117"/>
-      <c r="AW15" s="117"/>
-      <c r="AX15" s="117"/>
-      <c r="AY15" s="117"/>
-      <c r="AZ15" s="117"/>
-      <c r="BA15" s="117"/>
-      <c r="BB15" s="117"/>
-      <c r="BC15" s="117"/>
-      <c r="BD15" s="117"/>
-      <c r="BE15" s="117"/>
-      <c r="BF15" s="117"/>
-      <c r="BG15" s="117"/>
-      <c r="BH15" s="117"/>
-      <c r="BI15" s="117"/>
-      <c r="BJ15" s="117"/>
-      <c r="BK15" s="117"/>
-      <c r="BL15" s="117"/>
-      <c r="BM15" s="118"/>
+      <c r="AH15" s="119"/>
+      <c r="AI15" s="120"/>
+      <c r="AJ15" s="120"/>
+      <c r="AK15" s="120"/>
+      <c r="AL15" s="120"/>
+      <c r="AM15" s="120"/>
+      <c r="AN15" s="120"/>
+      <c r="AO15" s="120"/>
+      <c r="AP15" s="120"/>
+      <c r="AQ15" s="120"/>
+      <c r="AR15" s="120"/>
+      <c r="AS15" s="120"/>
+      <c r="AT15" s="120"/>
+      <c r="AU15" s="120"/>
+      <c r="AV15" s="120"/>
+      <c r="AW15" s="120"/>
+      <c r="AX15" s="120"/>
+      <c r="AY15" s="120"/>
+      <c r="AZ15" s="120"/>
+      <c r="BA15" s="120"/>
+      <c r="BB15" s="120"/>
+      <c r="BC15" s="120"/>
+      <c r="BD15" s="120"/>
+      <c r="BE15" s="120"/>
+      <c r="BF15" s="120"/>
+      <c r="BG15" s="120"/>
+      <c r="BH15" s="120"/>
+      <c r="BI15" s="120"/>
+      <c r="BJ15" s="120"/>
+      <c r="BK15" s="120"/>
+      <c r="BL15" s="120"/>
+      <c r="BM15" s="121"/>
       <c r="BN15" s="5"/>
       <c r="BO15" s="9"/>
       <c r="BP15" s="9"/>
@@ -6448,10 +6577,10 @@
       <c r="CC15" s="2"/>
     </row>
     <row r="16" spans="1:81" ht="12.75" customHeight="1">
-      <c r="A16" s="292"/>
-      <c r="B16" s="292"/>
-      <c r="C16" s="165"/>
-      <c r="D16" s="165"/>
+      <c r="A16" s="300"/>
+      <c r="B16" s="300"/>
+      <c r="C16" s="168"/>
+      <c r="D16" s="168"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -6532,142 +6661,142 @@
       <c r="CB16" s="9"/>
     </row>
     <row r="17" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A17" s="292"/>
-      <c r="B17" s="292"/>
-      <c r="C17" s="165"/>
-      <c r="D17" s="165"/>
+      <c r="A17" s="300"/>
+      <c r="B17" s="300"/>
+      <c r="C17" s="168"/>
+      <c r="D17" s="168"/>
       <c r="F17" s="18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A18" s="292"/>
-      <c r="B18" s="292"/>
-      <c r="C18" s="165"/>
-      <c r="D18" s="165"/>
+      <c r="A18" s="300"/>
+      <c r="B18" s="300"/>
+      <c r="C18" s="168"/>
+      <c r="D18" s="168"/>
       <c r="F18" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="AN18" s="135" t="s">
+      <c r="AN18" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="AO18" s="135"/>
-      <c r="AP18" s="135"/>
-      <c r="AQ18" s="135"/>
-      <c r="AR18" s="135"/>
-      <c r="AS18" s="135"/>
-      <c r="AT18" s="135"/>
-      <c r="AU18" s="135"/>
-      <c r="AV18" s="135"/>
-      <c r="AW18" s="135"/>
-      <c r="AX18" s="135"/>
-      <c r="AY18" s="135"/>
-      <c r="AZ18" s="135"/>
-      <c r="BA18" s="135"/>
-      <c r="BB18" s="135"/>
-      <c r="BC18" s="135"/>
-      <c r="BD18" s="135"/>
-      <c r="BE18" s="135"/>
-      <c r="BF18" s="135"/>
-      <c r="BG18" s="135"/>
-      <c r="BH18" s="135"/>
-      <c r="BI18" s="135"/>
-      <c r="BJ18" s="135"/>
-      <c r="BK18" s="135"/>
-      <c r="BL18" s="135"/>
-      <c r="BM18" s="135"/>
-      <c r="BN18" s="135"/>
-      <c r="BO18" s="135"/>
-      <c r="BP18" s="135"/>
-      <c r="BQ18" s="135"/>
-      <c r="BR18" s="135"/>
-      <c r="BS18" s="135"/>
-      <c r="BT18" s="135"/>
-      <c r="BU18" s="135"/>
-      <c r="BV18" s="135"/>
-      <c r="BW18" s="135"/>
+      <c r="AO18" s="138"/>
+      <c r="AP18" s="138"/>
+      <c r="AQ18" s="138"/>
+      <c r="AR18" s="138"/>
+      <c r="AS18" s="138"/>
+      <c r="AT18" s="138"/>
+      <c r="AU18" s="138"/>
+      <c r="AV18" s="138"/>
+      <c r="AW18" s="138"/>
+      <c r="AX18" s="138"/>
+      <c r="AY18" s="138"/>
+      <c r="AZ18" s="138"/>
+      <c r="BA18" s="138"/>
+      <c r="BB18" s="138"/>
+      <c r="BC18" s="138"/>
+      <c r="BD18" s="138"/>
+      <c r="BE18" s="138"/>
+      <c r="BF18" s="138"/>
+      <c r="BG18" s="138"/>
+      <c r="BH18" s="138"/>
+      <c r="BI18" s="138"/>
+      <c r="BJ18" s="138"/>
+      <c r="BK18" s="138"/>
+      <c r="BL18" s="138"/>
+      <c r="BM18" s="138"/>
+      <c r="BN18" s="138"/>
+      <c r="BO18" s="138"/>
+      <c r="BP18" s="138"/>
+      <c r="BQ18" s="138"/>
+      <c r="BR18" s="138"/>
+      <c r="BS18" s="138"/>
+      <c r="BT18" s="138"/>
+      <c r="BU18" s="138"/>
+      <c r="BV18" s="138"/>
+      <c r="BW18" s="138"/>
     </row>
     <row r="19" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A19" s="292"/>
-      <c r="B19" s="292"/>
-      <c r="C19" s="165"/>
-      <c r="D19" s="165"/>
-      <c r="E19" s="249" t="s">
+      <c r="A19" s="300"/>
+      <c r="B19" s="300"/>
+      <c r="C19" s="168"/>
+      <c r="D19" s="168"/>
+      <c r="E19" s="252" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="250"/>
-      <c r="G19" s="250"/>
-      <c r="H19" s="250"/>
-      <c r="I19" s="250"/>
-      <c r="J19" s="250"/>
-      <c r="K19" s="250"/>
-      <c r="L19" s="250"/>
-      <c r="M19" s="250"/>
-      <c r="N19" s="250"/>
-      <c r="O19" s="250"/>
-      <c r="P19" s="250"/>
-      <c r="Q19" s="250"/>
-      <c r="R19" s="250"/>
-      <c r="S19" s="250"/>
-      <c r="T19" s="250"/>
-      <c r="U19" s="250"/>
-      <c r="V19" s="250"/>
-      <c r="W19" s="250"/>
-      <c r="X19" s="250"/>
-      <c r="Y19" s="250"/>
-      <c r="Z19" s="250"/>
-      <c r="AA19" s="250"/>
-      <c r="AB19" s="250"/>
-      <c r="AC19" s="250"/>
-      <c r="AD19" s="250"/>
-      <c r="AE19" s="250"/>
-      <c r="AF19" s="250"/>
-      <c r="AG19" s="250"/>
-      <c r="AH19" s="250"/>
-      <c r="AI19" s="250"/>
-      <c r="AJ19" s="250"/>
-      <c r="AN19" s="135"/>
-      <c r="AO19" s="135"/>
-      <c r="AP19" s="135"/>
-      <c r="AQ19" s="135"/>
-      <c r="AR19" s="135"/>
-      <c r="AS19" s="135"/>
-      <c r="AT19" s="135"/>
-      <c r="AU19" s="135"/>
-      <c r="AV19" s="135"/>
-      <c r="AW19" s="135"/>
-      <c r="AX19" s="135"/>
-      <c r="AY19" s="135"/>
-      <c r="AZ19" s="135"/>
-      <c r="BA19" s="135"/>
-      <c r="BB19" s="135"/>
-      <c r="BC19" s="135"/>
-      <c r="BD19" s="135"/>
-      <c r="BE19" s="135"/>
-      <c r="BF19" s="135"/>
-      <c r="BG19" s="135"/>
-      <c r="BH19" s="135"/>
-      <c r="BI19" s="135"/>
-      <c r="BJ19" s="135"/>
-      <c r="BK19" s="135"/>
-      <c r="BL19" s="135"/>
-      <c r="BM19" s="135"/>
-      <c r="BN19" s="135"/>
-      <c r="BO19" s="135"/>
-      <c r="BP19" s="135"/>
-      <c r="BQ19" s="135"/>
-      <c r="BR19" s="135"/>
-      <c r="BS19" s="135"/>
-      <c r="BT19" s="135"/>
-      <c r="BU19" s="135"/>
-      <c r="BV19" s="135"/>
-      <c r="BW19" s="135"/>
+      <c r="F19" s="253"/>
+      <c r="G19" s="253"/>
+      <c r="H19" s="253"/>
+      <c r="I19" s="253"/>
+      <c r="J19" s="253"/>
+      <c r="K19" s="253"/>
+      <c r="L19" s="253"/>
+      <c r="M19" s="253"/>
+      <c r="N19" s="253"/>
+      <c r="O19" s="253"/>
+      <c r="P19" s="253"/>
+      <c r="Q19" s="253"/>
+      <c r="R19" s="253"/>
+      <c r="S19" s="253"/>
+      <c r="T19" s="253"/>
+      <c r="U19" s="253"/>
+      <c r="V19" s="253"/>
+      <c r="W19" s="253"/>
+      <c r="X19" s="253"/>
+      <c r="Y19" s="253"/>
+      <c r="Z19" s="253"/>
+      <c r="AA19" s="253"/>
+      <c r="AB19" s="253"/>
+      <c r="AC19" s="253"/>
+      <c r="AD19" s="253"/>
+      <c r="AE19" s="253"/>
+      <c r="AF19" s="253"/>
+      <c r="AG19" s="253"/>
+      <c r="AH19" s="253"/>
+      <c r="AI19" s="253"/>
+      <c r="AJ19" s="253"/>
+      <c r="AN19" s="138"/>
+      <c r="AO19" s="138"/>
+      <c r="AP19" s="138"/>
+      <c r="AQ19" s="138"/>
+      <c r="AR19" s="138"/>
+      <c r="AS19" s="138"/>
+      <c r="AT19" s="138"/>
+      <c r="AU19" s="138"/>
+      <c r="AV19" s="138"/>
+      <c r="AW19" s="138"/>
+      <c r="AX19" s="138"/>
+      <c r="AY19" s="138"/>
+      <c r="AZ19" s="138"/>
+      <c r="BA19" s="138"/>
+      <c r="BB19" s="138"/>
+      <c r="BC19" s="138"/>
+      <c r="BD19" s="138"/>
+      <c r="BE19" s="138"/>
+      <c r="BF19" s="138"/>
+      <c r="BG19" s="138"/>
+      <c r="BH19" s="138"/>
+      <c r="BI19" s="138"/>
+      <c r="BJ19" s="138"/>
+      <c r="BK19" s="138"/>
+      <c r="BL19" s="138"/>
+      <c r="BM19" s="138"/>
+      <c r="BN19" s="138"/>
+      <c r="BO19" s="138"/>
+      <c r="BP19" s="138"/>
+      <c r="BQ19" s="138"/>
+      <c r="BR19" s="138"/>
+      <c r="BS19" s="138"/>
+      <c r="BT19" s="138"/>
+      <c r="BU19" s="138"/>
+      <c r="BV19" s="138"/>
+      <c r="BW19" s="138"/>
     </row>
     <row r="20" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A20" s="292"/>
-      <c r="B20" s="292"/>
-      <c r="C20" s="165"/>
-      <c r="D20" s="165"/>
+      <c r="A20" s="300"/>
+      <c r="B20" s="300"/>
+      <c r="C20" s="168"/>
+      <c r="D20" s="168"/>
       <c r="E20" s="99" t="s">
         <v>43</v>
       </c>
@@ -6724,12 +6853,12 @@
       </c>
       <c r="AY20" s="19"/>
       <c r="AZ20" s="19"/>
-      <c r="BA20" s="125"/>
-      <c r="BB20" s="125"/>
-      <c r="BC20" s="125"/>
-      <c r="BD20" s="125"/>
-      <c r="BE20" s="125"/>
-      <c r="BF20" s="125"/>
+      <c r="BA20" s="128"/>
+      <c r="BB20" s="128"/>
+      <c r="BC20" s="128"/>
+      <c r="BD20" s="128"/>
+      <c r="BE20" s="128"/>
+      <c r="BF20" s="128"/>
       <c r="BG20" s="102"/>
       <c r="BH20" s="103"/>
       <c r="BI20" s="103"/>
@@ -6741,17 +6870,17 @@
       <c r="BO20" s="104"/>
     </row>
     <row r="21" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A21" s="292"/>
-      <c r="B21" s="292"/>
-      <c r="C21" s="165"/>
-      <c r="D21" s="165"/>
-      <c r="E21" s="166"/>
+      <c r="A21" s="300"/>
+      <c r="B21" s="300"/>
+      <c r="C21" s="168"/>
+      <c r="D21" s="168"/>
+      <c r="E21" s="169"/>
       <c r="F21" s="74"/>
       <c r="G21" s="74"/>
       <c r="H21" s="74"/>
       <c r="I21" s="74"/>
       <c r="J21" s="74"/>
-      <c r="K21" s="234"/>
+      <c r="K21" s="237"/>
       <c r="L21" s="71"/>
       <c r="M21" s="71"/>
       <c r="N21" s="72"/>
@@ -6761,7 +6890,7 @@
       <c r="R21" s="74"/>
       <c r="S21" s="74"/>
       <c r="T21" s="75"/>
-      <c r="U21" s="169"/>
+      <c r="U21" s="172"/>
       <c r="V21" s="74"/>
       <c r="W21" s="74"/>
       <c r="X21" s="74"/>
@@ -6769,13 +6898,13 @@
       <c r="Z21" s="56"/>
       <c r="AA21" s="55"/>
       <c r="AB21" s="80"/>
-      <c r="AC21" s="126" t="s">
+      <c r="AC21" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="AD21" s="127"/>
-      <c r="AE21" s="127"/>
-      <c r="AF21" s="128"/>
-      <c r="AG21" s="217"/>
+      <c r="AD21" s="130"/>
+      <c r="AE21" s="130"/>
+      <c r="AF21" s="131"/>
+      <c r="AG21" s="220"/>
       <c r="AH21" s="105"/>
       <c r="AI21" s="105"/>
       <c r="AJ21" s="106"/>
@@ -6786,14 +6915,14 @@
       <c r="AO21" s="51"/>
       <c r="AP21" s="52"/>
       <c r="AQ21" s="52"/>
-      <c r="AR21" s="134"/>
-      <c r="AS21" s="170" t="s">
+      <c r="AR21" s="137"/>
+      <c r="AS21" s="173" t="s">
         <v>41</v>
       </c>
-      <c r="AT21" s="171"/>
-      <c r="AU21" s="171"/>
-      <c r="AV21" s="171"/>
-      <c r="AW21" s="172"/>
+      <c r="AT21" s="174"/>
+      <c r="AU21" s="174"/>
+      <c r="AV21" s="174"/>
+      <c r="AW21" s="175"/>
       <c r="AX21" s="21" t="s">
         <v>19</v>
       </c>
@@ -6818,17 +6947,17 @@
       <c r="BO21" s="114"/>
     </row>
     <row r="22" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A22" s="292"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="165"/>
-      <c r="D22" s="165"/>
-      <c r="E22" s="166"/>
+      <c r="A22" s="300"/>
+      <c r="B22" s="300"/>
+      <c r="C22" s="168"/>
+      <c r="D22" s="168"/>
+      <c r="E22" s="169"/>
       <c r="F22" s="74"/>
       <c r="G22" s="74"/>
       <c r="H22" s="74"/>
       <c r="I22" s="74"/>
       <c r="J22" s="74"/>
-      <c r="K22" s="234"/>
+      <c r="K22" s="237"/>
       <c r="L22" s="71"/>
       <c r="M22" s="71"/>
       <c r="N22" s="72"/>
@@ -6838,7 +6967,7 @@
       <c r="R22" s="74"/>
       <c r="S22" s="74"/>
       <c r="T22" s="75"/>
-      <c r="U22" s="169"/>
+      <c r="U22" s="172"/>
       <c r="V22" s="74"/>
       <c r="W22" s="74"/>
       <c r="X22" s="74"/>
@@ -6846,10 +6975,10 @@
       <c r="Z22" s="53"/>
       <c r="AA22" s="57"/>
       <c r="AB22" s="81"/>
-      <c r="AC22" s="129"/>
-      <c r="AD22" s="130"/>
-      <c r="AE22" s="130"/>
-      <c r="AF22" s="131"/>
+      <c r="AC22" s="132"/>
+      <c r="AD22" s="133"/>
+      <c r="AE22" s="133"/>
+      <c r="AF22" s="134"/>
       <c r="AG22" s="111"/>
       <c r="AH22" s="54"/>
       <c r="AI22" s="54"/>
@@ -6862,11 +6991,11 @@
       <c r="AP22" s="54"/>
       <c r="AQ22" s="54"/>
       <c r="AR22" s="73"/>
-      <c r="AS22" s="173"/>
-      <c r="AT22" s="174"/>
-      <c r="AU22" s="174"/>
-      <c r="AV22" s="174"/>
-      <c r="AW22" s="175"/>
+      <c r="AS22" s="176"/>
+      <c r="AT22" s="177"/>
+      <c r="AU22" s="177"/>
+      <c r="AV22" s="177"/>
+      <c r="AW22" s="178"/>
       <c r="AX22" s="13"/>
       <c r="AY22" s="4"/>
       <c r="AZ22" s="64"/>
@@ -6887,15 +7016,15 @@
       <c r="BO22" s="115"/>
     </row>
     <row r="23" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A23" s="292"/>
-      <c r="B23" s="292"/>
-      <c r="C23" s="165"/>
-      <c r="D23" s="165"/>
-      <c r="E23" s="283" t="s">
+      <c r="A23" s="300"/>
+      <c r="B23" s="300"/>
+      <c r="C23" s="168"/>
+      <c r="D23" s="168"/>
+      <c r="E23" s="291" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="284"/>
-      <c r="G23" s="285"/>
+      <c r="F23" s="292"/>
+      <c r="G23" s="293"/>
       <c r="H23" s="48" t="s">
         <v>28</v>
       </c>
@@ -6977,262 +7106,262 @@
       <c r="CB23" s="101"/>
     </row>
     <row r="24" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A24" s="292"/>
-      <c r="B24" s="292"/>
-      <c r="C24" s="165"/>
-      <c r="D24" s="165"/>
+      <c r="A24" s="300"/>
+      <c r="B24" s="300"/>
+      <c r="C24" s="168"/>
+      <c r="D24" s="168"/>
       <c r="E24" s="65"/>
       <c r="F24" s="66"/>
-      <c r="G24" s="286"/>
-      <c r="H24" s="235"/>
+      <c r="G24" s="294"/>
+      <c r="H24" s="238"/>
       <c r="I24" s="56"/>
-      <c r="J24" s="151"/>
+      <c r="J24" s="154"/>
       <c r="K24" s="56"/>
-      <c r="L24" s="151"/>
+      <c r="L24" s="154"/>
       <c r="M24" s="56"/>
-      <c r="N24" s="151"/>
+      <c r="N24" s="154"/>
       <c r="O24" s="56"/>
-      <c r="P24" s="151"/>
+      <c r="P24" s="154"/>
       <c r="Q24" s="56"/>
-      <c r="R24" s="151"/>
+      <c r="R24" s="154"/>
       <c r="S24" s="56"/>
-      <c r="T24" s="151"/>
+      <c r="T24" s="154"/>
       <c r="U24" s="80"/>
-      <c r="V24" s="257" t="s">
+      <c r="V24" s="260" t="s">
         <v>18</v>
       </c>
-      <c r="W24" s="258"/>
-      <c r="X24" s="258"/>
-      <c r="Y24" s="258"/>
-      <c r="Z24" s="258"/>
-      <c r="AA24" s="258"/>
-      <c r="AB24" s="258"/>
-      <c r="AC24" s="258"/>
-      <c r="AD24" s="258"/>
-      <c r="AE24" s="259"/>
-      <c r="AF24" s="274" t="s">
+      <c r="W24" s="261"/>
+      <c r="X24" s="261"/>
+      <c r="Y24" s="261"/>
+      <c r="Z24" s="261"/>
+      <c r="AA24" s="261"/>
+      <c r="AB24" s="261"/>
+      <c r="AC24" s="261"/>
+      <c r="AD24" s="261"/>
+      <c r="AE24" s="262"/>
+      <c r="AF24" s="282" t="s">
         <v>15</v>
       </c>
-      <c r="AG24" s="275"/>
-      <c r="AH24" s="275"/>
-      <c r="AI24" s="275"/>
-      <c r="AJ24" s="241"/>
-      <c r="AK24" s="241"/>
-      <c r="AL24" s="241"/>
-      <c r="AM24" s="241"/>
-      <c r="AN24" s="241"/>
-      <c r="AO24" s="241"/>
-      <c r="AP24" s="241"/>
-      <c r="AQ24" s="241"/>
-      <c r="AR24" s="241"/>
-      <c r="AS24" s="241"/>
-      <c r="AT24" s="241"/>
-      <c r="AU24" s="241"/>
-      <c r="AV24" s="241"/>
-      <c r="AW24" s="241"/>
-      <c r="AX24" s="241"/>
-      <c r="AY24" s="241"/>
-      <c r="AZ24" s="241"/>
-      <c r="BA24" s="241"/>
-      <c r="BB24" s="241"/>
-      <c r="BC24" s="241"/>
-      <c r="BD24" s="241"/>
-      <c r="BE24" s="241"/>
-      <c r="BF24" s="241"/>
-      <c r="BG24" s="241"/>
-      <c r="BH24" s="241"/>
-      <c r="BI24" s="241"/>
-      <c r="BJ24" s="241"/>
-      <c r="BK24" s="241"/>
-      <c r="BL24" s="241"/>
-      <c r="BM24" s="242"/>
-      <c r="BN24" s="243" t="s">
+      <c r="AG24" s="283"/>
+      <c r="AH24" s="283"/>
+      <c r="AI24" s="283"/>
+      <c r="AJ24" s="244"/>
+      <c r="AK24" s="244"/>
+      <c r="AL24" s="244"/>
+      <c r="AM24" s="244"/>
+      <c r="AN24" s="244"/>
+      <c r="AO24" s="244"/>
+      <c r="AP24" s="244"/>
+      <c r="AQ24" s="244"/>
+      <c r="AR24" s="244"/>
+      <c r="AS24" s="244"/>
+      <c r="AT24" s="244"/>
+      <c r="AU24" s="244"/>
+      <c r="AV24" s="244"/>
+      <c r="AW24" s="244"/>
+      <c r="AX24" s="244"/>
+      <c r="AY24" s="244"/>
+      <c r="AZ24" s="244"/>
+      <c r="BA24" s="244"/>
+      <c r="BB24" s="244"/>
+      <c r="BC24" s="244"/>
+      <c r="BD24" s="244"/>
+      <c r="BE24" s="244"/>
+      <c r="BF24" s="244"/>
+      <c r="BG24" s="244"/>
+      <c r="BH24" s="244"/>
+      <c r="BI24" s="244"/>
+      <c r="BJ24" s="244"/>
+      <c r="BK24" s="244"/>
+      <c r="BL24" s="244"/>
+      <c r="BM24" s="245"/>
+      <c r="BN24" s="246" t="s">
         <v>50</v>
       </c>
-      <c r="BO24" s="244"/>
-      <c r="BP24" s="245"/>
-      <c r="BQ24" s="236"/>
-      <c r="BR24" s="252"/>
-      <c r="BS24" s="238"/>
-      <c r="BT24" s="240"/>
-      <c r="BU24" s="236"/>
-      <c r="BV24" s="252"/>
-      <c r="BW24" s="238"/>
-      <c r="BX24" s="240"/>
-      <c r="BY24" s="236"/>
-      <c r="BZ24" s="252"/>
-      <c r="CA24" s="238"/>
-      <c r="CB24" s="240"/>
+      <c r="BO24" s="247"/>
+      <c r="BP24" s="248"/>
+      <c r="BQ24" s="239"/>
+      <c r="BR24" s="255"/>
+      <c r="BS24" s="241"/>
+      <c r="BT24" s="243"/>
+      <c r="BU24" s="239"/>
+      <c r="BV24" s="255"/>
+      <c r="BW24" s="241"/>
+      <c r="BX24" s="243"/>
+      <c r="BY24" s="239"/>
+      <c r="BZ24" s="255"/>
+      <c r="CA24" s="241"/>
+      <c r="CB24" s="243"/>
     </row>
     <row r="25" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A25" s="292"/>
-      <c r="B25" s="292"/>
-      <c r="C25" s="165"/>
-      <c r="D25" s="165"/>
+      <c r="A25" s="300"/>
+      <c r="B25" s="300"/>
+      <c r="C25" s="168"/>
+      <c r="D25" s="168"/>
       <c r="E25" s="65"/>
       <c r="F25" s="66"/>
-      <c r="G25" s="286"/>
-      <c r="H25" s="236"/>
+      <c r="G25" s="294"/>
+      <c r="H25" s="239"/>
       <c r="I25" s="51"/>
-      <c r="J25" s="238"/>
+      <c r="J25" s="241"/>
       <c r="K25" s="51"/>
-      <c r="L25" s="238"/>
+      <c r="L25" s="241"/>
       <c r="M25" s="51"/>
-      <c r="N25" s="238"/>
+      <c r="N25" s="241"/>
       <c r="O25" s="51"/>
-      <c r="P25" s="238"/>
+      <c r="P25" s="241"/>
       <c r="Q25" s="51"/>
-      <c r="R25" s="238"/>
+      <c r="R25" s="241"/>
       <c r="S25" s="51"/>
-      <c r="T25" s="238"/>
-      <c r="U25" s="240"/>
-      <c r="V25" s="253"/>
-      <c r="W25" s="254"/>
-      <c r="X25" s="260"/>
-      <c r="Y25" s="254"/>
-      <c r="Z25" s="260"/>
-      <c r="AA25" s="254"/>
-      <c r="AB25" s="260"/>
-      <c r="AC25" s="254"/>
-      <c r="AD25" s="260"/>
-      <c r="AE25" s="276"/>
-      <c r="AF25" s="262"/>
-      <c r="AG25" s="209"/>
-      <c r="AH25" s="209"/>
-      <c r="AI25" s="209"/>
-      <c r="AJ25" s="209"/>
-      <c r="AK25" s="209"/>
-      <c r="AL25" s="209"/>
-      <c r="AM25" s="209"/>
-      <c r="AN25" s="209"/>
-      <c r="AO25" s="209"/>
-      <c r="AP25" s="209"/>
-      <c r="AQ25" s="209"/>
-      <c r="AR25" s="209"/>
-      <c r="AS25" s="209"/>
-      <c r="AT25" s="209"/>
-      <c r="AU25" s="209"/>
-      <c r="AV25" s="209"/>
-      <c r="AW25" s="209"/>
-      <c r="AX25" s="209"/>
-      <c r="AY25" s="209"/>
-      <c r="AZ25" s="209"/>
-      <c r="BA25" s="209"/>
-      <c r="BB25" s="209"/>
-      <c r="BC25" s="209"/>
-      <c r="BD25" s="209"/>
-      <c r="BE25" s="209"/>
-      <c r="BF25" s="209"/>
-      <c r="BG25" s="209"/>
-      <c r="BH25" s="209"/>
-      <c r="BI25" s="209"/>
-      <c r="BJ25" s="209"/>
-      <c r="BK25" s="209"/>
-      <c r="BL25" s="209"/>
-      <c r="BM25" s="210"/>
-      <c r="BN25" s="246"/>
-      <c r="BO25" s="244"/>
-      <c r="BP25" s="245"/>
-      <c r="BQ25" s="236"/>
-      <c r="BR25" s="252"/>
-      <c r="BS25" s="238"/>
-      <c r="BT25" s="240"/>
-      <c r="BU25" s="236"/>
-      <c r="BV25" s="252"/>
-      <c r="BW25" s="238"/>
-      <c r="BX25" s="240"/>
-      <c r="BY25" s="236"/>
-      <c r="BZ25" s="252"/>
-      <c r="CA25" s="238"/>
-      <c r="CB25" s="240"/>
+      <c r="T25" s="241"/>
+      <c r="U25" s="243"/>
+      <c r="V25" s="256"/>
+      <c r="W25" s="257"/>
+      <c r="X25" s="263"/>
+      <c r="Y25" s="257"/>
+      <c r="Z25" s="263"/>
+      <c r="AA25" s="257"/>
+      <c r="AB25" s="263"/>
+      <c r="AC25" s="257"/>
+      <c r="AD25" s="263"/>
+      <c r="AE25" s="284"/>
+      <c r="AF25" s="265"/>
+      <c r="AG25" s="212"/>
+      <c r="AH25" s="212"/>
+      <c r="AI25" s="212"/>
+      <c r="AJ25" s="212"/>
+      <c r="AK25" s="212"/>
+      <c r="AL25" s="212"/>
+      <c r="AM25" s="212"/>
+      <c r="AN25" s="212"/>
+      <c r="AO25" s="212"/>
+      <c r="AP25" s="212"/>
+      <c r="AQ25" s="212"/>
+      <c r="AR25" s="212"/>
+      <c r="AS25" s="212"/>
+      <c r="AT25" s="212"/>
+      <c r="AU25" s="212"/>
+      <c r="AV25" s="212"/>
+      <c r="AW25" s="212"/>
+      <c r="AX25" s="212"/>
+      <c r="AY25" s="212"/>
+      <c r="AZ25" s="212"/>
+      <c r="BA25" s="212"/>
+      <c r="BB25" s="212"/>
+      <c r="BC25" s="212"/>
+      <c r="BD25" s="212"/>
+      <c r="BE25" s="212"/>
+      <c r="BF25" s="212"/>
+      <c r="BG25" s="212"/>
+      <c r="BH25" s="212"/>
+      <c r="BI25" s="212"/>
+      <c r="BJ25" s="212"/>
+      <c r="BK25" s="212"/>
+      <c r="BL25" s="212"/>
+      <c r="BM25" s="213"/>
+      <c r="BN25" s="249"/>
+      <c r="BO25" s="247"/>
+      <c r="BP25" s="248"/>
+      <c r="BQ25" s="239"/>
+      <c r="BR25" s="255"/>
+      <c r="BS25" s="241"/>
+      <c r="BT25" s="243"/>
+      <c r="BU25" s="239"/>
+      <c r="BV25" s="255"/>
+      <c r="BW25" s="241"/>
+      <c r="BX25" s="243"/>
+      <c r="BY25" s="239"/>
+      <c r="BZ25" s="255"/>
+      <c r="CA25" s="241"/>
+      <c r="CB25" s="243"/>
     </row>
     <row r="26" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A26" s="292"/>
-      <c r="B26" s="292"/>
-      <c r="C26" s="165"/>
-      <c r="D26" s="165"/>
+      <c r="A26" s="300"/>
+      <c r="B26" s="300"/>
+      <c r="C26" s="168"/>
+      <c r="D26" s="168"/>
       <c r="E26" s="68"/>
       <c r="F26" s="69"/>
-      <c r="G26" s="287"/>
-      <c r="H26" s="237"/>
+      <c r="G26" s="295"/>
+      <c r="H26" s="240"/>
       <c r="I26" s="53"/>
-      <c r="J26" s="239"/>
+      <c r="J26" s="242"/>
       <c r="K26" s="53"/>
-      <c r="L26" s="239"/>
+      <c r="L26" s="242"/>
       <c r="M26" s="53"/>
-      <c r="N26" s="239"/>
+      <c r="N26" s="242"/>
       <c r="O26" s="53"/>
-      <c r="P26" s="239"/>
+      <c r="P26" s="242"/>
       <c r="Q26" s="53"/>
-      <c r="R26" s="239"/>
+      <c r="R26" s="242"/>
       <c r="S26" s="53"/>
-      <c r="T26" s="239"/>
+      <c r="T26" s="242"/>
       <c r="U26" s="81"/>
-      <c r="V26" s="255"/>
-      <c r="W26" s="256"/>
-      <c r="X26" s="261"/>
-      <c r="Y26" s="256"/>
-      <c r="Z26" s="261"/>
-      <c r="AA26" s="256"/>
-      <c r="AB26" s="261"/>
-      <c r="AC26" s="256"/>
-      <c r="AD26" s="261"/>
-      <c r="AE26" s="277"/>
-      <c r="AF26" s="263"/>
-      <c r="AG26" s="264"/>
-      <c r="AH26" s="264"/>
-      <c r="AI26" s="264"/>
-      <c r="AJ26" s="264"/>
-      <c r="AK26" s="264"/>
-      <c r="AL26" s="264"/>
-      <c r="AM26" s="264"/>
-      <c r="AN26" s="264"/>
-      <c r="AO26" s="264"/>
-      <c r="AP26" s="264"/>
-      <c r="AQ26" s="264"/>
-      <c r="AR26" s="264"/>
-      <c r="AS26" s="264"/>
-      <c r="AT26" s="264"/>
-      <c r="AU26" s="264"/>
-      <c r="AV26" s="264"/>
-      <c r="AW26" s="264"/>
-      <c r="AX26" s="264"/>
-      <c r="AY26" s="264"/>
-      <c r="AZ26" s="264"/>
-      <c r="BA26" s="264"/>
-      <c r="BB26" s="264"/>
-      <c r="BC26" s="264"/>
-      <c r="BD26" s="264"/>
-      <c r="BE26" s="264"/>
-      <c r="BF26" s="264"/>
-      <c r="BG26" s="264"/>
-      <c r="BH26" s="264"/>
-      <c r="BI26" s="264"/>
-      <c r="BJ26" s="264"/>
-      <c r="BK26" s="264"/>
-      <c r="BL26" s="264"/>
-      <c r="BM26" s="265"/>
-      <c r="BN26" s="246"/>
-      <c r="BO26" s="244"/>
-      <c r="BP26" s="245"/>
-      <c r="BQ26" s="236"/>
-      <c r="BR26" s="252"/>
-      <c r="BS26" s="238"/>
-      <c r="BT26" s="251"/>
-      <c r="BU26" s="236"/>
-      <c r="BV26" s="252"/>
-      <c r="BW26" s="238"/>
-      <c r="BX26" s="251"/>
-      <c r="BY26" s="236"/>
-      <c r="BZ26" s="252"/>
-      <c r="CA26" s="238"/>
-      <c r="CB26" s="251"/>
+      <c r="V26" s="258"/>
+      <c r="W26" s="259"/>
+      <c r="X26" s="264"/>
+      <c r="Y26" s="259"/>
+      <c r="Z26" s="264"/>
+      <c r="AA26" s="259"/>
+      <c r="AB26" s="264"/>
+      <c r="AC26" s="259"/>
+      <c r="AD26" s="264"/>
+      <c r="AE26" s="285"/>
+      <c r="AF26" s="266"/>
+      <c r="AG26" s="267"/>
+      <c r="AH26" s="267"/>
+      <c r="AI26" s="267"/>
+      <c r="AJ26" s="267"/>
+      <c r="AK26" s="267"/>
+      <c r="AL26" s="267"/>
+      <c r="AM26" s="267"/>
+      <c r="AN26" s="267"/>
+      <c r="AO26" s="267"/>
+      <c r="AP26" s="267"/>
+      <c r="AQ26" s="267"/>
+      <c r="AR26" s="267"/>
+      <c r="AS26" s="267"/>
+      <c r="AT26" s="267"/>
+      <c r="AU26" s="267"/>
+      <c r="AV26" s="267"/>
+      <c r="AW26" s="267"/>
+      <c r="AX26" s="267"/>
+      <c r="AY26" s="267"/>
+      <c r="AZ26" s="267"/>
+      <c r="BA26" s="267"/>
+      <c r="BB26" s="267"/>
+      <c r="BC26" s="267"/>
+      <c r="BD26" s="267"/>
+      <c r="BE26" s="267"/>
+      <c r="BF26" s="267"/>
+      <c r="BG26" s="267"/>
+      <c r="BH26" s="267"/>
+      <c r="BI26" s="267"/>
+      <c r="BJ26" s="267"/>
+      <c r="BK26" s="267"/>
+      <c r="BL26" s="267"/>
+      <c r="BM26" s="268"/>
+      <c r="BN26" s="249"/>
+      <c r="BO26" s="247"/>
+      <c r="BP26" s="248"/>
+      <c r="BQ26" s="239"/>
+      <c r="BR26" s="255"/>
+      <c r="BS26" s="241"/>
+      <c r="BT26" s="254"/>
+      <c r="BU26" s="239"/>
+      <c r="BV26" s="255"/>
+      <c r="BW26" s="241"/>
+      <c r="BX26" s="254"/>
+      <c r="BY26" s="239"/>
+      <c r="BZ26" s="255"/>
+      <c r="CA26" s="241"/>
+      <c r="CB26" s="254"/>
     </row>
     <row r="27" spans="1:83" ht="15.75" customHeight="1">
-      <c r="A27" s="292"/>
-      <c r="B27" s="292"/>
-      <c r="C27" s="165"/>
-      <c r="D27" s="165"/>
+      <c r="A27" s="300"/>
+      <c r="B27" s="300"/>
+      <c r="C27" s="168"/>
+      <c r="D27" s="168"/>
       <c r="E27" s="89" t="s">
         <v>26</v>
       </c>
@@ -7246,88 +7375,88 @@
       <c r="K27" s="46"/>
       <c r="L27" s="46"/>
       <c r="M27" s="47"/>
-      <c r="N27" s="288"/>
-      <c r="O27" s="215"/>
-      <c r="P27" s="215"/>
-      <c r="Q27" s="215"/>
-      <c r="R27" s="215"/>
-      <c r="S27" s="215"/>
-      <c r="T27" s="215"/>
-      <c r="U27" s="215"/>
-      <c r="V27" s="215"/>
-      <c r="W27" s="215"/>
-      <c r="X27" s="215"/>
-      <c r="Y27" s="215"/>
-      <c r="Z27" s="215"/>
-      <c r="AA27" s="215"/>
-      <c r="AB27" s="215"/>
-      <c r="AC27" s="215"/>
-      <c r="AD27" s="215"/>
-      <c r="AE27" s="215"/>
-      <c r="AF27" s="215"/>
-      <c r="AG27" s="215"/>
-      <c r="AH27" s="215"/>
-      <c r="AI27" s="215"/>
-      <c r="AJ27" s="215"/>
-      <c r="AK27" s="215"/>
-      <c r="AL27" s="215"/>
-      <c r="AM27" s="215"/>
-      <c r="AN27" s="215"/>
-      <c r="AO27" s="215"/>
-      <c r="AP27" s="215"/>
-      <c r="AQ27" s="215"/>
-      <c r="AR27" s="215"/>
-      <c r="AS27" s="215"/>
-      <c r="AT27" s="215"/>
-      <c r="AU27" s="215"/>
-      <c r="AV27" s="215"/>
-      <c r="AW27" s="215"/>
-      <c r="AX27" s="215"/>
-      <c r="AY27" s="215"/>
-      <c r="AZ27" s="215"/>
-      <c r="BA27" s="215"/>
-      <c r="BB27" s="215"/>
-      <c r="BC27" s="215"/>
-      <c r="BD27" s="215"/>
-      <c r="BE27" s="215"/>
-      <c r="BF27" s="215"/>
-      <c r="BG27" s="289"/>
+      <c r="N27" s="296"/>
+      <c r="O27" s="218"/>
+      <c r="P27" s="218"/>
+      <c r="Q27" s="218"/>
+      <c r="R27" s="218"/>
+      <c r="S27" s="218"/>
+      <c r="T27" s="218"/>
+      <c r="U27" s="218"/>
+      <c r="V27" s="218"/>
+      <c r="W27" s="218"/>
+      <c r="X27" s="218"/>
+      <c r="Y27" s="218"/>
+      <c r="Z27" s="218"/>
+      <c r="AA27" s="218"/>
+      <c r="AB27" s="218"/>
+      <c r="AC27" s="218"/>
+      <c r="AD27" s="218"/>
+      <c r="AE27" s="218"/>
+      <c r="AF27" s="218"/>
+      <c r="AG27" s="218"/>
+      <c r="AH27" s="218"/>
+      <c r="AI27" s="218"/>
+      <c r="AJ27" s="218"/>
+      <c r="AK27" s="218"/>
+      <c r="AL27" s="218"/>
+      <c r="AM27" s="218"/>
+      <c r="AN27" s="218"/>
+      <c r="AO27" s="218"/>
+      <c r="AP27" s="218"/>
+      <c r="AQ27" s="218"/>
+      <c r="AR27" s="218"/>
+      <c r="AS27" s="218"/>
+      <c r="AT27" s="218"/>
+      <c r="AU27" s="218"/>
+      <c r="AV27" s="218"/>
+      <c r="AW27" s="218"/>
+      <c r="AX27" s="218"/>
+      <c r="AY27" s="218"/>
+      <c r="AZ27" s="218"/>
+      <c r="BA27" s="218"/>
+      <c r="BB27" s="218"/>
+      <c r="BC27" s="218"/>
+      <c r="BD27" s="218"/>
+      <c r="BE27" s="218"/>
+      <c r="BF27" s="218"/>
+      <c r="BG27" s="297"/>
       <c r="BH27" s="39" t="s">
         <v>35</v>
       </c>
       <c r="BI27" s="40"/>
       <c r="BJ27" s="41"/>
-      <c r="BK27" s="293" t="s">
+      <c r="BK27" s="302" t="s">
         <v>60</v>
       </c>
-      <c r="BL27" s="293"/>
-      <c r="BM27" s="293"/>
-      <c r="BN27" s="293"/>
-      <c r="BO27" s="293"/>
-      <c r="BP27" s="293"/>
-      <c r="BQ27" s="293"/>
-      <c r="BR27" s="293"/>
-      <c r="BS27" s="293"/>
-      <c r="BT27" s="293"/>
-      <c r="BU27" s="293"/>
-      <c r="BV27" s="293"/>
-      <c r="BW27" s="293"/>
-      <c r="BX27" s="293"/>
-      <c r="BY27" s="293"/>
-      <c r="BZ27" s="293"/>
-      <c r="CA27" s="293"/>
-      <c r="CB27" s="293"/>
-      <c r="CC27" s="293"/>
-      <c r="CD27" s="294"/>
+      <c r="BL27" s="303"/>
+      <c r="BM27" s="303"/>
+      <c r="BN27" s="303"/>
+      <c r="BO27" s="303"/>
+      <c r="BP27" s="303"/>
+      <c r="BQ27" s="303"/>
+      <c r="BR27" s="303"/>
+      <c r="BS27" s="303"/>
+      <c r="BT27" s="303"/>
+      <c r="BU27" s="303"/>
+      <c r="BV27" s="303"/>
+      <c r="BW27" s="303"/>
+      <c r="BX27" s="303"/>
+      <c r="BY27" s="303"/>
+      <c r="BZ27" s="303"/>
+      <c r="CA27" s="303"/>
+      <c r="CB27" s="303"/>
+      <c r="CC27" s="303"/>
+      <c r="CD27" s="304"/>
       <c r="CE27" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:83" ht="22.5" customHeight="1">
-      <c r="A28" s="292"/>
-      <c r="B28" s="292"/>
-      <c r="C28" s="165"/>
-      <c r="D28" s="165"/>
+      <c r="A28" s="300"/>
+      <c r="B28" s="300"/>
+      <c r="C28" s="168"/>
+      <c r="D28" s="168"/>
       <c r="E28" s="92"/>
       <c r="F28" s="93"/>
       <c r="G28" s="94"/>
@@ -7339,75 +7468,75 @@
       <c r="K28" s="83"/>
       <c r="L28" s="83"/>
       <c r="M28" s="84"/>
-      <c r="N28" s="290"/>
-      <c r="O28" s="212"/>
-      <c r="P28" s="212"/>
-      <c r="Q28" s="212"/>
-      <c r="R28" s="212"/>
-      <c r="S28" s="212"/>
-      <c r="T28" s="212"/>
-      <c r="U28" s="212"/>
-      <c r="V28" s="212"/>
-      <c r="W28" s="212"/>
-      <c r="X28" s="212"/>
-      <c r="Y28" s="212"/>
-      <c r="Z28" s="212"/>
-      <c r="AA28" s="212"/>
-      <c r="AB28" s="212"/>
-      <c r="AC28" s="212"/>
-      <c r="AD28" s="212"/>
-      <c r="AE28" s="212"/>
-      <c r="AF28" s="212"/>
-      <c r="AG28" s="212"/>
-      <c r="AH28" s="212"/>
-      <c r="AI28" s="212"/>
-      <c r="AJ28" s="212"/>
-      <c r="AK28" s="212"/>
-      <c r="AL28" s="212"/>
-      <c r="AM28" s="212"/>
-      <c r="AN28" s="212"/>
-      <c r="AO28" s="212"/>
-      <c r="AP28" s="212"/>
-      <c r="AQ28" s="212"/>
-      <c r="AR28" s="212"/>
-      <c r="AS28" s="212"/>
-      <c r="AT28" s="212"/>
-      <c r="AU28" s="212"/>
-      <c r="AV28" s="212"/>
-      <c r="AW28" s="212"/>
-      <c r="AX28" s="212"/>
-      <c r="AY28" s="212"/>
-      <c r="AZ28" s="212"/>
-      <c r="BA28" s="212"/>
-      <c r="BB28" s="212"/>
-      <c r="BC28" s="212"/>
-      <c r="BD28" s="212"/>
-      <c r="BE28" s="212"/>
-      <c r="BF28" s="212"/>
-      <c r="BG28" s="291"/>
+      <c r="N28" s="298"/>
+      <c r="O28" s="215"/>
+      <c r="P28" s="215"/>
+      <c r="Q28" s="215"/>
+      <c r="R28" s="215"/>
+      <c r="S28" s="215"/>
+      <c r="T28" s="215"/>
+      <c r="U28" s="215"/>
+      <c r="V28" s="215"/>
+      <c r="W28" s="215"/>
+      <c r="X28" s="215"/>
+      <c r="Y28" s="215"/>
+      <c r="Z28" s="215"/>
+      <c r="AA28" s="215"/>
+      <c r="AB28" s="215"/>
+      <c r="AC28" s="215"/>
+      <c r="AD28" s="215"/>
+      <c r="AE28" s="215"/>
+      <c r="AF28" s="215"/>
+      <c r="AG28" s="215"/>
+      <c r="AH28" s="215"/>
+      <c r="AI28" s="215"/>
+      <c r="AJ28" s="215"/>
+      <c r="AK28" s="215"/>
+      <c r="AL28" s="215"/>
+      <c r="AM28" s="215"/>
+      <c r="AN28" s="215"/>
+      <c r="AO28" s="215"/>
+      <c r="AP28" s="215"/>
+      <c r="AQ28" s="215"/>
+      <c r="AR28" s="215"/>
+      <c r="AS28" s="215"/>
+      <c r="AT28" s="215"/>
+      <c r="AU28" s="215"/>
+      <c r="AV28" s="215"/>
+      <c r="AW28" s="215"/>
+      <c r="AX28" s="215"/>
+      <c r="AY28" s="215"/>
+      <c r="AZ28" s="215"/>
+      <c r="BA28" s="215"/>
+      <c r="BB28" s="215"/>
+      <c r="BC28" s="215"/>
+      <c r="BD28" s="215"/>
+      <c r="BE28" s="215"/>
+      <c r="BF28" s="215"/>
+      <c r="BG28" s="299"/>
       <c r="BH28" s="42"/>
       <c r="BI28" s="43"/>
       <c r="BJ28" s="44"/>
-      <c r="BK28" s="295"/>
-      <c r="BL28" s="295"/>
-      <c r="BM28" s="295"/>
-      <c r="BN28" s="295"/>
-      <c r="BO28" s="295"/>
-      <c r="BP28" s="295"/>
-      <c r="BQ28" s="295"/>
-      <c r="BR28" s="295"/>
-      <c r="BS28" s="295"/>
-      <c r="BT28" s="295"/>
-      <c r="BU28" s="295"/>
-      <c r="BV28" s="295"/>
-      <c r="BW28" s="295"/>
-      <c r="BX28" s="295"/>
-      <c r="BY28" s="295"/>
-      <c r="BZ28" s="295"/>
-      <c r="CA28" s="295"/>
-      <c r="CB28" s="295"/>
-      <c r="CC28" s="295"/>
-      <c r="CD28" s="296"/>
+      <c r="BK28" s="305"/>
+      <c r="BL28" s="306"/>
+      <c r="BM28" s="306"/>
+      <c r="BN28" s="306"/>
+      <c r="BO28" s="306"/>
+      <c r="BP28" s="306"/>
+      <c r="BQ28" s="306"/>
+      <c r="BR28" s="306"/>
+      <c r="BS28" s="306"/>
+      <c r="BT28" s="306"/>
+      <c r="BU28" s="306"/>
+      <c r="BV28" s="306"/>
+      <c r="BW28" s="306"/>
+      <c r="BX28" s="306"/>
+      <c r="BY28" s="306"/>
+      <c r="BZ28" s="306"/>
+      <c r="CA28" s="306"/>
+      <c r="CB28" s="306"/>
+      <c r="CC28" s="306"/>
+      <c r="CD28" s="307"/>
     </row>
     <row r="29" spans="1:83" ht="10.5" customHeight="1">
       <c r="A29" s="20"/>
@@ -7517,74 +7646,74 @@
       <c r="Z30"/>
       <c r="AA30"/>
       <c r="AB30"/>
-      <c r="BQ30" s="257" t="s">
+      <c r="BQ30" s="260" t="s">
         <v>45</v>
       </c>
-      <c r="BR30" s="258"/>
-      <c r="BS30" s="258"/>
-      <c r="BT30" s="258"/>
-      <c r="BU30" s="258"/>
-      <c r="BV30" s="258"/>
-      <c r="BW30" s="258"/>
-      <c r="BX30" s="258"/>
-      <c r="BY30" s="258"/>
-      <c r="BZ30" s="258"/>
-      <c r="CA30" s="258"/>
-      <c r="CB30" s="259"/>
+      <c r="BR30" s="261"/>
+      <c r="BS30" s="261"/>
+      <c r="BT30" s="261"/>
+      <c r="BU30" s="261"/>
+      <c r="BV30" s="261"/>
+      <c r="BW30" s="261"/>
+      <c r="BX30" s="261"/>
+      <c r="BY30" s="261"/>
+      <c r="BZ30" s="261"/>
+      <c r="CA30" s="261"/>
+      <c r="CB30" s="262"/>
     </row>
     <row r="31" spans="1:83" ht="15.75" customHeight="1">
       <c r="A31" s="20"/>
-      <c r="B31" s="278" t="s">
+      <c r="B31" s="286" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="279"/>
-      <c r="D31" s="279"/>
-      <c r="E31" s="279"/>
-      <c r="F31" s="279"/>
-      <c r="G31" s="279"/>
-      <c r="H31" s="279"/>
-      <c r="I31" s="279"/>
-      <c r="J31" s="279"/>
-      <c r="K31" s="279"/>
-      <c r="L31" s="279"/>
-      <c r="M31" s="279"/>
-      <c r="N31" s="279"/>
-      <c r="O31" s="279"/>
-      <c r="P31" s="279"/>
-      <c r="Q31" s="279"/>
-      <c r="R31" s="279"/>
-      <c r="S31" s="279"/>
-      <c r="T31" s="279"/>
-      <c r="U31" s="279"/>
-      <c r="V31" s="279"/>
-      <c r="W31" s="279"/>
-      <c r="X31" s="279"/>
-      <c r="Y31" s="279"/>
-      <c r="Z31" s="279"/>
-      <c r="AA31" s="279"/>
-      <c r="AB31" s="280"/>
-      <c r="AU31" s="297" t="s">
+      <c r="C31" s="287"/>
+      <c r="D31" s="287"/>
+      <c r="E31" s="287"/>
+      <c r="F31" s="287"/>
+      <c r="G31" s="287"/>
+      <c r="H31" s="287"/>
+      <c r="I31" s="287"/>
+      <c r="J31" s="287"/>
+      <c r="K31" s="287"/>
+      <c r="L31" s="287"/>
+      <c r="M31" s="287"/>
+      <c r="N31" s="287"/>
+      <c r="O31" s="287"/>
+      <c r="P31" s="287"/>
+      <c r="Q31" s="287"/>
+      <c r="R31" s="287"/>
+      <c r="S31" s="287"/>
+      <c r="T31" s="287"/>
+      <c r="U31" s="287"/>
+      <c r="V31" s="287"/>
+      <c r="W31" s="287"/>
+      <c r="X31" s="287"/>
+      <c r="Y31" s="287"/>
+      <c r="Z31" s="287"/>
+      <c r="AA31" s="287"/>
+      <c r="AB31" s="288"/>
+      <c r="AU31" s="301" t="s">
         <v>51</v>
       </c>
-      <c r="AV31" s="297"/>
-      <c r="AW31" s="297"/>
-      <c r="AX31" s="297"/>
-      <c r="AY31" s="297"/>
-      <c r="AZ31" s="297"/>
-      <c r="BA31" s="297"/>
-      <c r="BB31" s="297"/>
-      <c r="BC31" s="297"/>
-      <c r="BD31" s="297"/>
-      <c r="BE31" s="297"/>
-      <c r="BF31" s="297"/>
-      <c r="BG31" s="297"/>
-      <c r="BH31" s="297"/>
-      <c r="BI31" s="297"/>
-      <c r="BJ31" s="297"/>
-      <c r="BK31" s="297"/>
-      <c r="BL31" s="297"/>
-      <c r="BM31" s="297"/>
-      <c r="BN31" s="297"/>
+      <c r="AV31" s="301"/>
+      <c r="AW31" s="301"/>
+      <c r="AX31" s="301"/>
+      <c r="AY31" s="301"/>
+      <c r="AZ31" s="301"/>
+      <c r="BA31" s="301"/>
+      <c r="BB31" s="301"/>
+      <c r="BC31" s="301"/>
+      <c r="BD31" s="301"/>
+      <c r="BE31" s="301"/>
+      <c r="BF31" s="301"/>
+      <c r="BG31" s="301"/>
+      <c r="BH31" s="301"/>
+      <c r="BI31" s="301"/>
+      <c r="BJ31" s="301"/>
+      <c r="BK31" s="301"/>
+      <c r="BL31" s="301"/>
+      <c r="BM31" s="301"/>
+      <c r="BN31" s="301"/>
       <c r="BQ31" s="48"/>
       <c r="BR31" s="49"/>
       <c r="BS31" s="49"/>
@@ -7633,25 +7762,25 @@
       <c r="BF32" s="24"/>
       <c r="BI32" s="24"/>
       <c r="BJ32" s="24"/>
-      <c r="BQ32" s="266"/>
-      <c r="BR32" s="267"/>
-      <c r="BS32" s="267"/>
-      <c r="BT32" s="267"/>
-      <c r="BU32" s="267"/>
-      <c r="BV32" s="267"/>
-      <c r="BW32" s="267"/>
-      <c r="BX32" s="267"/>
-      <c r="BY32" s="267"/>
-      <c r="BZ32" s="267"/>
-      <c r="CA32" s="267"/>
-      <c r="CB32" s="268"/>
+      <c r="BQ32" s="269"/>
+      <c r="BR32" s="270"/>
+      <c r="BS32" s="270"/>
+      <c r="BT32" s="270"/>
+      <c r="BU32" s="270"/>
+      <c r="BV32" s="270"/>
+      <c r="BW32" s="270"/>
+      <c r="BX32" s="270"/>
+      <c r="BY32" s="270"/>
+      <c r="BZ32" s="270"/>
+      <c r="CA32" s="270"/>
+      <c r="CB32" s="271"/>
     </row>
     <row r="33" spans="1:81" ht="21" customHeight="1">
       <c r="A33" s="20"/>
-      <c r="B33" s="302" t="s">
+      <c r="B33" s="272" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="299"/>
+      <c r="C33" s="273"/>
       <c r="D33" s="29" t="s">
         <v>9</v>
       </c>
@@ -7661,24 +7790,24 @@
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
-      <c r="K33" s="271"/>
-      <c r="L33" s="271"/>
-      <c r="M33" s="271"/>
-      <c r="N33" s="271"/>
-      <c r="O33" s="271"/>
-      <c r="P33" s="271"/>
-      <c r="Q33" s="271"/>
-      <c r="R33" s="271"/>
-      <c r="S33" s="271"/>
-      <c r="T33" s="271"/>
-      <c r="U33" s="271"/>
-      <c r="V33" s="271"/>
-      <c r="W33" s="271"/>
-      <c r="X33" s="271"/>
-      <c r="Y33" s="271"/>
-      <c r="Z33" s="271"/>
-      <c r="AA33" s="271"/>
-      <c r="AB33" s="272"/>
+      <c r="K33" s="279"/>
+      <c r="L33" s="279"/>
+      <c r="M33" s="279"/>
+      <c r="N33" s="279"/>
+      <c r="O33" s="279"/>
+      <c r="P33" s="279"/>
+      <c r="Q33" s="279"/>
+      <c r="R33" s="279"/>
+      <c r="S33" s="279"/>
+      <c r="T33" s="279"/>
+      <c r="U33" s="279"/>
+      <c r="V33" s="279"/>
+      <c r="W33" s="279"/>
+      <c r="X33" s="279"/>
+      <c r="Y33" s="279"/>
+      <c r="Z33" s="279"/>
+      <c r="AA33" s="279"/>
+      <c r="AB33" s="280"/>
       <c r="AG33" s="58"/>
       <c r="AH33" s="58"/>
       <c r="AI33" s="9"/>
@@ -7709,23 +7838,23 @@
       <c r="BH33" s="2"/>
       <c r="BI33" s="2"/>
       <c r="BJ33" s="2"/>
-      <c r="BQ33" s="266"/>
-      <c r="BR33" s="267"/>
-      <c r="BS33" s="267"/>
-      <c r="BT33" s="267"/>
-      <c r="BU33" s="267"/>
-      <c r="BV33" s="267"/>
-      <c r="BW33" s="267"/>
-      <c r="BX33" s="267"/>
-      <c r="BY33" s="267"/>
-      <c r="BZ33" s="267"/>
-      <c r="CA33" s="267"/>
-      <c r="CB33" s="268"/>
+      <c r="BQ33" s="269"/>
+      <c r="BR33" s="270"/>
+      <c r="BS33" s="270"/>
+      <c r="BT33" s="270"/>
+      <c r="BU33" s="270"/>
+      <c r="BV33" s="270"/>
+      <c r="BW33" s="270"/>
+      <c r="BX33" s="270"/>
+      <c r="BY33" s="270"/>
+      <c r="BZ33" s="270"/>
+      <c r="CA33" s="270"/>
+      <c r="CB33" s="271"/>
     </row>
     <row r="34" spans="1:81" ht="21" customHeight="1">
       <c r="A34" s="20"/>
-      <c r="B34" s="298"/>
-      <c r="C34" s="299"/>
+      <c r="B34" s="274"/>
+      <c r="C34" s="273"/>
       <c r="D34" s="29" t="s">
         <v>8</v>
       </c>
@@ -7735,24 +7864,24 @@
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
-      <c r="K34" s="271"/>
-      <c r="L34" s="271"/>
-      <c r="M34" s="271"/>
-      <c r="N34" s="271"/>
-      <c r="O34" s="271"/>
-      <c r="P34" s="271"/>
-      <c r="Q34" s="271"/>
-      <c r="R34" s="271"/>
-      <c r="S34" s="271"/>
-      <c r="T34" s="271"/>
-      <c r="U34" s="271"/>
-      <c r="V34" s="271"/>
-      <c r="W34" s="271"/>
-      <c r="X34" s="271"/>
-      <c r="Y34" s="271"/>
-      <c r="Z34" s="271"/>
-      <c r="AA34" s="271"/>
-      <c r="AB34" s="272"/>
+      <c r="K34" s="279"/>
+      <c r="L34" s="279"/>
+      <c r="M34" s="279"/>
+      <c r="N34" s="279"/>
+      <c r="O34" s="279"/>
+      <c r="P34" s="279"/>
+      <c r="Q34" s="279"/>
+      <c r="R34" s="279"/>
+      <c r="S34" s="279"/>
+      <c r="T34" s="279"/>
+      <c r="U34" s="279"/>
+      <c r="V34" s="279"/>
+      <c r="W34" s="279"/>
+      <c r="X34" s="279"/>
+      <c r="Y34" s="279"/>
+      <c r="Z34" s="279"/>
+      <c r="AA34" s="279"/>
+      <c r="AB34" s="280"/>
       <c r="AG34" s="58"/>
       <c r="AH34" s="58"/>
       <c r="AI34" s="48"/>
@@ -7783,23 +7912,23 @@
       <c r="BH34" s="9"/>
       <c r="BI34" s="9"/>
       <c r="BJ34" s="9"/>
-      <c r="BQ34" s="266"/>
-      <c r="BR34" s="267"/>
-      <c r="BS34" s="267"/>
-      <c r="BT34" s="267"/>
-      <c r="BU34" s="267"/>
-      <c r="BV34" s="267"/>
-      <c r="BW34" s="267"/>
-      <c r="BX34" s="267"/>
-      <c r="BY34" s="267"/>
-      <c r="BZ34" s="267"/>
-      <c r="CA34" s="267"/>
-      <c r="CB34" s="268"/>
+      <c r="BQ34" s="269"/>
+      <c r="BR34" s="270"/>
+      <c r="BS34" s="270"/>
+      <c r="BT34" s="270"/>
+      <c r="BU34" s="270"/>
+      <c r="BV34" s="270"/>
+      <c r="BW34" s="270"/>
+      <c r="BX34" s="270"/>
+      <c r="BY34" s="270"/>
+      <c r="BZ34" s="270"/>
+      <c r="CA34" s="270"/>
+      <c r="CB34" s="271"/>
     </row>
     <row r="35" spans="1:81" ht="21" customHeight="1">
       <c r="A35" s="20"/>
-      <c r="B35" s="298"/>
-      <c r="C35" s="299"/>
+      <c r="B35" s="274"/>
+      <c r="C35" s="273"/>
       <c r="D35" s="29" t="s">
         <v>10</v>
       </c>
@@ -7809,22 +7938,22 @@
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
-      <c r="K35" s="271"/>
-      <c r="L35" s="271"/>
-      <c r="M35" s="271"/>
-      <c r="N35" s="271"/>
-      <c r="O35" s="271"/>
-      <c r="P35" s="271"/>
-      <c r="Q35" s="271"/>
-      <c r="R35" s="271"/>
-      <c r="S35" s="271"/>
-      <c r="T35" s="271"/>
-      <c r="U35" s="271"/>
-      <c r="V35" s="271"/>
-      <c r="W35" s="271"/>
-      <c r="X35" s="271"/>
-      <c r="Y35" s="271"/>
-      <c r="Z35" s="271"/>
+      <c r="K35" s="279"/>
+      <c r="L35" s="279"/>
+      <c r="M35" s="279"/>
+      <c r="N35" s="279"/>
+      <c r="O35" s="279"/>
+      <c r="P35" s="279"/>
+      <c r="Q35" s="279"/>
+      <c r="R35" s="279"/>
+      <c r="S35" s="279"/>
+      <c r="T35" s="279"/>
+      <c r="U35" s="279"/>
+      <c r="V35" s="279"/>
+      <c r="W35" s="279"/>
+      <c r="X35" s="279"/>
+      <c r="Y35" s="279"/>
+      <c r="Z35" s="279"/>
       <c r="AA35" s="35" t="s">
         <v>7</v>
       </c>
@@ -7854,7 +7983,7 @@
       <c r="BC35" s="60"/>
       <c r="BD35" s="60"/>
       <c r="BE35" s="60"/>
-      <c r="BF35" s="258" t="s">
+      <c r="BF35" s="261" t="s">
         <v>7</v>
       </c>
       <c r="BG35" s="36"/>
@@ -7865,50 +7994,50 @@
       <c r="BN35"/>
       <c r="BO35"/>
       <c r="BP35"/>
-      <c r="BQ35" s="266"/>
-      <c r="BR35" s="267"/>
-      <c r="BS35" s="267"/>
-      <c r="BT35" s="267"/>
-      <c r="BU35" s="267"/>
-      <c r="BV35" s="267"/>
-      <c r="BW35" s="267"/>
-      <c r="BX35" s="267"/>
-      <c r="BY35" s="267"/>
-      <c r="BZ35" s="267"/>
-      <c r="CA35" s="267"/>
-      <c r="CB35" s="268"/>
+      <c r="BQ35" s="269"/>
+      <c r="BR35" s="270"/>
+      <c r="BS35" s="270"/>
+      <c r="BT35" s="270"/>
+      <c r="BU35" s="270"/>
+      <c r="BV35" s="270"/>
+      <c r="BW35" s="270"/>
+      <c r="BX35" s="270"/>
+      <c r="BY35" s="270"/>
+      <c r="BZ35" s="270"/>
+      <c r="CA35" s="270"/>
+      <c r="CB35" s="271"/>
     </row>
     <row r="36" spans="1:81" ht="12.75" customHeight="1">
       <c r="A36" s="20"/>
-      <c r="B36" s="298"/>
-      <c r="C36" s="299"/>
-      <c r="D36" s="269" t="s">
+      <c r="B36" s="274"/>
+      <c r="C36" s="273"/>
+      <c r="D36" s="277" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="269"/>
-      <c r="F36" s="269"/>
-      <c r="G36" s="269"/>
-      <c r="H36" s="269"/>
-      <c r="I36" s="269"/>
-      <c r="J36" s="269"/>
-      <c r="K36" s="271"/>
-      <c r="L36" s="271"/>
-      <c r="M36" s="271"/>
-      <c r="N36" s="271"/>
-      <c r="O36" s="271"/>
-      <c r="P36" s="271"/>
-      <c r="Q36" s="271"/>
-      <c r="R36" s="271"/>
-      <c r="S36" s="271"/>
-      <c r="T36" s="271"/>
-      <c r="U36" s="271"/>
-      <c r="V36" s="271"/>
-      <c r="W36" s="271"/>
-      <c r="X36" s="271"/>
-      <c r="Y36" s="271"/>
-      <c r="Z36" s="271"/>
-      <c r="AA36" s="271"/>
-      <c r="AB36" s="272"/>
+      <c r="E36" s="277"/>
+      <c r="F36" s="277"/>
+      <c r="G36" s="277"/>
+      <c r="H36" s="277"/>
+      <c r="I36" s="277"/>
+      <c r="J36" s="277"/>
+      <c r="K36" s="279"/>
+      <c r="L36" s="279"/>
+      <c r="M36" s="279"/>
+      <c r="N36" s="279"/>
+      <c r="O36" s="279"/>
+      <c r="P36" s="279"/>
+      <c r="Q36" s="279"/>
+      <c r="R36" s="279"/>
+      <c r="S36" s="279"/>
+      <c r="T36" s="279"/>
+      <c r="U36" s="279"/>
+      <c r="V36" s="279"/>
+      <c r="W36" s="279"/>
+      <c r="X36" s="279"/>
+      <c r="Y36" s="279"/>
+      <c r="Z36" s="279"/>
+      <c r="AA36" s="279"/>
+      <c r="AB36" s="280"/>
       <c r="AG36" s="58"/>
       <c r="AH36" s="58"/>
       <c r="AI36" s="61"/>
@@ -7934,7 +8063,7 @@
       <c r="BC36" s="62"/>
       <c r="BD36" s="62"/>
       <c r="BE36" s="62"/>
-      <c r="BF36" s="281"/>
+      <c r="BF36" s="289"/>
       <c r="BG36" s="9"/>
       <c r="BH36" s="9"/>
       <c r="BI36" s="38"/>
@@ -7942,30 +8071,30 @@
       <c r="BN36"/>
       <c r="BO36"/>
       <c r="BP36"/>
-      <c r="BQ36" s="266"/>
-      <c r="BR36" s="267"/>
-      <c r="BS36" s="267"/>
-      <c r="BT36" s="267"/>
-      <c r="BU36" s="267"/>
-      <c r="BV36" s="267"/>
-      <c r="BW36" s="267"/>
-      <c r="BX36" s="267"/>
-      <c r="BY36" s="267"/>
-      <c r="BZ36" s="267"/>
-      <c r="CA36" s="267"/>
-      <c r="CB36" s="268"/>
+      <c r="BQ36" s="269"/>
+      <c r="BR36" s="270"/>
+      <c r="BS36" s="270"/>
+      <c r="BT36" s="270"/>
+      <c r="BU36" s="270"/>
+      <c r="BV36" s="270"/>
+      <c r="BW36" s="270"/>
+      <c r="BX36" s="270"/>
+      <c r="BY36" s="270"/>
+      <c r="BZ36" s="270"/>
+      <c r="CA36" s="270"/>
+      <c r="CB36" s="271"/>
     </row>
     <row r="37" spans="1:81" ht="12.75" customHeight="1">
       <c r="A37"/>
-      <c r="B37" s="300"/>
-      <c r="C37" s="301"/>
-      <c r="D37" s="270"/>
-      <c r="E37" s="270"/>
-      <c r="F37" s="270"/>
-      <c r="G37" s="270"/>
-      <c r="H37" s="270"/>
-      <c r="I37" s="270"/>
-      <c r="J37" s="270"/>
+      <c r="B37" s="275"/>
+      <c r="C37" s="276"/>
+      <c r="D37" s="278"/>
+      <c r="E37" s="278"/>
+      <c r="F37" s="278"/>
+      <c r="G37" s="278"/>
+      <c r="H37" s="278"/>
+      <c r="I37" s="278"/>
+      <c r="J37" s="278"/>
       <c r="K37" s="79"/>
       <c r="L37" s="79"/>
       <c r="M37" s="79"/>
@@ -7983,7 +8112,7 @@
       <c r="Y37" s="79"/>
       <c r="Z37" s="79"/>
       <c r="AA37" s="79"/>
-      <c r="AB37" s="273"/>
+      <c r="AB37" s="281"/>
       <c r="AC37"/>
       <c r="AD37"/>
       <c r="AE37"/>
@@ -8013,7 +8142,7 @@
       <c r="BC37" s="64"/>
       <c r="BD37" s="64"/>
       <c r="BE37" s="64"/>
-      <c r="BF37" s="282"/>
+      <c r="BF37" s="290"/>
       <c r="BG37" s="26"/>
       <c r="BH37" s="26"/>
       <c r="BI37" s="27"/>
@@ -8024,18 +8153,18 @@
       <c r="BN37"/>
       <c r="BO37"/>
       <c r="BP37"/>
-      <c r="BQ37" s="185"/>
-      <c r="BR37" s="186"/>
-      <c r="BS37" s="186"/>
-      <c r="BT37" s="186"/>
-      <c r="BU37" s="186"/>
-      <c r="BV37" s="186"/>
-      <c r="BW37" s="186"/>
-      <c r="BX37" s="186"/>
-      <c r="BY37" s="186"/>
-      <c r="BZ37" s="186"/>
-      <c r="CA37" s="186"/>
-      <c r="CB37" s="187"/>
+      <c r="BQ37" s="188"/>
+      <c r="BR37" s="189"/>
+      <c r="BS37" s="189"/>
+      <c r="BT37" s="189"/>
+      <c r="BU37" s="189"/>
+      <c r="BV37" s="189"/>
+      <c r="BW37" s="189"/>
+      <c r="BX37" s="189"/>
+      <c r="BY37" s="189"/>
+      <c r="BZ37" s="189"/>
+      <c r="CA37" s="189"/>
+      <c r="CB37" s="190"/>
       <c r="CC37"/>
     </row>
     <row r="38" spans="1:81" ht="17.25" customHeight="1">
@@ -11140,20 +11269,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId8" name="221">
+            <control shapeId="1038" r:id="rId8" name="333">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>61</xdr:col>
-                    <xdr:colOff>95250</xdr:colOff>
-                    <xdr:row>26</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>64</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>27</xdr:row>
-                    <xdr:rowOff>76200</xdr:rowOff>
+                    <xdr:col>13</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>190500</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11162,7 +11291,29 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId9" name="223">
+            <control shapeId="1039" r:id="rId9" name="221">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>61</xdr:col>
+                    <xdr:colOff>95250</xdr:colOff>
+                    <xdr:row>26</xdr:row>
+                    <xdr:rowOff>57150</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>64</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>27</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1040" r:id="rId10" name="223">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -11184,20 +11335,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId10" name="222">
+            <control shapeId="1041" r:id="rId11" name="222">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>67</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>114300</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>85725</xdr:rowOff>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>70</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>57150</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>95250</xdr:rowOff>
+                    <xdr:rowOff>57150</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11206,42 +11357,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId11" name="224">
+            <control shapeId="1042" r:id="rId12" name="224">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>67</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>114300</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>70</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:colOff>57150</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>228600</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId12" name="333">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>10</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
-                    <xdr:row>17</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>13</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:rowOff>219075</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
[QSI014 - QUI001] Fix bug
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者住所変更届.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/被保険者住所変更届.xlsx
@@ -100,9 +100,10 @@
     <definedName name="B2_2_3">被保険者住所変更届（一枚目）!$R$7</definedName>
     <definedName name="B2_2_4">被保険者住所変更届（一枚目）!$T$7</definedName>
     <definedName name="B2_3">被保険者住所変更届（一枚目）!$V$7</definedName>
+    <definedName name="HIHI">被保険者住所変更届（一枚目）!$J$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">被保険者住所変更届（一枚目）!$A$1:$CJ$37</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -648,7 +649,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20">
     <font>
       <sz val="11"/>
@@ -2044,6 +2045,411 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2053,377 +2459,71 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -2443,75 +2543,111 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="255"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2524,56 +2660,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2601,96 +2692,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2765,7 +2766,7 @@
         <xdr:cNvPr id="4098" name="AutoShape 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002100000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002100000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2835,7 +2836,7 @@
         <xdr:cNvPr id="4099" name="AutoShape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003100000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003100000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2905,7 +2906,7 @@
         <xdr:cNvPr id="10" name="正方形/長方形 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2980,7 +2981,7 @@
         <xdr:cNvPr id="1027" name="AutoShape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3028,7 +3029,7 @@
         <xdr:cNvPr id="12" name="図 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3084,7 +3085,7 @@
         <xdr:cNvPr id="3" name="テキスト ボックス 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3157,7 +3158,7 @@
         <xdr:cNvPr id="11" name="正方形/長方形 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3237,7 +3238,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3304,7 +3305,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3371,7 +3372,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3438,7 +3439,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3505,7 +3506,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3567,7 +3568,7 @@
         <xdr:cNvPr id="22" name="A2_3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3633,7 +3634,7 @@
         <xdr:cNvPr id="23" name="A2_4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3699,7 +3700,7 @@
         <xdr:cNvPr id="24" name="A2_41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3765,7 +3766,7 @@
         <xdr:cNvPr id="26" name="A1_51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3831,7 +3832,7 @@
         <xdr:cNvPr id="27" name="A1_52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3897,7 +3898,7 @@
         <xdr:cNvPr id="28" name="A1_53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3963,7 +3964,7 @@
         <xdr:cNvPr id="29" name="A4_111">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4028,7 +4029,7 @@
         <xdr:cNvPr id="30" name="A4_113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4093,7 +4094,7 @@
         <xdr:cNvPr id="31" name="A4_112">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4158,7 +4159,7 @@
         <xdr:cNvPr id="32" name="A4_114">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4223,7 +4224,7 @@
         <xdr:cNvPr id="37" name="A4_1111">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4288,7 +4289,7 @@
         <xdr:cNvPr id="41" name="A2_19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4350,7 +4351,7 @@
         <xdr:cNvPr id="38" name="Picture 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E92B99-4293-4E41-A824-FAD99FACFBA0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E92B99-4293-4E41-A824-FAD99FACFBA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4399,7 +4400,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4466,7 +4467,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4533,7 +4534,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4600,7 +4601,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4662,7 +4663,7 @@
         <xdr:cNvPr id="43" name="A4_221">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4727,7 +4728,7 @@
         <xdr:cNvPr id="44" name="A4_222">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4792,7 +4793,7 @@
         <xdr:cNvPr id="45" name="A4_223">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4857,7 +4858,7 @@
         <xdr:cNvPr id="46" name="A4_224">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5109,7 +5110,7 @@
         <xdr:cNvPr id="50" name="A1_15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5174,7 +5175,7 @@
         <xdr:cNvPr id="51" name="A2_19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5239,7 +5240,7 @@
         <xdr:cNvPr id="54" name="A2_19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000055000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6063,7 +6064,7 @@
   <dimension ref="B1:CJ76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="BG7" sqref="BG7:BN7"/>
+      <selection activeCell="J7" sqref="J7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="17.25" customHeight="1"/>
@@ -6085,12 +6086,12 @@
   <sheetData>
     <row r="1" spans="6:86" ht="26.25" customHeight="1"/>
     <row r="2" spans="6:86" ht="20.25" customHeight="1">
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="146"/>
-      <c r="K2" s="146"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="149"/>
       <c r="L2" s="158"/>
       <c r="M2" s="158"/>
       <c r="BN2" s="189" t="s">
@@ -6124,12 +6125,12 @@
       <c r="CH2" s="184"/>
     </row>
     <row r="3" spans="6:86" ht="18" customHeight="1">
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="146"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="149"/>
+      <c r="K3" s="149"/>
       <c r="L3" s="158"/>
       <c r="M3" s="158"/>
       <c r="AB3" s="195" t="s">
@@ -6174,27 +6175,27 @@
       <c r="BK3" s="6"/>
       <c r="BL3" s="6"/>
       <c r="BM3" s="7"/>
-      <c r="BN3" s="147"/>
-      <c r="BO3" s="148"/>
-      <c r="BP3" s="148"/>
-      <c r="BQ3" s="148"/>
-      <c r="BR3" s="149"/>
-      <c r="BS3" s="147"/>
-      <c r="BT3" s="148"/>
-      <c r="BU3" s="148"/>
-      <c r="BV3" s="148"/>
-      <c r="BW3" s="148"/>
-      <c r="BX3" s="149"/>
-      <c r="BY3" s="147"/>
-      <c r="BZ3" s="148"/>
-      <c r="CA3" s="148"/>
-      <c r="CB3" s="148"/>
-      <c r="CC3" s="149"/>
-      <c r="CD3" s="147"/>
-      <c r="CE3" s="148"/>
-      <c r="CF3" s="148"/>
-      <c r="CG3" s="148"/>
-      <c r="CH3" s="149"/>
+      <c r="BN3" s="150"/>
+      <c r="BO3" s="151"/>
+      <c r="BP3" s="151"/>
+      <c r="BQ3" s="151"/>
+      <c r="BR3" s="152"/>
+      <c r="BS3" s="150"/>
+      <c r="BT3" s="151"/>
+      <c r="BU3" s="151"/>
+      <c r="BV3" s="151"/>
+      <c r="BW3" s="151"/>
+      <c r="BX3" s="152"/>
+      <c r="BY3" s="150"/>
+      <c r="BZ3" s="151"/>
+      <c r="CA3" s="151"/>
+      <c r="CB3" s="151"/>
+      <c r="CC3" s="152"/>
+      <c r="CD3" s="150"/>
+      <c r="CE3" s="151"/>
+      <c r="CF3" s="151"/>
+      <c r="CG3" s="151"/>
+      <c r="CH3" s="152"/>
     </row>
     <row r="4" spans="6:86" ht="18" customHeight="1">
       <c r="AB4" s="195" t="s">
@@ -6261,8 +6262,8 @@
     </row>
     <row r="5" spans="6:86" ht="9" customHeight="1"/>
     <row r="6" spans="6:86" ht="24" customHeight="1">
-      <c r="F6" s="296"/>
-      <c r="G6" s="296"/>
+      <c r="F6" s="280"/>
+      <c r="G6" s="280"/>
       <c r="H6" s="166"/>
       <c r="I6" s="166"/>
       <c r="J6" s="161" t="s">
@@ -6279,83 +6280,83 @@
       <c r="S6" s="161"/>
       <c r="T6" s="161"/>
       <c r="U6" s="161"/>
-      <c r="V6" s="98" t="s">
+      <c r="V6" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="W6" s="99"/>
-      <c r="X6" s="99"/>
-      <c r="Y6" s="99"/>
-      <c r="Z6" s="99"/>
-      <c r="AA6" s="104" t="s">
+      <c r="W6" s="98"/>
+      <c r="X6" s="98"/>
+      <c r="Y6" s="98"/>
+      <c r="Z6" s="98"/>
+      <c r="AA6" s="103" t="s">
         <v>51</v>
       </c>
-      <c r="AB6" s="105"/>
-      <c r="AC6" s="105"/>
-      <c r="AD6" s="105"/>
-      <c r="AE6" s="105"/>
-      <c r="AF6" s="105"/>
-      <c r="AG6" s="105"/>
-      <c r="AH6" s="105"/>
-      <c r="AI6" s="105"/>
-      <c r="AJ6" s="105"/>
-      <c r="AK6" s="105"/>
-      <c r="AL6" s="105"/>
-      <c r="AM6" s="105"/>
-      <c r="AN6" s="105"/>
-      <c r="AO6" s="105"/>
-      <c r="AP6" s="105"/>
-      <c r="AQ6" s="105"/>
-      <c r="AR6" s="105"/>
-      <c r="AS6" s="105"/>
-      <c r="AT6" s="105"/>
-      <c r="AU6" s="105"/>
-      <c r="AV6" s="105"/>
-      <c r="AW6" s="105"/>
-      <c r="AX6" s="106"/>
-      <c r="AY6" s="105" t="s">
+      <c r="AB6" s="104"/>
+      <c r="AC6" s="104"/>
+      <c r="AD6" s="104"/>
+      <c r="AE6" s="104"/>
+      <c r="AF6" s="104"/>
+      <c r="AG6" s="104"/>
+      <c r="AH6" s="104"/>
+      <c r="AI6" s="104"/>
+      <c r="AJ6" s="104"/>
+      <c r="AK6" s="104"/>
+      <c r="AL6" s="104"/>
+      <c r="AM6" s="104"/>
+      <c r="AN6" s="104"/>
+      <c r="AO6" s="104"/>
+      <c r="AP6" s="104"/>
+      <c r="AQ6" s="104"/>
+      <c r="AR6" s="104"/>
+      <c r="AS6" s="104"/>
+      <c r="AT6" s="104"/>
+      <c r="AU6" s="104"/>
+      <c r="AV6" s="104"/>
+      <c r="AW6" s="104"/>
+      <c r="AX6" s="105"/>
+      <c r="AY6" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="AZ6" s="105"/>
-      <c r="BA6" s="105"/>
-      <c r="BB6" s="105"/>
-      <c r="BC6" s="105"/>
-      <c r="BD6" s="105"/>
-      <c r="BE6" s="105"/>
-      <c r="BF6" s="105"/>
-      <c r="BG6" s="105"/>
-      <c r="BH6" s="105"/>
-      <c r="BI6" s="105"/>
-      <c r="BJ6" s="105"/>
-      <c r="BK6" s="105"/>
-      <c r="BL6" s="105"/>
-      <c r="BM6" s="105"/>
-      <c r="BN6" s="106"/>
-      <c r="BO6" s="147" t="s">
+      <c r="AZ6" s="104"/>
+      <c r="BA6" s="104"/>
+      <c r="BB6" s="104"/>
+      <c r="BC6" s="104"/>
+      <c r="BD6" s="104"/>
+      <c r="BE6" s="104"/>
+      <c r="BF6" s="104"/>
+      <c r="BG6" s="104"/>
+      <c r="BH6" s="104"/>
+      <c r="BI6" s="104"/>
+      <c r="BJ6" s="104"/>
+      <c r="BK6" s="104"/>
+      <c r="BL6" s="104"/>
+      <c r="BM6" s="104"/>
+      <c r="BN6" s="105"/>
+      <c r="BO6" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="BP6" s="148"/>
-      <c r="BQ6" s="148"/>
-      <c r="BR6" s="148"/>
-      <c r="BS6" s="148"/>
-      <c r="BT6" s="148"/>
-      <c r="BU6" s="148"/>
-      <c r="BV6" s="148"/>
-      <c r="BW6" s="148"/>
-      <c r="BX6" s="148"/>
-      <c r="BY6" s="148"/>
-      <c r="BZ6" s="148"/>
-      <c r="CA6" s="148"/>
-      <c r="CB6" s="148"/>
-      <c r="CC6" s="148"/>
-      <c r="CD6" s="148"/>
-      <c r="CE6" s="149"/>
-      <c r="CF6" s="198"/>
-      <c r="CG6" s="199"/>
+      <c r="BP6" s="151"/>
+      <c r="BQ6" s="151"/>
+      <c r="BR6" s="151"/>
+      <c r="BS6" s="151"/>
+      <c r="BT6" s="151"/>
+      <c r="BU6" s="151"/>
+      <c r="BV6" s="151"/>
+      <c r="BW6" s="151"/>
+      <c r="BX6" s="151"/>
+      <c r="BY6" s="151"/>
+      <c r="BZ6" s="151"/>
+      <c r="CA6" s="151"/>
+      <c r="CB6" s="151"/>
+      <c r="CC6" s="151"/>
+      <c r="CD6" s="151"/>
+      <c r="CE6" s="152"/>
+      <c r="CF6" s="197"/>
+      <c r="CG6" s="198"/>
       <c r="CH6" s="10"/>
     </row>
     <row r="7" spans="6:86" ht="15.75" customHeight="1">
-      <c r="F7" s="296"/>
-      <c r="G7" s="296"/>
+      <c r="F7" s="280"/>
+      <c r="G7" s="280"/>
       <c r="H7" s="166"/>
       <c r="I7" s="166"/>
       <c r="J7" s="159"/>
@@ -6363,21 +6364,21 @@
       <c r="L7" s="159"/>
       <c r="M7" s="160"/>
       <c r="N7" s="163"/>
-      <c r="O7" s="143"/>
-      <c r="P7" s="143"/>
-      <c r="Q7" s="143"/>
-      <c r="R7" s="143"/>
-      <c r="S7" s="143"/>
-      <c r="T7" s="143"/>
+      <c r="O7" s="142"/>
+      <c r="P7" s="142"/>
+      <c r="Q7" s="142"/>
+      <c r="R7" s="142"/>
+      <c r="S7" s="142"/>
+      <c r="T7" s="142"/>
       <c r="U7" s="162"/>
       <c r="V7" s="178"/>
       <c r="W7" s="179"/>
       <c r="X7" s="179"/>
       <c r="Y7" s="179"/>
       <c r="Z7" s="179"/>
-      <c r="AA7" s="100"/>
-      <c r="AB7" s="101"/>
-      <c r="AC7" s="156"/>
+      <c r="AA7" s="99"/>
+      <c r="AB7" s="100"/>
+      <c r="AC7" s="147"/>
       <c r="AD7" s="47"/>
       <c r="AE7" s="47"/>
       <c r="AF7" s="47"/>
@@ -6385,64 +6386,64 @@
       <c r="AH7" s="74"/>
       <c r="AI7" s="193"/>
       <c r="AJ7" s="69"/>
-      <c r="AK7" s="200"/>
+      <c r="AK7" s="199"/>
       <c r="AL7" s="69"/>
       <c r="AM7" s="47"/>
       <c r="AN7" s="47"/>
       <c r="AO7" s="47"/>
       <c r="AP7" s="74"/>
-      <c r="AQ7" s="156"/>
+      <c r="AQ7" s="147"/>
       <c r="AR7" s="47"/>
       <c r="AS7" s="47"/>
       <c r="AT7" s="47"/>
       <c r="AU7" s="47"/>
       <c r="AV7" s="47"/>
-      <c r="AW7" s="137"/>
-      <c r="AX7" s="138"/>
-      <c r="AY7" s="141" t="s">
+      <c r="AW7" s="136"/>
+      <c r="AX7" s="137"/>
+      <c r="AY7" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="AZ7" s="142"/>
-      <c r="BA7" s="123"/>
-      <c r="BB7" s="123"/>
-      <c r="BC7" s="123"/>
-      <c r="BD7" s="123"/>
-      <c r="BE7" s="123"/>
-      <c r="BF7" s="197"/>
+      <c r="AZ7" s="141"/>
+      <c r="BA7" s="122"/>
+      <c r="BB7" s="122"/>
+      <c r="BC7" s="122"/>
+      <c r="BD7" s="122"/>
+      <c r="BE7" s="122"/>
+      <c r="BF7" s="148"/>
       <c r="BG7" s="196"/>
-      <c r="BH7" s="123"/>
-      <c r="BI7" s="123"/>
-      <c r="BJ7" s="123"/>
-      <c r="BK7" s="123"/>
-      <c r="BL7" s="123"/>
-      <c r="BM7" s="123"/>
-      <c r="BN7" s="197"/>
-      <c r="BO7" s="124" t="s">
+      <c r="BH7" s="122"/>
+      <c r="BI7" s="122"/>
+      <c r="BJ7" s="122"/>
+      <c r="BK7" s="122"/>
+      <c r="BL7" s="122"/>
+      <c r="BM7" s="122"/>
+      <c r="BN7" s="148"/>
+      <c r="BO7" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="BP7" s="125"/>
-      <c r="BQ7" s="125"/>
-      <c r="BR7" s="126"/>
-      <c r="BS7" s="110"/>
-      <c r="BT7" s="155"/>
-      <c r="BU7" s="154"/>
-      <c r="BV7" s="150"/>
-      <c r="BW7" s="151"/>
-      <c r="BX7" s="155"/>
-      <c r="BY7" s="154"/>
-      <c r="BZ7" s="154"/>
-      <c r="CA7" s="95"/>
-      <c r="CB7" s="155"/>
-      <c r="CC7" s="154"/>
-      <c r="CD7" s="154"/>
+      <c r="BP7" s="124"/>
+      <c r="BQ7" s="124"/>
+      <c r="BR7" s="125"/>
+      <c r="BS7" s="109"/>
+      <c r="BT7" s="145"/>
+      <c r="BU7" s="146"/>
+      <c r="BV7" s="153"/>
+      <c r="BW7" s="154"/>
+      <c r="BX7" s="145"/>
+      <c r="BY7" s="146"/>
+      <c r="BZ7" s="146"/>
+      <c r="CA7" s="92"/>
+      <c r="CB7" s="145"/>
+      <c r="CC7" s="146"/>
+      <c r="CD7" s="146"/>
       <c r="CE7" s="157"/>
-      <c r="CF7" s="198"/>
-      <c r="CG7" s="199"/>
+      <c r="CF7" s="197"/>
+      <c r="CG7" s="198"/>
       <c r="CH7" s="10"/>
     </row>
     <row r="8" spans="6:86" ht="21.75" customHeight="1">
-      <c r="F8" s="296"/>
-      <c r="G8" s="296"/>
+      <c r="F8" s="280"/>
+      <c r="G8" s="280"/>
       <c r="H8" s="166"/>
       <c r="I8" s="166"/>
       <c r="J8" s="164"/>
@@ -6450,20 +6451,20 @@
       <c r="L8" s="169"/>
       <c r="M8" s="170"/>
       <c r="N8" s="163"/>
-      <c r="O8" s="143"/>
-      <c r="P8" s="143"/>
-      <c r="Q8" s="143"/>
-      <c r="R8" s="143"/>
-      <c r="S8" s="143"/>
-      <c r="T8" s="143"/>
+      <c r="O8" s="142"/>
+      <c r="P8" s="142"/>
+      <c r="Q8" s="142"/>
+      <c r="R8" s="142"/>
+      <c r="S8" s="142"/>
+      <c r="T8" s="142"/>
       <c r="U8" s="162"/>
       <c r="V8" s="180"/>
       <c r="W8" s="181"/>
       <c r="X8" s="181"/>
       <c r="Y8" s="181"/>
       <c r="Z8" s="181"/>
-      <c r="AA8" s="102"/>
-      <c r="AB8" s="103"/>
+      <c r="AA8" s="101"/>
+      <c r="AB8" s="102"/>
       <c r="AC8" s="171"/>
       <c r="AD8" s="48"/>
       <c r="AE8" s="48"/>
@@ -6471,9 +6472,9 @@
       <c r="AG8" s="48"/>
       <c r="AH8" s="75"/>
       <c r="AI8" s="194"/>
-      <c r="AJ8" s="89"/>
-      <c r="AK8" s="201"/>
-      <c r="AL8" s="89"/>
+      <c r="AJ8" s="86"/>
+      <c r="AK8" s="200"/>
+      <c r="AL8" s="86"/>
       <c r="AM8" s="48"/>
       <c r="AN8" s="48"/>
       <c r="AO8" s="48"/>
@@ -6484,48 +6485,48 @@
       <c r="AT8" s="48"/>
       <c r="AU8" s="48"/>
       <c r="AV8" s="48"/>
-      <c r="AW8" s="139"/>
-      <c r="AX8" s="140"/>
+      <c r="AW8" s="138"/>
+      <c r="AX8" s="139"/>
       <c r="AY8" s="39"/>
-      <c r="AZ8" s="219"/>
-      <c r="BA8" s="219"/>
-      <c r="BB8" s="219"/>
-      <c r="BC8" s="219"/>
-      <c r="BD8" s="219"/>
-      <c r="BE8" s="219"/>
-      <c r="BF8" s="220"/>
+      <c r="AZ8" s="242"/>
+      <c r="BA8" s="242"/>
+      <c r="BB8" s="242"/>
+      <c r="BC8" s="242"/>
+      <c r="BD8" s="242"/>
+      <c r="BE8" s="242"/>
+      <c r="BF8" s="243"/>
       <c r="BG8" s="40"/>
-      <c r="BH8" s="219"/>
-      <c r="BI8" s="219"/>
-      <c r="BJ8" s="219"/>
-      <c r="BK8" s="219"/>
-      <c r="BL8" s="219"/>
-      <c r="BM8" s="219"/>
-      <c r="BN8" s="220"/>
-      <c r="BO8" s="127"/>
-      <c r="BP8" s="128"/>
-      <c r="BQ8" s="128"/>
-      <c r="BR8" s="129"/>
+      <c r="BH8" s="242"/>
+      <c r="BI8" s="242"/>
+      <c r="BJ8" s="242"/>
+      <c r="BK8" s="242"/>
+      <c r="BL8" s="242"/>
+      <c r="BM8" s="242"/>
+      <c r="BN8" s="243"/>
+      <c r="BO8" s="126"/>
+      <c r="BP8" s="127"/>
+      <c r="BQ8" s="127"/>
+      <c r="BR8" s="128"/>
       <c r="BS8" s="69"/>
-      <c r="BT8" s="156"/>
+      <c r="BT8" s="147"/>
       <c r="BU8" s="47"/>
-      <c r="BV8" s="152"/>
-      <c r="BW8" s="153"/>
-      <c r="BX8" s="156"/>
+      <c r="BV8" s="155"/>
+      <c r="BW8" s="156"/>
+      <c r="BX8" s="147"/>
       <c r="BY8" s="47"/>
       <c r="BZ8" s="47"/>
-      <c r="CA8" s="91"/>
-      <c r="CB8" s="156"/>
+      <c r="CA8" s="88"/>
+      <c r="CB8" s="147"/>
       <c r="CC8" s="47"/>
       <c r="CD8" s="47"/>
       <c r="CE8" s="74"/>
-      <c r="CF8" s="198"/>
-      <c r="CG8" s="199"/>
+      <c r="CF8" s="197"/>
+      <c r="CG8" s="198"/>
       <c r="CH8" s="10"/>
     </row>
     <row r="9" spans="6:86" ht="15.75" customHeight="1">
-      <c r="F9" s="296"/>
-      <c r="G9" s="296"/>
+      <c r="F9" s="280"/>
+      <c r="G9" s="280"/>
       <c r="H9" s="166"/>
       <c r="I9" s="166"/>
       <c r="J9" s="49" t="s">
@@ -6533,15 +6534,15 @@
       </c>
       <c r="K9" s="50"/>
       <c r="L9" s="51"/>
-      <c r="M9" s="144" t="s">
+      <c r="M9" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="N9" s="145"/>
+      <c r="N9" s="144"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
       <c r="R9" s="14"/>
-      <c r="S9" s="89"/>
+      <c r="S9" s="86"/>
       <c r="T9" s="48"/>
       <c r="U9" s="48"/>
       <c r="V9" s="48"/>
@@ -6555,67 +6556,67 @@
       <c r="AD9" s="47"/>
       <c r="AE9" s="47"/>
       <c r="AF9" s="74"/>
-      <c r="AG9" s="211" t="s">
+      <c r="AG9" s="244" t="s">
         <v>4</v>
       </c>
-      <c r="AH9" s="212"/>
-      <c r="AI9" s="213"/>
-      <c r="AJ9" s="135" t="s">
+      <c r="AH9" s="245"/>
+      <c r="AI9" s="246"/>
+      <c r="AJ9" s="134" t="s">
         <v>24</v>
       </c>
-      <c r="AK9" s="136"/>
-      <c r="AL9" s="136"/>
-      <c r="AM9" s="136"/>
-      <c r="AN9" s="130"/>
-      <c r="AO9" s="130"/>
-      <c r="AP9" s="130"/>
-      <c r="AQ9" s="130"/>
-      <c r="AR9" s="130"/>
-      <c r="AS9" s="130"/>
-      <c r="AT9" s="130"/>
-      <c r="AU9" s="130"/>
-      <c r="AV9" s="130"/>
-      <c r="AW9" s="130"/>
-      <c r="AX9" s="130"/>
-      <c r="AY9" s="130"/>
-      <c r="AZ9" s="130"/>
-      <c r="BA9" s="130"/>
-      <c r="BB9" s="130"/>
-      <c r="BC9" s="130"/>
-      <c r="BD9" s="130"/>
-      <c r="BE9" s="130"/>
-      <c r="BF9" s="130"/>
-      <c r="BG9" s="130"/>
-      <c r="BH9" s="130"/>
-      <c r="BI9" s="130"/>
-      <c r="BJ9" s="130"/>
-      <c r="BK9" s="130"/>
-      <c r="BL9" s="130"/>
-      <c r="BM9" s="130"/>
-      <c r="BN9" s="130"/>
-      <c r="BO9" s="130"/>
-      <c r="BP9" s="130"/>
-      <c r="BQ9" s="130"/>
-      <c r="BR9" s="130"/>
-      <c r="BS9" s="130"/>
-      <c r="BT9" s="130"/>
-      <c r="BU9" s="130"/>
-      <c r="BV9" s="130"/>
-      <c r="BW9" s="130"/>
-      <c r="BX9" s="130"/>
-      <c r="BY9" s="130"/>
-      <c r="BZ9" s="130"/>
-      <c r="CA9" s="130"/>
-      <c r="CB9" s="130"/>
-      <c r="CC9" s="130"/>
-      <c r="CD9" s="130"/>
-      <c r="CE9" s="130"/>
-      <c r="CF9" s="130"/>
-      <c r="CG9" s="131"/>
+      <c r="AK9" s="135"/>
+      <c r="AL9" s="135"/>
+      <c r="AM9" s="135"/>
+      <c r="AN9" s="129"/>
+      <c r="AO9" s="129"/>
+      <c r="AP9" s="129"/>
+      <c r="AQ9" s="129"/>
+      <c r="AR9" s="129"/>
+      <c r="AS9" s="129"/>
+      <c r="AT9" s="129"/>
+      <c r="AU9" s="129"/>
+      <c r="AV9" s="129"/>
+      <c r="AW9" s="129"/>
+      <c r="AX9" s="129"/>
+      <c r="AY9" s="129"/>
+      <c r="AZ9" s="129"/>
+      <c r="BA9" s="129"/>
+      <c r="BB9" s="129"/>
+      <c r="BC9" s="129"/>
+      <c r="BD9" s="129"/>
+      <c r="BE9" s="129"/>
+      <c r="BF9" s="129"/>
+      <c r="BG9" s="129"/>
+      <c r="BH9" s="129"/>
+      <c r="BI9" s="129"/>
+      <c r="BJ9" s="129"/>
+      <c r="BK9" s="129"/>
+      <c r="BL9" s="129"/>
+      <c r="BM9" s="129"/>
+      <c r="BN9" s="129"/>
+      <c r="BO9" s="129"/>
+      <c r="BP9" s="129"/>
+      <c r="BQ9" s="129"/>
+      <c r="BR9" s="129"/>
+      <c r="BS9" s="129"/>
+      <c r="BT9" s="129"/>
+      <c r="BU9" s="129"/>
+      <c r="BV9" s="129"/>
+      <c r="BW9" s="129"/>
+      <c r="BX9" s="129"/>
+      <c r="BY9" s="129"/>
+      <c r="BZ9" s="129"/>
+      <c r="CA9" s="129"/>
+      <c r="CB9" s="129"/>
+      <c r="CC9" s="129"/>
+      <c r="CD9" s="129"/>
+      <c r="CE9" s="129"/>
+      <c r="CF9" s="129"/>
+      <c r="CG9" s="130"/>
     </row>
     <row r="10" spans="6:86" ht="15.75" customHeight="1">
-      <c r="F10" s="296"/>
-      <c r="G10" s="296"/>
+      <c r="F10" s="280"/>
+      <c r="G10" s="280"/>
       <c r="H10" s="166"/>
       <c r="I10" s="166"/>
       <c r="J10" s="52"/>
@@ -6629,7 +6630,7 @@
       <c r="P10" s="71"/>
       <c r="Q10" s="71"/>
       <c r="R10" s="71"/>
-      <c r="S10" s="89"/>
+      <c r="S10" s="86"/>
       <c r="T10" s="48"/>
       <c r="U10" s="48"/>
       <c r="V10" s="48"/>
@@ -6643,9 +6644,9 @@
       <c r="AD10" s="48"/>
       <c r="AE10" s="48"/>
       <c r="AF10" s="75"/>
-      <c r="AG10" s="211"/>
-      <c r="AH10" s="212"/>
-      <c r="AI10" s="213"/>
+      <c r="AG10" s="244"/>
+      <c r="AH10" s="245"/>
+      <c r="AI10" s="246"/>
       <c r="AJ10" s="58"/>
       <c r="AK10" s="59"/>
       <c r="AL10" s="59"/>
@@ -6698,8 +6699,8 @@
       <c r="CG10" s="60"/>
     </row>
     <row r="11" spans="6:86" ht="15.75" customHeight="1">
-      <c r="F11" s="296"/>
-      <c r="G11" s="296"/>
+      <c r="F11" s="280"/>
+      <c r="G11" s="280"/>
       <c r="H11" s="166"/>
       <c r="I11" s="166"/>
       <c r="J11" s="55"/>
@@ -6711,7 +6712,7 @@
       <c r="P11" s="73"/>
       <c r="Q11" s="73"/>
       <c r="R11" s="73"/>
-      <c r="S11" s="89"/>
+      <c r="S11" s="86"/>
       <c r="T11" s="48"/>
       <c r="U11" s="48"/>
       <c r="V11" s="48"/>
@@ -6725,9 +6726,9 @@
       <c r="AD11" s="48"/>
       <c r="AE11" s="48"/>
       <c r="AF11" s="75"/>
-      <c r="AG11" s="214"/>
-      <c r="AH11" s="215"/>
-      <c r="AI11" s="216"/>
+      <c r="AG11" s="247"/>
+      <c r="AH11" s="248"/>
+      <c r="AI11" s="249"/>
       <c r="AJ11" s="61"/>
       <c r="AK11" s="62"/>
       <c r="AL11" s="62"/>
@@ -6780,8 +6781,8 @@
       <c r="CG11" s="63"/>
     </row>
     <row r="12" spans="6:86" ht="15.75" customHeight="1">
-      <c r="F12" s="296"/>
-      <c r="G12" s="296"/>
+      <c r="F12" s="280"/>
+      <c r="G12" s="280"/>
       <c r="H12" s="166"/>
       <c r="I12" s="166"/>
       <c r="J12" s="41" t="s">
@@ -6789,16 +6790,16 @@
       </c>
       <c r="K12" s="42"/>
       <c r="L12" s="43"/>
-      <c r="M12" s="209" t="s">
+      <c r="M12" s="204" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="210"/>
-      <c r="O12" s="206" t="s">
+      <c r="N12" s="205"/>
+      <c r="O12" s="201" t="s">
         <v>6</v>
       </c>
-      <c r="P12" s="206"/>
-      <c r="Q12" s="206"/>
-      <c r="R12" s="207"/>
+      <c r="P12" s="201"/>
+      <c r="Q12" s="201"/>
+      <c r="R12" s="202"/>
       <c r="S12" s="64"/>
       <c r="T12" s="65"/>
       <c r="U12" s="65"/>
@@ -6868,8 +6869,8 @@
       <c r="CG12" s="66"/>
     </row>
     <row r="13" spans="6:86" ht="15.75" customHeight="1">
-      <c r="F13" s="296"/>
-      <c r="G13" s="296"/>
+      <c r="F13" s="280"/>
+      <c r="G13" s="280"/>
       <c r="H13" s="166"/>
       <c r="I13" s="166"/>
       <c r="J13" s="44"/>
@@ -6880,7 +6881,7 @@
       <c r="O13" s="73"/>
       <c r="P13" s="73"/>
       <c r="Q13" s="73"/>
-      <c r="R13" s="208"/>
+      <c r="R13" s="203"/>
       <c r="S13" s="61"/>
       <c r="T13" s="62"/>
       <c r="U13" s="62"/>
@@ -6950,79 +6951,79 @@
       <c r="CG13" s="63"/>
     </row>
     <row r="14" spans="6:86" ht="15.75" customHeight="1">
-      <c r="F14" s="296"/>
-      <c r="G14" s="296"/>
+      <c r="F14" s="280"/>
+      <c r="G14" s="280"/>
       <c r="H14" s="166"/>
       <c r="I14" s="166"/>
-      <c r="J14" s="87" t="s">
+      <c r="J14" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="87"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="87"/>
-      <c r="O14" s="88"/>
-      <c r="P14" s="92" t="s">
+      <c r="K14" s="84"/>
+      <c r="L14" s="84"/>
+      <c r="M14" s="84"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="85"/>
+      <c r="P14" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="Q14" s="93"/>
-      <c r="R14" s="93"/>
-      <c r="S14" s="94"/>
-      <c r="T14" s="155"/>
-      <c r="U14" s="154"/>
-      <c r="V14" s="95"/>
-      <c r="W14" s="96"/>
-      <c r="X14" s="96"/>
-      <c r="Y14" s="110"/>
-      <c r="Z14" s="95"/>
-      <c r="AA14" s="96"/>
-      <c r="AB14" s="96"/>
-      <c r="AC14" s="110"/>
-      <c r="AD14" s="154"/>
+      <c r="Q14" s="90"/>
+      <c r="R14" s="90"/>
+      <c r="S14" s="91"/>
+      <c r="T14" s="145"/>
+      <c r="U14" s="146"/>
+      <c r="V14" s="92"/>
+      <c r="W14" s="93"/>
+      <c r="X14" s="93"/>
+      <c r="Y14" s="109"/>
+      <c r="Z14" s="92"/>
+      <c r="AA14" s="93"/>
+      <c r="AB14" s="93"/>
+      <c r="AC14" s="109"/>
+      <c r="AD14" s="146"/>
       <c r="AE14" s="157"/>
-      <c r="AF14" s="117"/>
-      <c r="AG14" s="118"/>
-      <c r="AH14" s="119"/>
+      <c r="AF14" s="116"/>
+      <c r="AG14" s="117"/>
+      <c r="AH14" s="118"/>
       <c r="AI14" s="76" t="s">
         <v>13</v>
       </c>
       <c r="AJ14" s="77"/>
       <c r="AK14" s="77"/>
       <c r="AL14" s="77"/>
-      <c r="AM14" s="111" t="s">
+      <c r="AM14" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="AN14" s="112"/>
-      <c r="AO14" s="112"/>
-      <c r="AP14" s="112"/>
-      <c r="AQ14" s="112"/>
-      <c r="AR14" s="112"/>
-      <c r="AS14" s="112"/>
-      <c r="AT14" s="112"/>
-      <c r="AU14" s="112"/>
-      <c r="AV14" s="112"/>
-      <c r="AW14" s="112"/>
-      <c r="AX14" s="112"/>
-      <c r="AY14" s="112"/>
-      <c r="AZ14" s="112"/>
-      <c r="BA14" s="112"/>
-      <c r="BB14" s="112"/>
-      <c r="BC14" s="112"/>
-      <c r="BD14" s="112"/>
-      <c r="BE14" s="112"/>
-      <c r="BF14" s="112"/>
-      <c r="BG14" s="112"/>
-      <c r="BH14" s="112"/>
-      <c r="BI14" s="112"/>
-      <c r="BJ14" s="112"/>
-      <c r="BK14" s="112"/>
-      <c r="BL14" s="112"/>
-      <c r="BM14" s="112"/>
-      <c r="BN14" s="112"/>
-      <c r="BO14" s="112"/>
-      <c r="BP14" s="112"/>
-      <c r="BQ14" s="112"/>
-      <c r="BR14" s="113"/>
+      <c r="AN14" s="111"/>
+      <c r="AO14" s="111"/>
+      <c r="AP14" s="111"/>
+      <c r="AQ14" s="111"/>
+      <c r="AR14" s="111"/>
+      <c r="AS14" s="111"/>
+      <c r="AT14" s="111"/>
+      <c r="AU14" s="111"/>
+      <c r="AV14" s="111"/>
+      <c r="AW14" s="111"/>
+      <c r="AX14" s="111"/>
+      <c r="AY14" s="111"/>
+      <c r="AZ14" s="111"/>
+      <c r="BA14" s="111"/>
+      <c r="BB14" s="111"/>
+      <c r="BC14" s="111"/>
+      <c r="BD14" s="111"/>
+      <c r="BE14" s="111"/>
+      <c r="BF14" s="111"/>
+      <c r="BG14" s="111"/>
+      <c r="BH14" s="111"/>
+      <c r="BI14" s="111"/>
+      <c r="BJ14" s="111"/>
+      <c r="BK14" s="111"/>
+      <c r="BL14" s="111"/>
+      <c r="BM14" s="111"/>
+      <c r="BN14" s="111"/>
+      <c r="BO14" s="111"/>
+      <c r="BP14" s="111"/>
+      <c r="BQ14" s="111"/>
+      <c r="BR14" s="112"/>
       <c r="BS14" s="33"/>
       <c r="BT14" s="33"/>
       <c r="BU14" s="33"/>
@@ -7040,71 +7041,71 @@
       <c r="CG14" s="33"/>
     </row>
     <row r="15" spans="6:86" ht="15.75" customHeight="1">
-      <c r="F15" s="296"/>
-      <c r="G15" s="296"/>
+      <c r="F15" s="280"/>
+      <c r="G15" s="280"/>
       <c r="H15" s="166"/>
       <c r="I15" s="166"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
-      <c r="O15" s="88"/>
-      <c r="P15" s="92"/>
-      <c r="Q15" s="93"/>
-      <c r="R15" s="93"/>
-      <c r="S15" s="94"/>
-      <c r="T15" s="156"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="84"/>
+      <c r="M15" s="84"/>
+      <c r="N15" s="84"/>
+      <c r="O15" s="85"/>
+      <c r="P15" s="89"/>
+      <c r="Q15" s="90"/>
+      <c r="R15" s="90"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="147"/>
       <c r="U15" s="47"/>
-      <c r="V15" s="91"/>
-      <c r="W15" s="97"/>
-      <c r="X15" s="97"/>
+      <c r="V15" s="88"/>
+      <c r="W15" s="94"/>
+      <c r="X15" s="94"/>
       <c r="Y15" s="69"/>
-      <c r="Z15" s="91"/>
-      <c r="AA15" s="97"/>
-      <c r="AB15" s="97"/>
+      <c r="Z15" s="88"/>
+      <c r="AA15" s="94"/>
+      <c r="AB15" s="94"/>
       <c r="AC15" s="69"/>
       <c r="AD15" s="47"/>
       <c r="AE15" s="74"/>
-      <c r="AF15" s="120"/>
-      <c r="AG15" s="121"/>
-      <c r="AH15" s="122"/>
+      <c r="AF15" s="119"/>
+      <c r="AG15" s="120"/>
+      <c r="AH15" s="121"/>
       <c r="AI15" s="78"/>
       <c r="AJ15" s="79"/>
       <c r="AK15" s="79"/>
       <c r="AL15" s="79"/>
-      <c r="AM15" s="114"/>
-      <c r="AN15" s="115"/>
-      <c r="AO15" s="115"/>
-      <c r="AP15" s="115"/>
-      <c r="AQ15" s="115"/>
-      <c r="AR15" s="115"/>
-      <c r="AS15" s="115"/>
-      <c r="AT15" s="115"/>
-      <c r="AU15" s="115"/>
-      <c r="AV15" s="115"/>
-      <c r="AW15" s="115"/>
-      <c r="AX15" s="115"/>
-      <c r="AY15" s="115"/>
-      <c r="AZ15" s="115"/>
-      <c r="BA15" s="115"/>
-      <c r="BB15" s="115"/>
-      <c r="BC15" s="115"/>
-      <c r="BD15" s="115"/>
-      <c r="BE15" s="115"/>
-      <c r="BF15" s="115"/>
-      <c r="BG15" s="115"/>
-      <c r="BH15" s="115"/>
-      <c r="BI15" s="115"/>
-      <c r="BJ15" s="115"/>
-      <c r="BK15" s="115"/>
-      <c r="BL15" s="115"/>
-      <c r="BM15" s="115"/>
-      <c r="BN15" s="115"/>
-      <c r="BO15" s="115"/>
-      <c r="BP15" s="115"/>
-      <c r="BQ15" s="115"/>
-      <c r="BR15" s="116"/>
+      <c r="AM15" s="113"/>
+      <c r="AN15" s="114"/>
+      <c r="AO15" s="114"/>
+      <c r="AP15" s="114"/>
+      <c r="AQ15" s="114"/>
+      <c r="AR15" s="114"/>
+      <c r="AS15" s="114"/>
+      <c r="AT15" s="114"/>
+      <c r="AU15" s="114"/>
+      <c r="AV15" s="114"/>
+      <c r="AW15" s="114"/>
+      <c r="AX15" s="114"/>
+      <c r="AY15" s="114"/>
+      <c r="AZ15" s="114"/>
+      <c r="BA15" s="114"/>
+      <c r="BB15" s="114"/>
+      <c r="BC15" s="114"/>
+      <c r="BD15" s="114"/>
+      <c r="BE15" s="114"/>
+      <c r="BF15" s="114"/>
+      <c r="BG15" s="114"/>
+      <c r="BH15" s="114"/>
+      <c r="BI15" s="114"/>
+      <c r="BJ15" s="114"/>
+      <c r="BK15" s="114"/>
+      <c r="BL15" s="114"/>
+      <c r="BM15" s="114"/>
+      <c r="BN15" s="114"/>
+      <c r="BO15" s="114"/>
+      <c r="BP15" s="114"/>
+      <c r="BQ15" s="114"/>
+      <c r="BR15" s="115"/>
       <c r="BS15" s="5"/>
       <c r="BT15" s="9"/>
       <c r="BU15" s="9"/>
@@ -7123,8 +7124,8 @@
       <c r="CH15" s="2"/>
     </row>
     <row r="16" spans="6:86" ht="12.75" customHeight="1">
-      <c r="F16" s="296"/>
-      <c r="G16" s="296"/>
+      <c r="F16" s="280"/>
+      <c r="G16" s="280"/>
       <c r="H16" s="166"/>
       <c r="I16" s="166"/>
       <c r="J16" s="9"/>
@@ -7207,8 +7208,8 @@
       <c r="CG16" s="9"/>
     </row>
     <row r="17" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F17" s="296"/>
-      <c r="G17" s="296"/>
+      <c r="F17" s="280"/>
+      <c r="G17" s="280"/>
       <c r="H17" s="166"/>
       <c r="I17" s="166"/>
       <c r="K17" s="18" t="s">
@@ -7216,181 +7217,181 @@
       </c>
     </row>
     <row r="18" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F18" s="296"/>
-      <c r="G18" s="296"/>
+      <c r="F18" s="280"/>
+      <c r="G18" s="280"/>
       <c r="H18" s="166"/>
       <c r="I18" s="166"/>
       <c r="K18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AS18" s="134" t="s">
+      <c r="AS18" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="AT18" s="134"/>
-      <c r="AU18" s="134"/>
-      <c r="AV18" s="134"/>
-      <c r="AW18" s="134"/>
-      <c r="AX18" s="134"/>
-      <c r="AY18" s="134"/>
-      <c r="AZ18" s="134"/>
-      <c r="BA18" s="134"/>
-      <c r="BB18" s="134"/>
-      <c r="BC18" s="134"/>
-      <c r="BD18" s="134"/>
-      <c r="BE18" s="134"/>
-      <c r="BF18" s="134"/>
-      <c r="BG18" s="134"/>
-      <c r="BH18" s="134"/>
-      <c r="BI18" s="134"/>
-      <c r="BJ18" s="134"/>
-      <c r="BK18" s="134"/>
-      <c r="BL18" s="134"/>
-      <c r="BM18" s="134"/>
-      <c r="BN18" s="134"/>
-      <c r="BO18" s="134"/>
-      <c r="BP18" s="134"/>
-      <c r="BQ18" s="134"/>
-      <c r="BR18" s="134"/>
-      <c r="BS18" s="134"/>
-      <c r="BT18" s="134"/>
-      <c r="BU18" s="134"/>
-      <c r="BV18" s="134"/>
-      <c r="BW18" s="134"/>
-      <c r="BX18" s="134"/>
-      <c r="BY18" s="134"/>
-      <c r="BZ18" s="134"/>
-      <c r="CA18" s="134"/>
-      <c r="CB18" s="134"/>
+      <c r="AT18" s="133"/>
+      <c r="AU18" s="133"/>
+      <c r="AV18" s="133"/>
+      <c r="AW18" s="133"/>
+      <c r="AX18" s="133"/>
+      <c r="AY18" s="133"/>
+      <c r="AZ18" s="133"/>
+      <c r="BA18" s="133"/>
+      <c r="BB18" s="133"/>
+      <c r="BC18" s="133"/>
+      <c r="BD18" s="133"/>
+      <c r="BE18" s="133"/>
+      <c r="BF18" s="133"/>
+      <c r="BG18" s="133"/>
+      <c r="BH18" s="133"/>
+      <c r="BI18" s="133"/>
+      <c r="BJ18" s="133"/>
+      <c r="BK18" s="133"/>
+      <c r="BL18" s="133"/>
+      <c r="BM18" s="133"/>
+      <c r="BN18" s="133"/>
+      <c r="BO18" s="133"/>
+      <c r="BP18" s="133"/>
+      <c r="BQ18" s="133"/>
+      <c r="BR18" s="133"/>
+      <c r="BS18" s="133"/>
+      <c r="BT18" s="133"/>
+      <c r="BU18" s="133"/>
+      <c r="BV18" s="133"/>
+      <c r="BW18" s="133"/>
+      <c r="BX18" s="133"/>
+      <c r="BY18" s="133"/>
+      <c r="BZ18" s="133"/>
+      <c r="CA18" s="133"/>
+      <c r="CB18" s="133"/>
     </row>
     <row r="19" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F19" s="296"/>
-      <c r="G19" s="296"/>
+      <c r="F19" s="280"/>
+      <c r="G19" s="280"/>
       <c r="H19" s="166"/>
       <c r="I19" s="166"/>
-      <c r="J19" s="204" t="s">
+      <c r="J19" s="217" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="205"/>
-      <c r="L19" s="205"/>
-      <c r="M19" s="205"/>
-      <c r="N19" s="205"/>
-      <c r="O19" s="205"/>
-      <c r="P19" s="205"/>
-      <c r="Q19" s="205"/>
-      <c r="R19" s="205"/>
-      <c r="S19" s="205"/>
-      <c r="T19" s="205"/>
-      <c r="U19" s="205"/>
-      <c r="V19" s="205"/>
-      <c r="W19" s="205"/>
-      <c r="X19" s="205"/>
-      <c r="Y19" s="205"/>
-      <c r="Z19" s="205"/>
-      <c r="AA19" s="205"/>
-      <c r="AB19" s="205"/>
-      <c r="AC19" s="205"/>
-      <c r="AD19" s="205"/>
-      <c r="AE19" s="205"/>
-      <c r="AF19" s="205"/>
-      <c r="AG19" s="205"/>
-      <c r="AH19" s="205"/>
-      <c r="AI19" s="205"/>
-      <c r="AJ19" s="205"/>
-      <c r="AK19" s="205"/>
-      <c r="AL19" s="205"/>
-      <c r="AM19" s="205"/>
-      <c r="AN19" s="205"/>
-      <c r="AO19" s="205"/>
-      <c r="AS19" s="134"/>
-      <c r="AT19" s="134"/>
-      <c r="AU19" s="134"/>
-      <c r="AV19" s="134"/>
-      <c r="AW19" s="134"/>
-      <c r="AX19" s="134"/>
-      <c r="AY19" s="134"/>
-      <c r="AZ19" s="134"/>
-      <c r="BA19" s="134"/>
-      <c r="BB19" s="134"/>
-      <c r="BC19" s="134"/>
-      <c r="BD19" s="134"/>
-      <c r="BE19" s="134"/>
-      <c r="BF19" s="134"/>
-      <c r="BG19" s="134"/>
-      <c r="BH19" s="134"/>
-      <c r="BI19" s="134"/>
-      <c r="BJ19" s="134"/>
-      <c r="BK19" s="134"/>
-      <c r="BL19" s="134"/>
-      <c r="BM19" s="134"/>
-      <c r="BN19" s="134"/>
-      <c r="BO19" s="134"/>
-      <c r="BP19" s="134"/>
-      <c r="BQ19" s="134"/>
-      <c r="BR19" s="134"/>
-      <c r="BS19" s="134"/>
-      <c r="BT19" s="134"/>
-      <c r="BU19" s="134"/>
-      <c r="BV19" s="134"/>
-      <c r="BW19" s="134"/>
-      <c r="BX19" s="134"/>
-      <c r="BY19" s="134"/>
-      <c r="BZ19" s="134"/>
-      <c r="CA19" s="134"/>
-      <c r="CB19" s="134"/>
+      <c r="K19" s="218"/>
+      <c r="L19" s="218"/>
+      <c r="M19" s="218"/>
+      <c r="N19" s="218"/>
+      <c r="O19" s="218"/>
+      <c r="P19" s="218"/>
+      <c r="Q19" s="218"/>
+      <c r="R19" s="218"/>
+      <c r="S19" s="218"/>
+      <c r="T19" s="218"/>
+      <c r="U19" s="218"/>
+      <c r="V19" s="218"/>
+      <c r="W19" s="218"/>
+      <c r="X19" s="218"/>
+      <c r="Y19" s="218"/>
+      <c r="Z19" s="218"/>
+      <c r="AA19" s="218"/>
+      <c r="AB19" s="218"/>
+      <c r="AC19" s="218"/>
+      <c r="AD19" s="218"/>
+      <c r="AE19" s="218"/>
+      <c r="AF19" s="218"/>
+      <c r="AG19" s="218"/>
+      <c r="AH19" s="218"/>
+      <c r="AI19" s="218"/>
+      <c r="AJ19" s="218"/>
+      <c r="AK19" s="218"/>
+      <c r="AL19" s="218"/>
+      <c r="AM19" s="218"/>
+      <c r="AN19" s="218"/>
+      <c r="AO19" s="218"/>
+      <c r="AS19" s="133"/>
+      <c r="AT19" s="133"/>
+      <c r="AU19" s="133"/>
+      <c r="AV19" s="133"/>
+      <c r="AW19" s="133"/>
+      <c r="AX19" s="133"/>
+      <c r="AY19" s="133"/>
+      <c r="AZ19" s="133"/>
+      <c r="BA19" s="133"/>
+      <c r="BB19" s="133"/>
+      <c r="BC19" s="133"/>
+      <c r="BD19" s="133"/>
+      <c r="BE19" s="133"/>
+      <c r="BF19" s="133"/>
+      <c r="BG19" s="133"/>
+      <c r="BH19" s="133"/>
+      <c r="BI19" s="133"/>
+      <c r="BJ19" s="133"/>
+      <c r="BK19" s="133"/>
+      <c r="BL19" s="133"/>
+      <c r="BM19" s="133"/>
+      <c r="BN19" s="133"/>
+      <c r="BO19" s="133"/>
+      <c r="BP19" s="133"/>
+      <c r="BQ19" s="133"/>
+      <c r="BR19" s="133"/>
+      <c r="BS19" s="133"/>
+      <c r="BT19" s="133"/>
+      <c r="BU19" s="133"/>
+      <c r="BV19" s="133"/>
+      <c r="BW19" s="133"/>
+      <c r="BX19" s="133"/>
+      <c r="BY19" s="133"/>
+      <c r="BZ19" s="133"/>
+      <c r="CA19" s="133"/>
+      <c r="CB19" s="133"/>
     </row>
     <row r="20" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F20" s="296"/>
-      <c r="G20" s="296"/>
+      <c r="F20" s="280"/>
+      <c r="G20" s="280"/>
       <c r="H20" s="166"/>
       <c r="I20" s="166"/>
-      <c r="J20" s="104" t="s">
+      <c r="J20" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="K20" s="105"/>
-      <c r="L20" s="105"/>
-      <c r="M20" s="105"/>
-      <c r="N20" s="105"/>
-      <c r="O20" s="105"/>
-      <c r="P20" s="105"/>
-      <c r="Q20" s="105"/>
-      <c r="R20" s="105"/>
-      <c r="S20" s="105"/>
-      <c r="T20" s="105"/>
-      <c r="U20" s="105"/>
-      <c r="V20" s="105"/>
-      <c r="W20" s="105"/>
-      <c r="X20" s="105"/>
-      <c r="Y20" s="105"/>
-      <c r="Z20" s="105"/>
-      <c r="AA20" s="105"/>
-      <c r="AB20" s="105"/>
-      <c r="AC20" s="105"/>
-      <c r="AD20" s="105"/>
-      <c r="AE20" s="105"/>
-      <c r="AF20" s="105"/>
-      <c r="AG20" s="106"/>
-      <c r="AH20" s="104" t="s">
+      <c r="K20" s="104"/>
+      <c r="L20" s="104"/>
+      <c r="M20" s="104"/>
+      <c r="N20" s="104"/>
+      <c r="O20" s="104"/>
+      <c r="P20" s="104"/>
+      <c r="Q20" s="104"/>
+      <c r="R20" s="104"/>
+      <c r="S20" s="104"/>
+      <c r="T20" s="104"/>
+      <c r="U20" s="104"/>
+      <c r="V20" s="104"/>
+      <c r="W20" s="104"/>
+      <c r="X20" s="104"/>
+      <c r="Y20" s="104"/>
+      <c r="Z20" s="104"/>
+      <c r="AA20" s="104"/>
+      <c r="AB20" s="104"/>
+      <c r="AC20" s="104"/>
+      <c r="AD20" s="104"/>
+      <c r="AE20" s="104"/>
+      <c r="AF20" s="104"/>
+      <c r="AG20" s="105"/>
+      <c r="AH20" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="AI20" s="105"/>
-      <c r="AJ20" s="105"/>
-      <c r="AK20" s="105"/>
-      <c r="AL20" s="105"/>
-      <c r="AM20" s="105"/>
-      <c r="AN20" s="105"/>
-      <c r="AO20" s="105"/>
-      <c r="AP20" s="105"/>
-      <c r="AQ20" s="105"/>
-      <c r="AR20" s="105"/>
-      <c r="AS20" s="105"/>
-      <c r="AT20" s="105"/>
-      <c r="AU20" s="105"/>
-      <c r="AV20" s="105"/>
-      <c r="AW20" s="106"/>
-      <c r="AX20" s="217" t="s">
+      <c r="AI20" s="104"/>
+      <c r="AJ20" s="104"/>
+      <c r="AK20" s="104"/>
+      <c r="AL20" s="104"/>
+      <c r="AM20" s="104"/>
+      <c r="AN20" s="104"/>
+      <c r="AO20" s="104"/>
+      <c r="AP20" s="104"/>
+      <c r="AQ20" s="104"/>
+      <c r="AR20" s="104"/>
+      <c r="AS20" s="104"/>
+      <c r="AT20" s="104"/>
+      <c r="AU20" s="104"/>
+      <c r="AV20" s="104"/>
+      <c r="AW20" s="105"/>
+      <c r="AX20" s="240" t="s">
         <v>32</v>
       </c>
-      <c r="AY20" s="218"/>
+      <c r="AY20" s="241"/>
       <c r="AZ20" s="16"/>
       <c r="BA20" s="16"/>
       <c r="BB20" s="16"/>
@@ -7399,25 +7400,25 @@
       </c>
       <c r="BD20" s="19"/>
       <c r="BE20" s="19"/>
-      <c r="BF20" s="123"/>
-      <c r="BG20" s="123"/>
-      <c r="BH20" s="123"/>
-      <c r="BI20" s="123"/>
-      <c r="BJ20" s="123"/>
-      <c r="BK20" s="123"/>
-      <c r="BL20" s="107"/>
-      <c r="BM20" s="108"/>
-      <c r="BN20" s="108"/>
-      <c r="BO20" s="108"/>
-      <c r="BP20" s="108"/>
-      <c r="BQ20" s="108"/>
-      <c r="BR20" s="108"/>
-      <c r="BS20" s="108"/>
-      <c r="BT20" s="109"/>
+      <c r="BF20" s="122"/>
+      <c r="BG20" s="122"/>
+      <c r="BH20" s="122"/>
+      <c r="BI20" s="122"/>
+      <c r="BJ20" s="122"/>
+      <c r="BK20" s="122"/>
+      <c r="BL20" s="106"/>
+      <c r="BM20" s="107"/>
+      <c r="BN20" s="107"/>
+      <c r="BO20" s="107"/>
+      <c r="BP20" s="107"/>
+      <c r="BQ20" s="107"/>
+      <c r="BR20" s="107"/>
+      <c r="BS20" s="107"/>
+      <c r="BT20" s="108"/>
     </row>
     <row r="21" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F21" s="296"/>
-      <c r="G21" s="296"/>
+      <c r="F21" s="280"/>
+      <c r="G21" s="280"/>
       <c r="H21" s="166"/>
       <c r="I21" s="166"/>
       <c r="J21" s="167"/>
@@ -7426,10 +7427,10 @@
       <c r="M21" s="48"/>
       <c r="N21" s="48"/>
       <c r="O21" s="48"/>
-      <c r="P21" s="202"/>
-      <c r="Q21" s="203"/>
-      <c r="R21" s="203"/>
-      <c r="S21" s="89"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="96"/>
+      <c r="R21" s="96"/>
+      <c r="S21" s="86"/>
       <c r="T21" s="48"/>
       <c r="U21" s="48"/>
       <c r="V21" s="48"/>
@@ -7441,27 +7442,27 @@
       <c r="AB21" s="48"/>
       <c r="AC21" s="48"/>
       <c r="AD21" s="80"/>
-      <c r="AE21" s="155"/>
+      <c r="AE21" s="145"/>
       <c r="AF21" s="80"/>
       <c r="AG21" s="81"/>
-      <c r="AH21" s="124" t="s">
+      <c r="AH21" s="123" t="s">
         <v>44</v>
       </c>
-      <c r="AI21" s="125"/>
-      <c r="AJ21" s="125"/>
-      <c r="AK21" s="126"/>
+      <c r="AI21" s="124"/>
+      <c r="AJ21" s="124"/>
+      <c r="AK21" s="125"/>
       <c r="AL21" s="67"/>
       <c r="AM21" s="68"/>
       <c r="AN21" s="68"/>
-      <c r="AO21" s="90"/>
+      <c r="AO21" s="87"/>
       <c r="AP21" s="168"/>
-      <c r="AQ21" s="132"/>
+      <c r="AQ21" s="131"/>
       <c r="AR21" s="68"/>
-      <c r="AS21" s="90"/>
+      <c r="AS21" s="87"/>
       <c r="AT21" s="168"/>
-      <c r="AU21" s="132"/>
-      <c r="AV21" s="132"/>
-      <c r="AW21" s="133"/>
+      <c r="AU21" s="131"/>
+      <c r="AV21" s="131"/>
+      <c r="AW21" s="132"/>
       <c r="AX21" s="172" t="s">
         <v>37</v>
       </c>
@@ -7493,8 +7494,8 @@
       <c r="BT21" s="60"/>
     </row>
     <row r="22" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F22" s="296"/>
-      <c r="G22" s="296"/>
+      <c r="F22" s="280"/>
+      <c r="G22" s="280"/>
       <c r="H22" s="166"/>
       <c r="I22" s="166"/>
       <c r="J22" s="167"/>
@@ -7503,10 +7504,10 @@
       <c r="M22" s="48"/>
       <c r="N22" s="48"/>
       <c r="O22" s="48"/>
-      <c r="P22" s="202"/>
-      <c r="Q22" s="203"/>
-      <c r="R22" s="203"/>
-      <c r="S22" s="89"/>
+      <c r="P22" s="95"/>
+      <c r="Q22" s="96"/>
+      <c r="R22" s="96"/>
+      <c r="S22" s="86"/>
       <c r="T22" s="48"/>
       <c r="U22" s="48"/>
       <c r="V22" s="48"/>
@@ -7518,22 +7519,22 @@
       <c r="AB22" s="48"/>
       <c r="AC22" s="48"/>
       <c r="AD22" s="82"/>
-      <c r="AE22" s="156"/>
+      <c r="AE22" s="147"/>
       <c r="AF22" s="82"/>
       <c r="AG22" s="83"/>
-      <c r="AH22" s="127"/>
-      <c r="AI22" s="128"/>
-      <c r="AJ22" s="128"/>
-      <c r="AK22" s="129"/>
+      <c r="AH22" s="126"/>
+      <c r="AI22" s="127"/>
+      <c r="AJ22" s="127"/>
+      <c r="AK22" s="128"/>
       <c r="AL22" s="69"/>
       <c r="AM22" s="47"/>
       <c r="AN22" s="47"/>
-      <c r="AO22" s="91"/>
-      <c r="AP22" s="156"/>
+      <c r="AO22" s="88"/>
+      <c r="AP22" s="147"/>
       <c r="AQ22" s="47"/>
       <c r="AR22" s="47"/>
-      <c r="AS22" s="91"/>
-      <c r="AT22" s="156"/>
+      <c r="AS22" s="88"/>
+      <c r="AT22" s="147"/>
       <c r="AU22" s="47"/>
       <c r="AV22" s="47"/>
       <c r="AW22" s="74"/>
@@ -7562,216 +7563,216 @@
       <c r="BT22" s="63"/>
     </row>
     <row r="23" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F23" s="296"/>
-      <c r="G23" s="296"/>
+      <c r="F23" s="280"/>
+      <c r="G23" s="280"/>
       <c r="H23" s="166"/>
       <c r="I23" s="166"/>
-      <c r="J23" s="287" t="s">
+      <c r="J23" s="271" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="288"/>
-      <c r="L23" s="289"/>
-      <c r="M23" s="147" t="s">
+      <c r="K23" s="272"/>
+      <c r="L23" s="273"/>
+      <c r="M23" s="150" t="s">
         <v>27</v>
       </c>
-      <c r="N23" s="148"/>
-      <c r="O23" s="148"/>
-      <c r="P23" s="148"/>
-      <c r="Q23" s="148"/>
-      <c r="R23" s="148"/>
-      <c r="S23" s="148"/>
-      <c r="T23" s="148"/>
-      <c r="U23" s="148"/>
-      <c r="V23" s="148"/>
-      <c r="W23" s="148"/>
-      <c r="X23" s="148"/>
-      <c r="Y23" s="148"/>
-      <c r="Z23" s="149"/>
-      <c r="AA23" s="147" t="s">
+      <c r="N23" s="151"/>
+      <c r="O23" s="151"/>
+      <c r="P23" s="151"/>
+      <c r="Q23" s="151"/>
+      <c r="R23" s="151"/>
+      <c r="S23" s="151"/>
+      <c r="T23" s="151"/>
+      <c r="U23" s="151"/>
+      <c r="V23" s="151"/>
+      <c r="W23" s="151"/>
+      <c r="X23" s="151"/>
+      <c r="Y23" s="151"/>
+      <c r="Z23" s="152"/>
+      <c r="AA23" s="150" t="s">
         <v>54</v>
       </c>
-      <c r="AB23" s="148"/>
-      <c r="AC23" s="148"/>
-      <c r="AD23" s="148"/>
-      <c r="AE23" s="148"/>
-      <c r="AF23" s="148"/>
-      <c r="AG23" s="148"/>
-      <c r="AH23" s="148"/>
-      <c r="AI23" s="148"/>
-      <c r="AJ23" s="148"/>
-      <c r="AK23" s="148"/>
-      <c r="AL23" s="148"/>
-      <c r="AM23" s="148"/>
-      <c r="AN23" s="148"/>
-      <c r="AO23" s="148"/>
-      <c r="AP23" s="148"/>
-      <c r="AQ23" s="148"/>
-      <c r="AR23" s="148"/>
-      <c r="AS23" s="148"/>
-      <c r="AT23" s="148"/>
-      <c r="AU23" s="148"/>
-      <c r="AV23" s="148"/>
-      <c r="AW23" s="148"/>
-      <c r="AX23" s="148"/>
-      <c r="AY23" s="148"/>
-      <c r="AZ23" s="148"/>
-      <c r="BA23" s="148"/>
-      <c r="BB23" s="148"/>
-      <c r="BC23" s="148"/>
-      <c r="BD23" s="148"/>
-      <c r="BE23" s="148"/>
-      <c r="BF23" s="148"/>
-      <c r="BG23" s="148"/>
-      <c r="BH23" s="148"/>
-      <c r="BI23" s="148"/>
-      <c r="BJ23" s="148"/>
-      <c r="BK23" s="148"/>
-      <c r="BL23" s="148"/>
-      <c r="BM23" s="148"/>
-      <c r="BN23" s="148"/>
-      <c r="BO23" s="148"/>
-      <c r="BP23" s="148"/>
-      <c r="BQ23" s="148"/>
-      <c r="BR23" s="149"/>
-      <c r="BS23" s="104" t="s">
+      <c r="AB23" s="151"/>
+      <c r="AC23" s="151"/>
+      <c r="AD23" s="151"/>
+      <c r="AE23" s="151"/>
+      <c r="AF23" s="151"/>
+      <c r="AG23" s="151"/>
+      <c r="AH23" s="151"/>
+      <c r="AI23" s="151"/>
+      <c r="AJ23" s="151"/>
+      <c r="AK23" s="151"/>
+      <c r="AL23" s="151"/>
+      <c r="AM23" s="151"/>
+      <c r="AN23" s="151"/>
+      <c r="AO23" s="151"/>
+      <c r="AP23" s="151"/>
+      <c r="AQ23" s="151"/>
+      <c r="AR23" s="151"/>
+      <c r="AS23" s="151"/>
+      <c r="AT23" s="151"/>
+      <c r="AU23" s="151"/>
+      <c r="AV23" s="151"/>
+      <c r="AW23" s="151"/>
+      <c r="AX23" s="151"/>
+      <c r="AY23" s="151"/>
+      <c r="AZ23" s="151"/>
+      <c r="BA23" s="151"/>
+      <c r="BB23" s="151"/>
+      <c r="BC23" s="151"/>
+      <c r="BD23" s="151"/>
+      <c r="BE23" s="151"/>
+      <c r="BF23" s="151"/>
+      <c r="BG23" s="151"/>
+      <c r="BH23" s="151"/>
+      <c r="BI23" s="151"/>
+      <c r="BJ23" s="151"/>
+      <c r="BK23" s="151"/>
+      <c r="BL23" s="151"/>
+      <c r="BM23" s="151"/>
+      <c r="BN23" s="151"/>
+      <c r="BO23" s="151"/>
+      <c r="BP23" s="151"/>
+      <c r="BQ23" s="151"/>
+      <c r="BR23" s="152"/>
+      <c r="BS23" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="BT23" s="105"/>
-      <c r="BU23" s="105"/>
-      <c r="BV23" s="105"/>
-      <c r="BW23" s="105"/>
-      <c r="BX23" s="105"/>
-      <c r="BY23" s="105"/>
-      <c r="BZ23" s="105"/>
-      <c r="CA23" s="105"/>
-      <c r="CB23" s="105"/>
-      <c r="CC23" s="105"/>
-      <c r="CD23" s="105"/>
-      <c r="CE23" s="105"/>
-      <c r="CF23" s="105"/>
-      <c r="CG23" s="106"/>
+      <c r="BT23" s="104"/>
+      <c r="BU23" s="104"/>
+      <c r="BV23" s="104"/>
+      <c r="BW23" s="104"/>
+      <c r="BX23" s="104"/>
+      <c r="BY23" s="104"/>
+      <c r="BZ23" s="104"/>
+      <c r="CA23" s="104"/>
+      <c r="CB23" s="104"/>
+      <c r="CC23" s="104"/>
+      <c r="CD23" s="104"/>
+      <c r="CE23" s="104"/>
+      <c r="CF23" s="104"/>
+      <c r="CG23" s="105"/>
     </row>
     <row r="24" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F24" s="296"/>
-      <c r="G24" s="296"/>
+      <c r="F24" s="280"/>
+      <c r="G24" s="280"/>
       <c r="H24" s="166"/>
       <c r="I24" s="166"/>
-      <c r="J24" s="211"/>
-      <c r="K24" s="212"/>
-      <c r="L24" s="290"/>
-      <c r="M24" s="298"/>
-      <c r="N24" s="155"/>
-      <c r="O24" s="150"/>
-      <c r="P24" s="155"/>
-      <c r="Q24" s="150"/>
-      <c r="R24" s="155"/>
-      <c r="S24" s="150"/>
-      <c r="T24" s="155"/>
-      <c r="U24" s="150"/>
-      <c r="V24" s="155"/>
-      <c r="W24" s="150"/>
-      <c r="X24" s="155"/>
-      <c r="Y24" s="150"/>
+      <c r="J24" s="244"/>
+      <c r="K24" s="245"/>
+      <c r="L24" s="274"/>
+      <c r="M24" s="289"/>
+      <c r="N24" s="145"/>
+      <c r="O24" s="153"/>
+      <c r="P24" s="145"/>
+      <c r="Q24" s="153"/>
+      <c r="R24" s="145"/>
+      <c r="S24" s="153"/>
+      <c r="T24" s="145"/>
+      <c r="U24" s="153"/>
+      <c r="V24" s="145"/>
+      <c r="W24" s="153"/>
+      <c r="X24" s="145"/>
+      <c r="Y24" s="153"/>
       <c r="Z24" s="81"/>
-      <c r="AA24" s="236" t="s">
+      <c r="AA24" s="283" t="s">
         <v>17</v>
       </c>
-      <c r="AB24" s="229"/>
-      <c r="AC24" s="229"/>
-      <c r="AD24" s="229"/>
-      <c r="AE24" s="229"/>
-      <c r="AF24" s="229"/>
-      <c r="AG24" s="229"/>
-      <c r="AH24" s="229"/>
-      <c r="AI24" s="229"/>
-      <c r="AJ24" s="237"/>
-      <c r="AK24" s="280" t="s">
+      <c r="AB24" s="214"/>
+      <c r="AC24" s="214"/>
+      <c r="AD24" s="214"/>
+      <c r="AE24" s="214"/>
+      <c r="AF24" s="214"/>
+      <c r="AG24" s="214"/>
+      <c r="AH24" s="214"/>
+      <c r="AI24" s="214"/>
+      <c r="AJ24" s="284"/>
+      <c r="AK24" s="260" t="s">
         <v>14</v>
       </c>
-      <c r="AL24" s="281"/>
-      <c r="AM24" s="281"/>
-      <c r="AN24" s="281"/>
-      <c r="AO24" s="250"/>
-      <c r="AP24" s="250"/>
-      <c r="AQ24" s="250"/>
-      <c r="AR24" s="250"/>
-      <c r="AS24" s="250"/>
-      <c r="AT24" s="250"/>
-      <c r="AU24" s="250"/>
-      <c r="AV24" s="250"/>
-      <c r="AW24" s="250"/>
-      <c r="AX24" s="250"/>
-      <c r="AY24" s="250"/>
-      <c r="AZ24" s="250"/>
-      <c r="BA24" s="250"/>
-      <c r="BB24" s="250"/>
-      <c r="BC24" s="250"/>
-      <c r="BD24" s="250"/>
-      <c r="BE24" s="250"/>
-      <c r="BF24" s="250"/>
-      <c r="BG24" s="250"/>
-      <c r="BH24" s="250"/>
-      <c r="BI24" s="250"/>
-      <c r="BJ24" s="250"/>
-      <c r="BK24" s="250"/>
-      <c r="BL24" s="250"/>
-      <c r="BM24" s="250"/>
-      <c r="BN24" s="250"/>
-      <c r="BO24" s="250"/>
-      <c r="BP24" s="250"/>
-      <c r="BQ24" s="250"/>
-      <c r="BR24" s="251"/>
-      <c r="BS24" s="252" t="s">
+      <c r="AL24" s="261"/>
+      <c r="AM24" s="261"/>
+      <c r="AN24" s="261"/>
+      <c r="AO24" s="228"/>
+      <c r="AP24" s="228"/>
+      <c r="AQ24" s="228"/>
+      <c r="AR24" s="228"/>
+      <c r="AS24" s="228"/>
+      <c r="AT24" s="228"/>
+      <c r="AU24" s="228"/>
+      <c r="AV24" s="228"/>
+      <c r="AW24" s="228"/>
+      <c r="AX24" s="228"/>
+      <c r="AY24" s="228"/>
+      <c r="AZ24" s="228"/>
+      <c r="BA24" s="228"/>
+      <c r="BB24" s="228"/>
+      <c r="BC24" s="228"/>
+      <c r="BD24" s="228"/>
+      <c r="BE24" s="228"/>
+      <c r="BF24" s="228"/>
+      <c r="BG24" s="228"/>
+      <c r="BH24" s="228"/>
+      <c r="BI24" s="228"/>
+      <c r="BJ24" s="228"/>
+      <c r="BK24" s="228"/>
+      <c r="BL24" s="228"/>
+      <c r="BM24" s="228"/>
+      <c r="BN24" s="228"/>
+      <c r="BO24" s="228"/>
+      <c r="BP24" s="228"/>
+      <c r="BQ24" s="228"/>
+      <c r="BR24" s="229"/>
+      <c r="BS24" s="230" t="s">
         <v>53</v>
       </c>
-      <c r="BT24" s="253"/>
-      <c r="BU24" s="254"/>
-      <c r="BV24" s="227"/>
-      <c r="BW24" s="228"/>
-      <c r="BX24" s="224"/>
-      <c r="BY24" s="225"/>
-      <c r="BZ24" s="227"/>
-      <c r="CA24" s="228"/>
-      <c r="CB24" s="224"/>
-      <c r="CC24" s="225"/>
-      <c r="CD24" s="227"/>
-      <c r="CE24" s="228"/>
-      <c r="CF24" s="224"/>
-      <c r="CG24" s="225"/>
+      <c r="BT24" s="231"/>
+      <c r="BU24" s="232"/>
+      <c r="BV24" s="212"/>
+      <c r="BW24" s="213"/>
+      <c r="BX24" s="209"/>
+      <c r="BY24" s="210"/>
+      <c r="BZ24" s="212"/>
+      <c r="CA24" s="213"/>
+      <c r="CB24" s="209"/>
+      <c r="CC24" s="210"/>
+      <c r="CD24" s="212"/>
+      <c r="CE24" s="213"/>
+      <c r="CF24" s="209"/>
+      <c r="CG24" s="210"/>
     </row>
     <row r="25" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F25" s="296"/>
-      <c r="G25" s="296"/>
+      <c r="F25" s="280"/>
+      <c r="G25" s="280"/>
       <c r="H25" s="166"/>
       <c r="I25" s="166"/>
-      <c r="J25" s="211"/>
-      <c r="K25" s="212"/>
-      <c r="L25" s="290"/>
-      <c r="M25" s="227"/>
+      <c r="J25" s="244"/>
+      <c r="K25" s="245"/>
+      <c r="L25" s="274"/>
+      <c r="M25" s="212"/>
       <c r="N25" s="168"/>
-      <c r="O25" s="224"/>
+      <c r="O25" s="209"/>
       <c r="P25" s="168"/>
-      <c r="Q25" s="224"/>
+      <c r="Q25" s="209"/>
       <c r="R25" s="168"/>
-      <c r="S25" s="224"/>
+      <c r="S25" s="209"/>
       <c r="T25" s="168"/>
-      <c r="U25" s="224"/>
+      <c r="U25" s="209"/>
       <c r="V25" s="168"/>
-      <c r="W25" s="224"/>
+      <c r="W25" s="209"/>
       <c r="X25" s="168"/>
-      <c r="Y25" s="224"/>
-      <c r="Z25" s="225"/>
-      <c r="AA25" s="232"/>
-      <c r="AB25" s="233"/>
-      <c r="AC25" s="238"/>
-      <c r="AD25" s="233"/>
-      <c r="AE25" s="238"/>
-      <c r="AF25" s="233"/>
-      <c r="AG25" s="238"/>
-      <c r="AH25" s="233"/>
-      <c r="AI25" s="238"/>
-      <c r="AJ25" s="282"/>
-      <c r="AK25" s="240"/>
+      <c r="Y25" s="209"/>
+      <c r="Z25" s="210"/>
+      <c r="AA25" s="281"/>
+      <c r="AB25" s="266"/>
+      <c r="AC25" s="262"/>
+      <c r="AD25" s="266"/>
+      <c r="AE25" s="262"/>
+      <c r="AF25" s="266"/>
+      <c r="AG25" s="262"/>
+      <c r="AH25" s="266"/>
+      <c r="AI25" s="262"/>
+      <c r="AJ25" s="263"/>
+      <c r="AK25" s="285"/>
       <c r="AL25" s="59"/>
       <c r="AM25" s="59"/>
       <c r="AN25" s="59"/>
@@ -7805,107 +7806,107 @@
       <c r="BP25" s="59"/>
       <c r="BQ25" s="59"/>
       <c r="BR25" s="60"/>
-      <c r="BS25" s="252"/>
-      <c r="BT25" s="253"/>
-      <c r="BU25" s="254"/>
-      <c r="BV25" s="227"/>
-      <c r="BW25" s="228"/>
-      <c r="BX25" s="224"/>
-      <c r="BY25" s="225"/>
-      <c r="BZ25" s="227"/>
-      <c r="CA25" s="228"/>
-      <c r="CB25" s="224"/>
-      <c r="CC25" s="225"/>
-      <c r="CD25" s="227"/>
-      <c r="CE25" s="228"/>
-      <c r="CF25" s="224"/>
-      <c r="CG25" s="225"/>
+      <c r="BS25" s="230"/>
+      <c r="BT25" s="231"/>
+      <c r="BU25" s="232"/>
+      <c r="BV25" s="212"/>
+      <c r="BW25" s="213"/>
+      <c r="BX25" s="209"/>
+      <c r="BY25" s="210"/>
+      <c r="BZ25" s="212"/>
+      <c r="CA25" s="213"/>
+      <c r="CB25" s="209"/>
+      <c r="CC25" s="210"/>
+      <c r="CD25" s="212"/>
+      <c r="CE25" s="213"/>
+      <c r="CF25" s="209"/>
+      <c r="CG25" s="210"/>
     </row>
     <row r="26" spans="6:88" ht="15.75" customHeight="1">
-      <c r="F26" s="296"/>
-      <c r="G26" s="296"/>
+      <c r="F26" s="280"/>
+      <c r="G26" s="280"/>
       <c r="H26" s="166"/>
       <c r="I26" s="166"/>
-      <c r="J26" s="214"/>
-      <c r="K26" s="215"/>
-      <c r="L26" s="291"/>
-      <c r="M26" s="299"/>
-      <c r="N26" s="156"/>
-      <c r="O26" s="249"/>
-      <c r="P26" s="156"/>
-      <c r="Q26" s="249"/>
-      <c r="R26" s="156"/>
-      <c r="S26" s="249"/>
-      <c r="T26" s="156"/>
-      <c r="U26" s="249"/>
-      <c r="V26" s="156"/>
-      <c r="W26" s="249"/>
-      <c r="X26" s="156"/>
-      <c r="Y26" s="249"/>
+      <c r="J26" s="247"/>
+      <c r="K26" s="248"/>
+      <c r="L26" s="275"/>
+      <c r="M26" s="290"/>
+      <c r="N26" s="147"/>
+      <c r="O26" s="227"/>
+      <c r="P26" s="147"/>
+      <c r="Q26" s="227"/>
+      <c r="R26" s="147"/>
+      <c r="S26" s="227"/>
+      <c r="T26" s="147"/>
+      <c r="U26" s="227"/>
+      <c r="V26" s="147"/>
+      <c r="W26" s="227"/>
+      <c r="X26" s="147"/>
+      <c r="Y26" s="227"/>
       <c r="Z26" s="83"/>
-      <c r="AA26" s="234"/>
-      <c r="AB26" s="235"/>
-      <c r="AC26" s="239"/>
-      <c r="AD26" s="235"/>
-      <c r="AE26" s="239"/>
-      <c r="AF26" s="235"/>
-      <c r="AG26" s="239"/>
-      <c r="AH26" s="235"/>
-      <c r="AI26" s="239"/>
-      <c r="AJ26" s="283"/>
-      <c r="AK26" s="241"/>
-      <c r="AL26" s="242"/>
-      <c r="AM26" s="242"/>
-      <c r="AN26" s="242"/>
-      <c r="AO26" s="242"/>
-      <c r="AP26" s="242"/>
-      <c r="AQ26" s="242"/>
-      <c r="AR26" s="242"/>
-      <c r="AS26" s="242"/>
-      <c r="AT26" s="242"/>
-      <c r="AU26" s="242"/>
-      <c r="AV26" s="242"/>
-      <c r="AW26" s="242"/>
-      <c r="AX26" s="242"/>
-      <c r="AY26" s="242"/>
-      <c r="AZ26" s="242"/>
-      <c r="BA26" s="242"/>
-      <c r="BB26" s="242"/>
-      <c r="BC26" s="242"/>
-      <c r="BD26" s="242"/>
-      <c r="BE26" s="242"/>
-      <c r="BF26" s="242"/>
-      <c r="BG26" s="242"/>
-      <c r="BH26" s="242"/>
-      <c r="BI26" s="242"/>
-      <c r="BJ26" s="242"/>
-      <c r="BK26" s="242"/>
-      <c r="BL26" s="242"/>
-      <c r="BM26" s="242"/>
-      <c r="BN26" s="242"/>
-      <c r="BO26" s="242"/>
-      <c r="BP26" s="242"/>
-      <c r="BQ26" s="242"/>
-      <c r="BR26" s="243"/>
-      <c r="BS26" s="252"/>
-      <c r="BT26" s="253"/>
-      <c r="BU26" s="254"/>
-      <c r="BV26" s="227"/>
-      <c r="BW26" s="228"/>
-      <c r="BX26" s="224"/>
-      <c r="BY26" s="226"/>
-      <c r="BZ26" s="227"/>
-      <c r="CA26" s="228"/>
-      <c r="CB26" s="224"/>
-      <c r="CC26" s="226"/>
-      <c r="CD26" s="227"/>
-      <c r="CE26" s="228"/>
-      <c r="CF26" s="224"/>
-      <c r="CG26" s="226"/>
+      <c r="AA26" s="282"/>
+      <c r="AB26" s="267"/>
+      <c r="AC26" s="264"/>
+      <c r="AD26" s="267"/>
+      <c r="AE26" s="264"/>
+      <c r="AF26" s="267"/>
+      <c r="AG26" s="264"/>
+      <c r="AH26" s="267"/>
+      <c r="AI26" s="264"/>
+      <c r="AJ26" s="265"/>
+      <c r="AK26" s="286"/>
+      <c r="AL26" s="287"/>
+      <c r="AM26" s="287"/>
+      <c r="AN26" s="287"/>
+      <c r="AO26" s="287"/>
+      <c r="AP26" s="287"/>
+      <c r="AQ26" s="287"/>
+      <c r="AR26" s="287"/>
+      <c r="AS26" s="287"/>
+      <c r="AT26" s="287"/>
+      <c r="AU26" s="287"/>
+      <c r="AV26" s="287"/>
+      <c r="AW26" s="287"/>
+      <c r="AX26" s="287"/>
+      <c r="AY26" s="287"/>
+      <c r="AZ26" s="287"/>
+      <c r="BA26" s="287"/>
+      <c r="BB26" s="287"/>
+      <c r="BC26" s="287"/>
+      <c r="BD26" s="287"/>
+      <c r="BE26" s="287"/>
+      <c r="BF26" s="287"/>
+      <c r="BG26" s="287"/>
+      <c r="BH26" s="287"/>
+      <c r="BI26" s="287"/>
+      <c r="BJ26" s="287"/>
+      <c r="BK26" s="287"/>
+      <c r="BL26" s="287"/>
+      <c r="BM26" s="287"/>
+      <c r="BN26" s="287"/>
+      <c r="BO26" s="287"/>
+      <c r="BP26" s="287"/>
+      <c r="BQ26" s="287"/>
+      <c r="BR26" s="288"/>
+      <c r="BS26" s="230"/>
+      <c r="BT26" s="231"/>
+      <c r="BU26" s="232"/>
+      <c r="BV26" s="212"/>
+      <c r="BW26" s="213"/>
+      <c r="BX26" s="209"/>
+      <c r="BY26" s="211"/>
+      <c r="BZ26" s="212"/>
+      <c r="CA26" s="213"/>
+      <c r="CB26" s="209"/>
+      <c r="CC26" s="211"/>
+      <c r="CD26" s="212"/>
+      <c r="CE26" s="213"/>
+      <c r="CF26" s="209"/>
+      <c r="CG26" s="211"/>
     </row>
     <row r="27" spans="6:88" ht="18" customHeight="1">
-      <c r="F27" s="296"/>
-      <c r="G27" s="296"/>
+      <c r="F27" s="280"/>
+      <c r="G27" s="280"/>
       <c r="H27" s="166"/>
       <c r="I27" s="166"/>
       <c r="J27" s="41" t="s">
@@ -7913,15 +7914,15 @@
       </c>
       <c r="K27" s="42"/>
       <c r="L27" s="43"/>
-      <c r="M27" s="261" t="s">
+      <c r="M27" s="291" t="s">
         <v>28</v>
       </c>
-      <c r="N27" s="262"/>
-      <c r="O27" s="262"/>
-      <c r="P27" s="262"/>
-      <c r="Q27" s="262"/>
-      <c r="R27" s="263"/>
-      <c r="S27" s="292"/>
+      <c r="N27" s="292"/>
+      <c r="O27" s="292"/>
+      <c r="P27" s="292"/>
+      <c r="Q27" s="292"/>
+      <c r="R27" s="293"/>
+      <c r="S27" s="276"/>
       <c r="T27" s="65"/>
       <c r="U27" s="65"/>
       <c r="V27" s="65"/>
@@ -7966,55 +7967,55 @@
       <c r="BI27" s="65"/>
       <c r="BJ27" s="65"/>
       <c r="BK27" s="65"/>
-      <c r="BL27" s="293"/>
-      <c r="BM27" s="255" t="s">
+      <c r="BL27" s="277"/>
+      <c r="BM27" s="233" t="s">
         <v>33</v>
       </c>
-      <c r="BN27" s="256"/>
-      <c r="BO27" s="257"/>
-      <c r="BP27" s="264" t="s">
+      <c r="BN27" s="234"/>
+      <c r="BO27" s="235"/>
+      <c r="BP27" s="294" t="s">
         <v>56</v>
       </c>
-      <c r="BQ27" s="265"/>
-      <c r="BR27" s="265"/>
-      <c r="BS27" s="265"/>
-      <c r="BT27" s="265"/>
-      <c r="BU27" s="265"/>
-      <c r="BV27" s="265"/>
-      <c r="BW27" s="265"/>
-      <c r="BX27" s="265"/>
-      <c r="BY27" s="265"/>
-      <c r="BZ27" s="265"/>
-      <c r="CA27" s="265"/>
-      <c r="CB27" s="265"/>
-      <c r="CC27" s="265"/>
-      <c r="CD27" s="265"/>
-      <c r="CE27" s="265"/>
-      <c r="CF27" s="265"/>
-      <c r="CG27" s="265"/>
-      <c r="CH27" s="265"/>
-      <c r="CI27" s="266"/>
+      <c r="BQ27" s="295"/>
+      <c r="BR27" s="295"/>
+      <c r="BS27" s="295"/>
+      <c r="BT27" s="295"/>
+      <c r="BU27" s="295"/>
+      <c r="BV27" s="295"/>
+      <c r="BW27" s="295"/>
+      <c r="BX27" s="295"/>
+      <c r="BY27" s="295"/>
+      <c r="BZ27" s="295"/>
+      <c r="CA27" s="295"/>
+      <c r="CB27" s="295"/>
+      <c r="CC27" s="295"/>
+      <c r="CD27" s="295"/>
+      <c r="CE27" s="295"/>
+      <c r="CF27" s="295"/>
+      <c r="CG27" s="295"/>
+      <c r="CH27" s="295"/>
+      <c r="CI27" s="296"/>
       <c r="CJ27" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="6:88" ht="18" customHeight="1">
-      <c r="F28" s="296"/>
-      <c r="G28" s="296"/>
+      <c r="F28" s="280"/>
+      <c r="G28" s="280"/>
       <c r="H28" s="166"/>
       <c r="I28" s="166"/>
       <c r="J28" s="44"/>
       <c r="K28" s="45"/>
       <c r="L28" s="46"/>
-      <c r="M28" s="84" t="s">
+      <c r="M28" s="219" t="s">
         <v>29</v>
       </c>
-      <c r="N28" s="85"/>
-      <c r="O28" s="85"/>
-      <c r="P28" s="85"/>
-      <c r="Q28" s="85"/>
-      <c r="R28" s="86"/>
-      <c r="S28" s="294"/>
+      <c r="N28" s="220"/>
+      <c r="O28" s="220"/>
+      <c r="P28" s="220"/>
+      <c r="Q28" s="220"/>
+      <c r="R28" s="221"/>
+      <c r="S28" s="278"/>
       <c r="T28" s="62"/>
       <c r="U28" s="62"/>
       <c r="V28" s="62"/>
@@ -8059,32 +8060,32 @@
       <c r="BI28" s="62"/>
       <c r="BJ28" s="62"/>
       <c r="BK28" s="62"/>
-      <c r="BL28" s="295"/>
-      <c r="BM28" s="258"/>
-      <c r="BN28" s="259"/>
-      <c r="BO28" s="260"/>
-      <c r="BP28" s="267" t="s">
+      <c r="BL28" s="279"/>
+      <c r="BM28" s="236"/>
+      <c r="BN28" s="237"/>
+      <c r="BO28" s="238"/>
+      <c r="BP28" s="297" t="s">
         <v>57</v>
       </c>
-      <c r="BQ28" s="268"/>
-      <c r="BR28" s="268"/>
-      <c r="BS28" s="268"/>
-      <c r="BT28" s="268"/>
-      <c r="BU28" s="268"/>
-      <c r="BV28" s="268"/>
-      <c r="BW28" s="268"/>
-      <c r="BX28" s="268"/>
-      <c r="BY28" s="268"/>
-      <c r="BZ28" s="268"/>
-      <c r="CA28" s="268"/>
-      <c r="CB28" s="268"/>
-      <c r="CC28" s="268"/>
-      <c r="CD28" s="268"/>
-      <c r="CE28" s="268"/>
-      <c r="CF28" s="268"/>
-      <c r="CG28" s="268"/>
-      <c r="CH28" s="268"/>
-      <c r="CI28" s="269"/>
+      <c r="BQ28" s="298"/>
+      <c r="BR28" s="298"/>
+      <c r="BS28" s="298"/>
+      <c r="BT28" s="298"/>
+      <c r="BU28" s="298"/>
+      <c r="BV28" s="298"/>
+      <c r="BW28" s="298"/>
+      <c r="BX28" s="298"/>
+      <c r="BY28" s="298"/>
+      <c r="BZ28" s="298"/>
+      <c r="CA28" s="298"/>
+      <c r="CB28" s="298"/>
+      <c r="CC28" s="298"/>
+      <c r="CD28" s="298"/>
+      <c r="CE28" s="298"/>
+      <c r="CF28" s="298"/>
+      <c r="CG28" s="298"/>
+      <c r="CH28" s="298"/>
+      <c r="CI28" s="299"/>
     </row>
     <row r="29" spans="6:88" ht="10.5" customHeight="1">
       <c r="F29" s="20"/>
@@ -8194,86 +8195,86 @@
       <c r="AE30"/>
       <c r="AF30"/>
       <c r="AG30"/>
-      <c r="BV30" s="236" t="s">
+      <c r="BV30" s="283" t="s">
         <v>41</v>
       </c>
-      <c r="BW30" s="229"/>
-      <c r="BX30" s="229"/>
-      <c r="BY30" s="229"/>
-      <c r="BZ30" s="229"/>
-      <c r="CA30" s="229"/>
-      <c r="CB30" s="229"/>
-      <c r="CC30" s="229"/>
-      <c r="CD30" s="229"/>
-      <c r="CE30" s="229"/>
-      <c r="CF30" s="229"/>
-      <c r="CG30" s="237"/>
+      <c r="BW30" s="214"/>
+      <c r="BX30" s="214"/>
+      <c r="BY30" s="214"/>
+      <c r="BZ30" s="214"/>
+      <c r="CA30" s="214"/>
+      <c r="CB30" s="214"/>
+      <c r="CC30" s="214"/>
+      <c r="CD30" s="214"/>
+      <c r="CE30" s="214"/>
+      <c r="CF30" s="214"/>
+      <c r="CG30" s="284"/>
     </row>
     <row r="31" spans="6:88" ht="15.75" customHeight="1">
       <c r="F31" s="20"/>
-      <c r="G31" s="284" t="s">
+      <c r="G31" s="268" t="s">
         <v>49</v>
       </c>
-      <c r="H31" s="285"/>
-      <c r="I31" s="285"/>
-      <c r="J31" s="285"/>
-      <c r="K31" s="285"/>
-      <c r="L31" s="285"/>
-      <c r="M31" s="285"/>
-      <c r="N31" s="285"/>
-      <c r="O31" s="285"/>
-      <c r="P31" s="285"/>
-      <c r="Q31" s="285"/>
-      <c r="R31" s="285"/>
-      <c r="S31" s="285"/>
-      <c r="T31" s="285"/>
-      <c r="U31" s="285"/>
-      <c r="V31" s="285"/>
-      <c r="W31" s="285"/>
-      <c r="X31" s="285"/>
-      <c r="Y31" s="285"/>
-      <c r="Z31" s="285"/>
-      <c r="AA31" s="285"/>
-      <c r="AB31" s="285"/>
-      <c r="AC31" s="285"/>
-      <c r="AD31" s="285"/>
-      <c r="AE31" s="285"/>
-      <c r="AF31" s="285"/>
-      <c r="AG31" s="286"/>
-      <c r="AZ31" s="297" t="s">
+      <c r="H31" s="269"/>
+      <c r="I31" s="269"/>
+      <c r="J31" s="269"/>
+      <c r="K31" s="269"/>
+      <c r="L31" s="269"/>
+      <c r="M31" s="269"/>
+      <c r="N31" s="269"/>
+      <c r="O31" s="269"/>
+      <c r="P31" s="269"/>
+      <c r="Q31" s="269"/>
+      <c r="R31" s="269"/>
+      <c r="S31" s="269"/>
+      <c r="T31" s="269"/>
+      <c r="U31" s="269"/>
+      <c r="V31" s="269"/>
+      <c r="W31" s="269"/>
+      <c r="X31" s="269"/>
+      <c r="Y31" s="269"/>
+      <c r="Z31" s="269"/>
+      <c r="AA31" s="269"/>
+      <c r="AB31" s="269"/>
+      <c r="AC31" s="269"/>
+      <c r="AD31" s="269"/>
+      <c r="AE31" s="269"/>
+      <c r="AF31" s="269"/>
+      <c r="AG31" s="270"/>
+      <c r="AZ31" s="239" t="s">
         <v>46</v>
       </c>
-      <c r="BA31" s="297"/>
-      <c r="BB31" s="297"/>
-      <c r="BC31" s="297"/>
-      <c r="BD31" s="297"/>
-      <c r="BE31" s="297"/>
-      <c r="BF31" s="297"/>
-      <c r="BG31" s="297"/>
-      <c r="BH31" s="297"/>
-      <c r="BI31" s="297"/>
-      <c r="BJ31" s="297"/>
-      <c r="BK31" s="297"/>
-      <c r="BL31" s="297"/>
-      <c r="BM31" s="297"/>
-      <c r="BN31" s="297"/>
-      <c r="BO31" s="297"/>
-      <c r="BP31" s="297"/>
-      <c r="BQ31" s="297"/>
-      <c r="BR31" s="297"/>
-      <c r="BS31" s="297"/>
-      <c r="BV31" s="147"/>
-      <c r="BW31" s="148"/>
-      <c r="BX31" s="148"/>
-      <c r="BY31" s="148"/>
-      <c r="BZ31" s="148"/>
-      <c r="CA31" s="148"/>
-      <c r="CB31" s="148"/>
-      <c r="CC31" s="148"/>
-      <c r="CD31" s="148"/>
-      <c r="CE31" s="148"/>
-      <c r="CF31" s="148"/>
-      <c r="CG31" s="149"/>
+      <c r="BA31" s="239"/>
+      <c r="BB31" s="239"/>
+      <c r="BC31" s="239"/>
+      <c r="BD31" s="239"/>
+      <c r="BE31" s="239"/>
+      <c r="BF31" s="239"/>
+      <c r="BG31" s="239"/>
+      <c r="BH31" s="239"/>
+      <c r="BI31" s="239"/>
+      <c r="BJ31" s="239"/>
+      <c r="BK31" s="239"/>
+      <c r="BL31" s="239"/>
+      <c r="BM31" s="239"/>
+      <c r="BN31" s="239"/>
+      <c r="BO31" s="239"/>
+      <c r="BP31" s="239"/>
+      <c r="BQ31" s="239"/>
+      <c r="BR31" s="239"/>
+      <c r="BS31" s="239"/>
+      <c r="BV31" s="150"/>
+      <c r="BW31" s="151"/>
+      <c r="BX31" s="151"/>
+      <c r="BY31" s="151"/>
+      <c r="BZ31" s="151"/>
+      <c r="CA31" s="151"/>
+      <c r="CB31" s="151"/>
+      <c r="CC31" s="151"/>
+      <c r="CD31" s="151"/>
+      <c r="CE31" s="151"/>
+      <c r="CF31" s="151"/>
+      <c r="CG31" s="152"/>
     </row>
     <row r="32" spans="6:88" ht="21" customHeight="1">
       <c r="F32" s="25"/>
@@ -8310,23 +8311,23 @@
       <c r="BK32" s="24"/>
       <c r="BN32" s="24"/>
       <c r="BO32" s="24"/>
-      <c r="BV32" s="221"/>
-      <c r="BW32" s="222"/>
-      <c r="BX32" s="222"/>
-      <c r="BY32" s="222"/>
-      <c r="BZ32" s="222"/>
-      <c r="CA32" s="222"/>
-      <c r="CB32" s="222"/>
-      <c r="CC32" s="222"/>
-      <c r="CD32" s="222"/>
-      <c r="CE32" s="222"/>
-      <c r="CF32" s="222"/>
-      <c r="CG32" s="223"/>
+      <c r="BV32" s="206"/>
+      <c r="BW32" s="207"/>
+      <c r="BX32" s="207"/>
+      <c r="BY32" s="207"/>
+      <c r="BZ32" s="207"/>
+      <c r="CA32" s="207"/>
+      <c r="CB32" s="207"/>
+      <c r="CC32" s="207"/>
+      <c r="CD32" s="207"/>
+      <c r="CE32" s="207"/>
+      <c r="CF32" s="207"/>
+      <c r="CG32" s="208"/>
     </row>
     <row r="33" spans="6:86" ht="21" customHeight="1">
       <c r="F33" s="20"/>
-      <c r="G33" s="270"/>
-      <c r="H33" s="271"/>
+      <c r="G33" s="250"/>
+      <c r="H33" s="251"/>
       <c r="I33" s="29" t="s">
         <v>9</v>
       </c>
@@ -8336,26 +8337,26 @@
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
-      <c r="P33" s="277"/>
-      <c r="Q33" s="277"/>
-      <c r="R33" s="277"/>
-      <c r="S33" s="277"/>
-      <c r="T33" s="277"/>
-      <c r="U33" s="277"/>
-      <c r="V33" s="277"/>
-      <c r="W33" s="277"/>
-      <c r="X33" s="277"/>
-      <c r="Y33" s="277"/>
-      <c r="Z33" s="277"/>
-      <c r="AA33" s="277"/>
-      <c r="AB33" s="277"/>
-      <c r="AC33" s="277"/>
-      <c r="AD33" s="277"/>
-      <c r="AE33" s="277"/>
-      <c r="AF33" s="277"/>
-      <c r="AG33" s="278"/>
-      <c r="AL33" s="244"/>
-      <c r="AM33" s="244"/>
+      <c r="P33" s="257"/>
+      <c r="Q33" s="257"/>
+      <c r="R33" s="257"/>
+      <c r="S33" s="257"/>
+      <c r="T33" s="257"/>
+      <c r="U33" s="257"/>
+      <c r="V33" s="257"/>
+      <c r="W33" s="257"/>
+      <c r="X33" s="257"/>
+      <c r="Y33" s="257"/>
+      <c r="Z33" s="257"/>
+      <c r="AA33" s="257"/>
+      <c r="AB33" s="257"/>
+      <c r="AC33" s="257"/>
+      <c r="AD33" s="257"/>
+      <c r="AE33" s="257"/>
+      <c r="AF33" s="257"/>
+      <c r="AG33" s="258"/>
+      <c r="AL33" s="222"/>
+      <c r="AM33" s="222"/>
       <c r="AN33" s="9"/>
       <c r="AO33" s="9"/>
       <c r="AP33" s="9"/>
@@ -8384,23 +8385,23 @@
       <c r="BM33" s="2"/>
       <c r="BN33" s="2"/>
       <c r="BO33" s="2"/>
-      <c r="BV33" s="221"/>
-      <c r="BW33" s="222"/>
-      <c r="BX33" s="222"/>
-      <c r="BY33" s="222"/>
-      <c r="BZ33" s="222"/>
-      <c r="CA33" s="222"/>
-      <c r="CB33" s="222"/>
-      <c r="CC33" s="222"/>
-      <c r="CD33" s="222"/>
-      <c r="CE33" s="222"/>
-      <c r="CF33" s="222"/>
-      <c r="CG33" s="223"/>
+      <c r="BV33" s="206"/>
+      <c r="BW33" s="207"/>
+      <c r="BX33" s="207"/>
+      <c r="BY33" s="207"/>
+      <c r="BZ33" s="207"/>
+      <c r="CA33" s="207"/>
+      <c r="CB33" s="207"/>
+      <c r="CC33" s="207"/>
+      <c r="CD33" s="207"/>
+      <c r="CE33" s="207"/>
+      <c r="CF33" s="207"/>
+      <c r="CG33" s="208"/>
     </row>
     <row r="34" spans="6:86" ht="21" customHeight="1">
       <c r="F34" s="20"/>
-      <c r="G34" s="272"/>
-      <c r="H34" s="271"/>
+      <c r="G34" s="252"/>
+      <c r="H34" s="251"/>
       <c r="I34" s="29" t="s">
         <v>8</v>
       </c>
@@ -8410,38 +8411,38 @@
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
       <c r="O34" s="9"/>
-      <c r="P34" s="277"/>
-      <c r="Q34" s="277"/>
-      <c r="R34" s="277"/>
-      <c r="S34" s="277"/>
-      <c r="T34" s="277"/>
-      <c r="U34" s="277"/>
-      <c r="V34" s="277"/>
-      <c r="W34" s="277"/>
-      <c r="X34" s="277"/>
-      <c r="Y34" s="277"/>
-      <c r="Z34" s="277"/>
-      <c r="AA34" s="277"/>
-      <c r="AB34" s="277"/>
-      <c r="AC34" s="277"/>
-      <c r="AD34" s="277"/>
-      <c r="AE34" s="277"/>
-      <c r="AF34" s="277"/>
-      <c r="AG34" s="278"/>
-      <c r="AL34" s="244"/>
-      <c r="AM34" s="244"/>
-      <c r="AN34" s="147"/>
-      <c r="AO34" s="148"/>
-      <c r="AP34" s="148"/>
-      <c r="AQ34" s="148"/>
-      <c r="AR34" s="148"/>
-      <c r="AS34" s="148"/>
-      <c r="AT34" s="148"/>
-      <c r="AU34" s="148"/>
-      <c r="AV34" s="148"/>
-      <c r="AW34" s="148"/>
-      <c r="AX34" s="148"/>
-      <c r="AY34" s="149"/>
+      <c r="P34" s="257"/>
+      <c r="Q34" s="257"/>
+      <c r="R34" s="257"/>
+      <c r="S34" s="257"/>
+      <c r="T34" s="257"/>
+      <c r="U34" s="257"/>
+      <c r="V34" s="257"/>
+      <c r="W34" s="257"/>
+      <c r="X34" s="257"/>
+      <c r="Y34" s="257"/>
+      <c r="Z34" s="257"/>
+      <c r="AA34" s="257"/>
+      <c r="AB34" s="257"/>
+      <c r="AC34" s="257"/>
+      <c r="AD34" s="257"/>
+      <c r="AE34" s="257"/>
+      <c r="AF34" s="257"/>
+      <c r="AG34" s="258"/>
+      <c r="AL34" s="222"/>
+      <c r="AM34" s="222"/>
+      <c r="AN34" s="150"/>
+      <c r="AO34" s="151"/>
+      <c r="AP34" s="151"/>
+      <c r="AQ34" s="151"/>
+      <c r="AR34" s="151"/>
+      <c r="AS34" s="151"/>
+      <c r="AT34" s="151"/>
+      <c r="AU34" s="151"/>
+      <c r="AV34" s="151"/>
+      <c r="AW34" s="151"/>
+      <c r="AX34" s="151"/>
+      <c r="AY34" s="152"/>
       <c r="AZ34" s="9"/>
       <c r="BA34" s="9"/>
       <c r="BB34" s="9"/>
@@ -8458,23 +8459,23 @@
       <c r="BM34" s="9"/>
       <c r="BN34" s="9"/>
       <c r="BO34" s="9"/>
-      <c r="BV34" s="221"/>
-      <c r="BW34" s="222"/>
-      <c r="BX34" s="222"/>
-      <c r="BY34" s="222"/>
-      <c r="BZ34" s="222"/>
-      <c r="CA34" s="222"/>
-      <c r="CB34" s="222"/>
-      <c r="CC34" s="222"/>
-      <c r="CD34" s="222"/>
-      <c r="CE34" s="222"/>
-      <c r="CF34" s="222"/>
-      <c r="CG34" s="223"/>
+      <c r="BV34" s="206"/>
+      <c r="BW34" s="207"/>
+      <c r="BX34" s="207"/>
+      <c r="BY34" s="207"/>
+      <c r="BZ34" s="207"/>
+      <c r="CA34" s="207"/>
+      <c r="CB34" s="207"/>
+      <c r="CC34" s="207"/>
+      <c r="CD34" s="207"/>
+      <c r="CE34" s="207"/>
+      <c r="CF34" s="207"/>
+      <c r="CG34" s="208"/>
     </row>
     <row r="35" spans="6:86" ht="21" customHeight="1">
       <c r="F35" s="20"/>
-      <c r="G35" s="272"/>
-      <c r="H35" s="271"/>
+      <c r="G35" s="252"/>
+      <c r="H35" s="251"/>
       <c r="I35" s="29" t="s">
         <v>10</v>
       </c>
@@ -8484,52 +8485,52 @@
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
       <c r="O35" s="9"/>
-      <c r="P35" s="277"/>
-      <c r="Q35" s="277"/>
-      <c r="R35" s="277"/>
-      <c r="S35" s="277"/>
-      <c r="T35" s="277"/>
-      <c r="U35" s="277"/>
-      <c r="V35" s="277"/>
-      <c r="W35" s="277"/>
-      <c r="X35" s="277"/>
-      <c r="Y35" s="277"/>
-      <c r="Z35" s="277"/>
-      <c r="AA35" s="277"/>
-      <c r="AB35" s="277"/>
-      <c r="AC35" s="277"/>
-      <c r="AD35" s="277"/>
-      <c r="AE35" s="277"/>
+      <c r="P35" s="257"/>
+      <c r="Q35" s="257"/>
+      <c r="R35" s="257"/>
+      <c r="S35" s="257"/>
+      <c r="T35" s="257"/>
+      <c r="U35" s="257"/>
+      <c r="V35" s="257"/>
+      <c r="W35" s="257"/>
+      <c r="X35" s="257"/>
+      <c r="Y35" s="257"/>
+      <c r="Z35" s="257"/>
+      <c r="AA35" s="257"/>
+      <c r="AB35" s="257"/>
+      <c r="AC35" s="257"/>
+      <c r="AD35" s="257"/>
+      <c r="AE35" s="257"/>
       <c r="AF35" s="35" t="s">
         <v>7</v>
       </c>
       <c r="AG35" s="3"/>
-      <c r="AL35" s="244"/>
-      <c r="AM35" s="244"/>
-      <c r="AN35" s="245"/>
-      <c r="AO35" s="246"/>
-      <c r="AP35" s="246"/>
-      <c r="AQ35" s="246"/>
-      <c r="AR35" s="246"/>
-      <c r="AS35" s="246"/>
-      <c r="AT35" s="246"/>
-      <c r="AU35" s="246"/>
-      <c r="AV35" s="246"/>
-      <c r="AW35" s="246"/>
-      <c r="AX35" s="246"/>
-      <c r="AY35" s="246"/>
-      <c r="AZ35" s="246"/>
-      <c r="BA35" s="246"/>
-      <c r="BB35" s="246"/>
-      <c r="BC35" s="246"/>
-      <c r="BD35" s="246"/>
-      <c r="BE35" s="246"/>
-      <c r="BF35" s="246"/>
-      <c r="BG35" s="246"/>
-      <c r="BH35" s="246"/>
-      <c r="BI35" s="246"/>
-      <c r="BJ35" s="246"/>
-      <c r="BK35" s="229" t="s">
+      <c r="AL35" s="222"/>
+      <c r="AM35" s="222"/>
+      <c r="AN35" s="223"/>
+      <c r="AO35" s="224"/>
+      <c r="AP35" s="224"/>
+      <c r="AQ35" s="224"/>
+      <c r="AR35" s="224"/>
+      <c r="AS35" s="224"/>
+      <c r="AT35" s="224"/>
+      <c r="AU35" s="224"/>
+      <c r="AV35" s="224"/>
+      <c r="AW35" s="224"/>
+      <c r="AX35" s="224"/>
+      <c r="AY35" s="224"/>
+      <c r="AZ35" s="224"/>
+      <c r="BA35" s="224"/>
+      <c r="BB35" s="224"/>
+      <c r="BC35" s="224"/>
+      <c r="BD35" s="224"/>
+      <c r="BE35" s="224"/>
+      <c r="BF35" s="224"/>
+      <c r="BG35" s="224"/>
+      <c r="BH35" s="224"/>
+      <c r="BI35" s="224"/>
+      <c r="BJ35" s="224"/>
+      <c r="BK35" s="214" t="s">
         <v>7</v>
       </c>
       <c r="BL35" s="36"/>
@@ -8540,76 +8541,76 @@
       <c r="BS35"/>
       <c r="BT35"/>
       <c r="BU35"/>
-      <c r="BV35" s="221"/>
-      <c r="BW35" s="222"/>
-      <c r="BX35" s="222"/>
-      <c r="BY35" s="222"/>
-      <c r="BZ35" s="222"/>
-      <c r="CA35" s="222"/>
-      <c r="CB35" s="222"/>
-      <c r="CC35" s="222"/>
-      <c r="CD35" s="222"/>
-      <c r="CE35" s="222"/>
-      <c r="CF35" s="222"/>
-      <c r="CG35" s="223"/>
+      <c r="BV35" s="206"/>
+      <c r="BW35" s="207"/>
+      <c r="BX35" s="207"/>
+      <c r="BY35" s="207"/>
+      <c r="BZ35" s="207"/>
+      <c r="CA35" s="207"/>
+      <c r="CB35" s="207"/>
+      <c r="CC35" s="207"/>
+      <c r="CD35" s="207"/>
+      <c r="CE35" s="207"/>
+      <c r="CF35" s="207"/>
+      <c r="CG35" s="208"/>
     </row>
     <row r="36" spans="6:86" ht="12.75" customHeight="1">
       <c r="F36" s="20"/>
-      <c r="G36" s="272"/>
-      <c r="H36" s="271"/>
-      <c r="I36" s="275" t="s">
+      <c r="G36" s="252"/>
+      <c r="H36" s="251"/>
+      <c r="I36" s="255" t="s">
         <v>52</v>
       </c>
-      <c r="J36" s="275"/>
-      <c r="K36" s="275"/>
-      <c r="L36" s="275"/>
-      <c r="M36" s="275"/>
-      <c r="N36" s="275"/>
-      <c r="O36" s="275"/>
-      <c r="P36" s="277"/>
-      <c r="Q36" s="277"/>
-      <c r="R36" s="277"/>
-      <c r="S36" s="277"/>
-      <c r="T36" s="277"/>
-      <c r="U36" s="277"/>
-      <c r="V36" s="277"/>
-      <c r="W36" s="277"/>
-      <c r="X36" s="277"/>
-      <c r="Y36" s="277"/>
-      <c r="Z36" s="277"/>
-      <c r="AA36" s="277"/>
-      <c r="AB36" s="277"/>
-      <c r="AC36" s="277"/>
-      <c r="AD36" s="277"/>
-      <c r="AE36" s="277"/>
-      <c r="AF36" s="277"/>
-      <c r="AG36" s="278"/>
-      <c r="AL36" s="244"/>
-      <c r="AM36" s="244"/>
-      <c r="AN36" s="100"/>
-      <c r="AO36" s="247"/>
-      <c r="AP36" s="247"/>
-      <c r="AQ36" s="247"/>
-      <c r="AR36" s="247"/>
-      <c r="AS36" s="247"/>
-      <c r="AT36" s="247"/>
-      <c r="AU36" s="247"/>
-      <c r="AV36" s="247"/>
-      <c r="AW36" s="247"/>
-      <c r="AX36" s="247"/>
-      <c r="AY36" s="247"/>
-      <c r="AZ36" s="247"/>
-      <c r="BA36" s="247"/>
-      <c r="BB36" s="247"/>
-      <c r="BC36" s="247"/>
-      <c r="BD36" s="247"/>
-      <c r="BE36" s="247"/>
-      <c r="BF36" s="247"/>
-      <c r="BG36" s="247"/>
-      <c r="BH36" s="247"/>
-      <c r="BI36" s="247"/>
-      <c r="BJ36" s="247"/>
-      <c r="BK36" s="230"/>
+      <c r="J36" s="255"/>
+      <c r="K36" s="255"/>
+      <c r="L36" s="255"/>
+      <c r="M36" s="255"/>
+      <c r="N36" s="255"/>
+      <c r="O36" s="255"/>
+      <c r="P36" s="257"/>
+      <c r="Q36" s="257"/>
+      <c r="R36" s="257"/>
+      <c r="S36" s="257"/>
+      <c r="T36" s="257"/>
+      <c r="U36" s="257"/>
+      <c r="V36" s="257"/>
+      <c r="W36" s="257"/>
+      <c r="X36" s="257"/>
+      <c r="Y36" s="257"/>
+      <c r="Z36" s="257"/>
+      <c r="AA36" s="257"/>
+      <c r="AB36" s="257"/>
+      <c r="AC36" s="257"/>
+      <c r="AD36" s="257"/>
+      <c r="AE36" s="257"/>
+      <c r="AF36" s="257"/>
+      <c r="AG36" s="258"/>
+      <c r="AL36" s="222"/>
+      <c r="AM36" s="222"/>
+      <c r="AN36" s="99"/>
+      <c r="AO36" s="225"/>
+      <c r="AP36" s="225"/>
+      <c r="AQ36" s="225"/>
+      <c r="AR36" s="225"/>
+      <c r="AS36" s="225"/>
+      <c r="AT36" s="225"/>
+      <c r="AU36" s="225"/>
+      <c r="AV36" s="225"/>
+      <c r="AW36" s="225"/>
+      <c r="AX36" s="225"/>
+      <c r="AY36" s="225"/>
+      <c r="AZ36" s="225"/>
+      <c r="BA36" s="225"/>
+      <c r="BB36" s="225"/>
+      <c r="BC36" s="225"/>
+      <c r="BD36" s="225"/>
+      <c r="BE36" s="225"/>
+      <c r="BF36" s="225"/>
+      <c r="BG36" s="225"/>
+      <c r="BH36" s="225"/>
+      <c r="BI36" s="225"/>
+      <c r="BJ36" s="225"/>
+      <c r="BK36" s="215"/>
       <c r="BL36" s="9"/>
       <c r="BM36" s="9"/>
       <c r="BN36" s="38"/>
@@ -8617,30 +8618,30 @@
       <c r="BS36"/>
       <c r="BT36"/>
       <c r="BU36"/>
-      <c r="BV36" s="221"/>
-      <c r="BW36" s="222"/>
-      <c r="BX36" s="222"/>
-      <c r="BY36" s="222"/>
-      <c r="BZ36" s="222"/>
-      <c r="CA36" s="222"/>
-      <c r="CB36" s="222"/>
-      <c r="CC36" s="222"/>
-      <c r="CD36" s="222"/>
-      <c r="CE36" s="222"/>
-      <c r="CF36" s="222"/>
-      <c r="CG36" s="223"/>
+      <c r="BV36" s="206"/>
+      <c r="BW36" s="207"/>
+      <c r="BX36" s="207"/>
+      <c r="BY36" s="207"/>
+      <c r="BZ36" s="207"/>
+      <c r="CA36" s="207"/>
+      <c r="CB36" s="207"/>
+      <c r="CC36" s="207"/>
+      <c r="CD36" s="207"/>
+      <c r="CE36" s="207"/>
+      <c r="CF36" s="207"/>
+      <c r="CG36" s="208"/>
     </row>
     <row r="37" spans="6:86" ht="12.75" customHeight="1">
       <c r="F37"/>
-      <c r="G37" s="273"/>
-      <c r="H37" s="274"/>
-      <c r="I37" s="276"/>
-      <c r="J37" s="276"/>
-      <c r="K37" s="276"/>
-      <c r="L37" s="276"/>
-      <c r="M37" s="276"/>
-      <c r="N37" s="276"/>
-      <c r="O37" s="276"/>
+      <c r="G37" s="253"/>
+      <c r="H37" s="254"/>
+      <c r="I37" s="256"/>
+      <c r="J37" s="256"/>
+      <c r="K37" s="256"/>
+      <c r="L37" s="256"/>
+      <c r="M37" s="256"/>
+      <c r="N37" s="256"/>
+      <c r="O37" s="256"/>
       <c r="P37" s="79"/>
       <c r="Q37" s="79"/>
       <c r="R37" s="79"/>
@@ -8658,37 +8659,37 @@
       <c r="AD37" s="79"/>
       <c r="AE37" s="79"/>
       <c r="AF37" s="79"/>
-      <c r="AG37" s="279"/>
+      <c r="AG37" s="259"/>
       <c r="AH37"/>
       <c r="AI37"/>
       <c r="AJ37"/>
       <c r="AK37"/>
-      <c r="AL37" s="244"/>
-      <c r="AM37" s="244"/>
-      <c r="AN37" s="102"/>
-      <c r="AO37" s="248"/>
-      <c r="AP37" s="248"/>
-      <c r="AQ37" s="248"/>
-      <c r="AR37" s="248"/>
-      <c r="AS37" s="248"/>
-      <c r="AT37" s="248"/>
-      <c r="AU37" s="248"/>
-      <c r="AV37" s="248"/>
-      <c r="AW37" s="248"/>
-      <c r="AX37" s="248"/>
-      <c r="AY37" s="248"/>
-      <c r="AZ37" s="248"/>
-      <c r="BA37" s="248"/>
-      <c r="BB37" s="248"/>
-      <c r="BC37" s="248"/>
-      <c r="BD37" s="248"/>
-      <c r="BE37" s="248"/>
-      <c r="BF37" s="248"/>
-      <c r="BG37" s="248"/>
-      <c r="BH37" s="248"/>
-      <c r="BI37" s="248"/>
-      <c r="BJ37" s="248"/>
-      <c r="BK37" s="231"/>
+      <c r="AL37" s="222"/>
+      <c r="AM37" s="222"/>
+      <c r="AN37" s="101"/>
+      <c r="AO37" s="226"/>
+      <c r="AP37" s="226"/>
+      <c r="AQ37" s="226"/>
+      <c r="AR37" s="226"/>
+      <c r="AS37" s="226"/>
+      <c r="AT37" s="226"/>
+      <c r="AU37" s="226"/>
+      <c r="AV37" s="226"/>
+      <c r="AW37" s="226"/>
+      <c r="AX37" s="226"/>
+      <c r="AY37" s="226"/>
+      <c r="AZ37" s="226"/>
+      <c r="BA37" s="226"/>
+      <c r="BB37" s="226"/>
+      <c r="BC37" s="226"/>
+      <c r="BD37" s="226"/>
+      <c r="BE37" s="226"/>
+      <c r="BF37" s="226"/>
+      <c r="BG37" s="226"/>
+      <c r="BH37" s="226"/>
+      <c r="BI37" s="226"/>
+      <c r="BJ37" s="226"/>
+      <c r="BK37" s="216"/>
       <c r="BL37" s="26"/>
       <c r="BM37" s="26"/>
       <c r="BN37" s="27"/>
@@ -11552,7 +11553,6 @@
     </row>
   </sheetData>
   <mergeCells count="162">
-    <mergeCell ref="M24:N26"/>
     <mergeCell ref="Q24:R26"/>
     <mergeCell ref="O24:P26"/>
     <mergeCell ref="Y24:Z26"/>
@@ -11561,6 +11561,10 @@
     <mergeCell ref="BP28:CI28"/>
     <mergeCell ref="BV30:CG30"/>
     <mergeCell ref="AA23:BR23"/>
+    <mergeCell ref="BV24:BW26"/>
+    <mergeCell ref="AZ8:BF8"/>
+    <mergeCell ref="BH8:BN8"/>
+    <mergeCell ref="AG9:AI11"/>
     <mergeCell ref="G33:H37"/>
     <mergeCell ref="I36:O37"/>
     <mergeCell ref="P36:AG37"/>
@@ -11582,20 +11586,6 @@
     <mergeCell ref="AD21:AE22"/>
     <mergeCell ref="AA25:AB26"/>
     <mergeCell ref="AA24:AJ24"/>
-    <mergeCell ref="AC25:AD26"/>
-    <mergeCell ref="AK25:BR26"/>
-    <mergeCell ref="BV24:BW26"/>
-    <mergeCell ref="AE25:AF26"/>
-    <mergeCell ref="AL33:AM37"/>
-    <mergeCell ref="AN35:BJ37"/>
-    <mergeCell ref="W24:X26"/>
-    <mergeCell ref="AO24:BR24"/>
-    <mergeCell ref="BS24:BU26"/>
-    <mergeCell ref="BM27:BO28"/>
-    <mergeCell ref="AZ31:BS31"/>
-    <mergeCell ref="AX20:AY20"/>
-    <mergeCell ref="AZ8:BF8"/>
-    <mergeCell ref="BH8:BN8"/>
     <mergeCell ref="BV31:CG37"/>
     <mergeCell ref="CB24:CC26"/>
     <mergeCell ref="BZ24:CA26"/>
@@ -11606,8 +11596,20 @@
     <mergeCell ref="BS23:CG23"/>
     <mergeCell ref="J19:AO19"/>
     <mergeCell ref="AH20:AW20"/>
-    <mergeCell ref="O12:R13"/>
-    <mergeCell ref="U9:V11"/>
+    <mergeCell ref="J27:L28"/>
+    <mergeCell ref="M28:R28"/>
+    <mergeCell ref="AL33:AM37"/>
+    <mergeCell ref="AN35:BJ37"/>
+    <mergeCell ref="W24:X26"/>
+    <mergeCell ref="AO24:BR24"/>
+    <mergeCell ref="BS24:BU26"/>
+    <mergeCell ref="BM27:BO28"/>
+    <mergeCell ref="AZ31:BS31"/>
+    <mergeCell ref="AX20:AY20"/>
+    <mergeCell ref="AC25:AD26"/>
+    <mergeCell ref="AK25:BR26"/>
+    <mergeCell ref="AE25:AF26"/>
+    <mergeCell ref="M24:N26"/>
     <mergeCell ref="R7:S8"/>
     <mergeCell ref="AB14:AC15"/>
     <mergeCell ref="AD14:AE15"/>
@@ -11616,7 +11618,6 @@
     <mergeCell ref="Z21:AA22"/>
     <mergeCell ref="X21:Y22"/>
     <mergeCell ref="M12:N12"/>
-    <mergeCell ref="AG9:AI11"/>
     <mergeCell ref="R21:S22"/>
     <mergeCell ref="CD2:CH2"/>
     <mergeCell ref="BY2:CC2"/>
@@ -11690,7 +11691,6 @@
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="T14:U15"/>
     <mergeCell ref="BA7:BF7"/>
-    <mergeCell ref="J27:L28"/>
     <mergeCell ref="J12:L13"/>
     <mergeCell ref="AC9:AD11"/>
     <mergeCell ref="J9:L11"/>
@@ -11702,7 +11702,6 @@
     <mergeCell ref="AB21:AC22"/>
     <mergeCell ref="AI14:AL15"/>
     <mergeCell ref="AF21:AG22"/>
-    <mergeCell ref="M28:R28"/>
     <mergeCell ref="L21:M22"/>
     <mergeCell ref="AA9:AB11"/>
     <mergeCell ref="J14:O15"/>
@@ -11714,6 +11713,8 @@
     <mergeCell ref="P14:S15"/>
     <mergeCell ref="V14:W15"/>
     <mergeCell ref="P21:Q22"/>
+    <mergeCell ref="O12:R13"/>
+    <mergeCell ref="U9:V11"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.39370078740157483" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.51181102362204722"/>

</xml_diff>